<commit_message>
Added 'row' and 'column' labels to the BUMPS_DOWN tab of the FADER2_bumps excel workbook.
</commit_message>
<xml_diff>
--- a/Files_for_TestPlan_TestReports/FADER2_bumps.xlsx
+++ b/Files_for_TestPlan_TestReports/FADER2_bumps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Fader25_board\fader25_pcb\Files_for_TestPlan_TestReports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caolen\Nokia\Fader2.5\fader25_pcb\Files_for_TestPlan_TestReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA119675-4BE2-4499-839A-96F24177562E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1326A3-9C62-430F-B85D-E5321EDB525D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="17715" windowHeight="9870" tabRatio="240" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32205" yWindow="1320" windowWidth="21420" windowHeight="13425" tabRatio="240" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="126">
   <si>
     <t>name</t>
   </si>
@@ -333,13 +331,91 @@
   </si>
   <si>
     <t>This sheet shows the bumps as they lay on PCB in flip-chip assembly. Layout is mirrored relative to Y axis (i.e. flipped left to right)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>AF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -376,6 +452,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Comic Sans MS"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Comic Sans MS"/>
+      <family val="4"/>
     </font>
   </fonts>
   <fills count="18">
@@ -720,7 +808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1010,6 +1098,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6517,10 +6611,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F1D2C4-C567-4531-BCF2-31E88F3EC739}">
-  <dimension ref="B2:AL34"/>
+  <dimension ref="A2:AL34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6528,12 +6622,91 @@
     <col min="1" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="2:38" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="98"/>
+      <c r="B8" s="99" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="99" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="99" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="99" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="99" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="99" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="99" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" s="99" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="99" t="s">
+        <v>117</v>
+      </c>
+      <c r="K8" s="99" t="s">
+        <v>116</v>
+      </c>
+      <c r="L8" s="99" t="s">
+        <v>115</v>
+      </c>
+      <c r="M8" s="99" t="s">
+        <v>114</v>
+      </c>
+      <c r="N8" s="99" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="99" t="s">
+        <v>112</v>
+      </c>
+      <c r="P8" s="99" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q8" s="99" t="s">
+        <v>110</v>
+      </c>
+      <c r="R8" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="S8" s="99" t="s">
+        <v>108</v>
+      </c>
+      <c r="T8" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="U8" s="99" t="s">
+        <v>106</v>
+      </c>
+      <c r="V8" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="W8" s="99" t="s">
+        <v>104</v>
+      </c>
+      <c r="X8" s="99" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y8" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z8" s="99" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA8" s="99" t="s">
+        <v>100</v>
+      </c>
       <c r="AK8" s="22" t="s">
         <v>15</v>
       </c>
@@ -6541,7 +6714,10 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="9" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="99">
+        <v>1</v>
+      </c>
       <c r="B9" s="43" t="str">
         <f>LEFT(Full!AA11,(FIND(";",Full!AA11,1)-1))</f>
         <v>NC</v>
@@ -6653,7 +6829,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="99">
+        <v>2</v>
+      </c>
       <c r="B10" s="44" t="str">
         <f>LEFT(Full!AA12,(FIND(";",Full!AA12,1)-1))</f>
         <v>VSS</v>
@@ -6765,7 +6944,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="99">
+        <v>3</v>
+      </c>
       <c r="B11" s="44" t="str">
         <f>LEFT(Full!AA13,(FIND(";",Full!AA13,1)-1))</f>
         <v>VSS</v>
@@ -6871,7 +7053,10 @@
         <v>SCAN_IN</v>
       </c>
     </row>
-    <row r="12" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="99">
+        <v>4</v>
+      </c>
       <c r="B12" s="58" t="str">
         <f>LEFT(Full!AA14,(FIND(";",Full!AA14,1)-1))</f>
         <v>VSS</v>
@@ -6984,7 +7169,10 @@
         <v>4.59</v>
       </c>
     </row>
-    <row r="13" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="99">
+        <v>5</v>
+      </c>
       <c r="B13" s="44" t="str">
         <f>LEFT(Full!AA15,(FIND(";",Full!AA15,1)-1))</f>
         <v>VSS</v>
@@ -7097,7 +7285,10 @@
         <v>4.59</v>
       </c>
     </row>
-    <row r="14" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="99">
+        <v>6</v>
+      </c>
       <c r="B14" s="58" t="str">
         <f>LEFT(Full!AA16,(FIND(";",Full!AA16,1)-1))</f>
         <v>VSS</v>
@@ -7203,7 +7394,10 @@
         <v>SCAN_OUT</v>
       </c>
     </row>
-    <row r="15" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="99">
+        <v>7</v>
+      </c>
       <c r="B15" s="44" t="str">
         <f>LEFT(Full!AA17,(FIND(";",Full!AA17,1)-1))</f>
         <v>VSS</v>
@@ -7309,7 +7503,10 @@
         <v>VSS</v>
       </c>
     </row>
-    <row r="16" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="99">
+        <v>8</v>
+      </c>
       <c r="B16" s="45" t="str">
         <f>LEFT(Full!AA18,(FIND(";",Full!AA18,1)-1))</f>
         <v>LINK_BM_TX_1_P</v>
@@ -7422,7 +7619,10 @@
         <v>376</v>
       </c>
     </row>
-    <row r="17" spans="2:38" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="99">
+        <v>9</v>
+      </c>
       <c r="B17" s="45" t="str">
         <f>LEFT(Full!AA19,(FIND(";",Full!AA19,1)-1))</f>
         <v>LINK_BM_TX_1_N</v>
@@ -7535,7 +7735,10 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="2:38" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="99">
+        <v>10</v>
+      </c>
       <c r="B18" s="44" t="str">
         <f>LEFT(Full!AA20,(FIND(";",Full!AA20,1)-1))</f>
         <v>VSS</v>
@@ -7648,7 +7851,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="99">
+        <v>11</v>
+      </c>
       <c r="B19" s="45" t="str">
         <f>LEFT(Full!AA21,(FIND(";",Full!AA21,1)-1))</f>
         <v>LINK_BM_RX_1_P</v>
@@ -7761,7 +7967,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="99">
+        <v>12</v>
+      </c>
       <c r="B20" s="45" t="str">
         <f>LEFT(Full!AA22,(FIND(";",Full!AA22,1)-1))</f>
         <v>LINK_BM_RX_1_N</v>
@@ -7874,7 +8083,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="99">
+        <v>13</v>
+      </c>
       <c r="B21" s="44" t="str">
         <f>LEFT(Full!AA23,(FIND(";",Full!AA23,1)-1))</f>
         <v>VSS</v>
@@ -7987,7 +8199,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="99">
+        <v>14</v>
+      </c>
       <c r="B22" s="45" t="str">
         <f>LEFT(Full!AA24,(FIND(";",Full!AA24,1)-1))</f>
         <v>LINK_CM_TX_0_P</v>
@@ -8093,7 +8308,10 @@
         <v>LINK_CM_RX_1_P</v>
       </c>
     </row>
-    <row r="23" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="99">
+        <v>15</v>
+      </c>
       <c r="B23" s="45" t="str">
         <f>LEFT(Full!AA25,(FIND(";",Full!AA25,1)-1))</f>
         <v>LINK_CM_TX_0_N</v>
@@ -8206,7 +8424,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="99">
+        <v>16</v>
+      </c>
       <c r="B24" s="44" t="str">
         <f>LEFT(Full!AA26,(FIND(";",Full!AA26,1)-1))</f>
         <v>VSS</v>
@@ -8319,7 +8540,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:38" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="99">
+        <v>17</v>
+      </c>
       <c r="B25" s="45" t="str">
         <f>LEFT(Full!AA27,(FIND(";",Full!AA27,1)-1))</f>
         <v>LINK_CM_RX_0_P</v>
@@ -8432,7 +8656,10 @@
         <v>635</v>
       </c>
     </row>
-    <row r="26" spans="2:38" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="99">
+        <v>18</v>
+      </c>
       <c r="B26" s="45" t="str">
         <f>LEFT(Full!AA28,(FIND(";",Full!AA28,1)-1))</f>
         <v>LINK_CM_RX_0_N</v>
@@ -8538,7 +8765,10 @@
         <v>LINK_CM_TX_1_N</v>
       </c>
     </row>
-    <row r="27" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="99">
+        <v>19</v>
+      </c>
       <c r="B27" s="44" t="str">
         <f>LEFT(Full!AA29,(FIND(";",Full!AA29,1)-1))</f>
         <v>VSS</v>
@@ -8644,7 +8874,10 @@
         <v>VSS</v>
       </c>
     </row>
-    <row r="28" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="99">
+        <v>20</v>
+      </c>
       <c r="B28" s="4" t="str">
         <f>LEFT(Full!AA30,(FIND(";",Full!AA30,1)-1))</f>
         <v>REF_SERDES_CM0_P</v>
@@ -8750,7 +8983,10 @@
         <v>REF_SERDES_CM1_P</v>
       </c>
     </row>
-    <row r="29" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="99">
+        <v>21</v>
+      </c>
       <c r="B29" s="4" t="str">
         <f>LEFT(Full!AA31,(FIND(";",Full!AA31,1)-1))</f>
         <v>REF_SERDES_CM0_N</v>
@@ -8856,7 +9092,10 @@
         <v>REF_SERDES_CM1_N</v>
       </c>
     </row>
-    <row r="30" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="99">
+        <v>22</v>
+      </c>
       <c r="B30" s="44" t="str">
         <f>LEFT(Full!AA32,(FIND(";",Full!AA32,1)-1))</f>
         <v>VSS</v>
@@ -8962,7 +9201,10 @@
         <v>VSS</v>
       </c>
     </row>
-    <row r="31" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="99">
+        <v>23</v>
+      </c>
       <c r="B31" s="46" t="str">
         <f>LEFT(Full!AA33,(FIND(";",Full!AA33,1)-1))</f>
         <v>REF_DIG_N</v>
@@ -9068,7 +9310,10 @@
         <v>REF_LO_N</v>
       </c>
     </row>
-    <row r="32" spans="2:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="99">
+        <v>24</v>
+      </c>
       <c r="B32" s="46" t="str">
         <f>LEFT(Full!AA34,(FIND(";",Full!AA34,1)-1))</f>
         <v>REF_DIG_P</v>
@@ -9174,7 +9419,10 @@
         <v>REF_LO_P</v>
       </c>
     </row>
-    <row r="33" spans="2:27" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="99">
+        <v>25</v>
+      </c>
       <c r="B33" s="44" t="str">
         <f>LEFT(Full!AA35,(FIND(";",Full!AA35,1)-1))</f>
         <v>VSS</v>
@@ -9280,7 +9528,10 @@
         <v>VSS</v>
       </c>
     </row>
-    <row r="34" spans="2:27" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="99">
+        <v>26</v>
+      </c>
       <c r="B34" s="43" t="str">
         <f>LEFT(Full!AA36,(FIND(";",Full!AA36,1)-1))</f>
         <v>NC</v>

</xml_diff>

<commit_message>
Added a BUMPS_DOWN_check tab to the Fader2_bumps workbook to help update net name assignments.
</commit_message>
<xml_diff>
--- a/Files_for_TestPlan_TestReports/FADER2_bumps.xlsx
+++ b/Files_for_TestPlan_TestReports/FADER2_bumps.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caolen\Nokia\Fader2.5\fader25_pcb\Files_for_TestPlan_TestReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1326A3-9C62-430F-B85D-E5321EDB525D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4807E160-1154-40C2-81D5-B168F491B0A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32205" yWindow="1320" windowWidth="21420" windowHeight="13425" tabRatio="240" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="240" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="1" r:id="rId1"/>
     <sheet name="Visual" sheetId="2" r:id="rId2"/>
     <sheet name="BUMP_DOWN" sheetId="4" r:id="rId3"/>
     <sheet name="Bare_for_export" sheetId="3" r:id="rId4"/>
+    <sheet name="BUMP_DOWN_check" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -30,8 +31,728 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={72BF5544-6E4C-4260-861A-7DF0C0773E58}</author>
+    <author>tc={07FFC8DB-00CB-441D-81E9-CEF80015BDB8}</author>
+    <author>tc={F97D81D6-3435-445F-9756-060110178598}</author>
+    <author>tc={EB4B2C77-9F1F-4170-9D0B-9709DFF32126}</author>
+    <author>tc={C5245D0F-4CAF-4FB0-A6D5-91B4CD388C89}</author>
+    <author>tc={50E10842-8EFF-4D34-8A51-123726BE6F6B}</author>
+    <author>tc={DAB148A7-F441-46DA-8DC3-DE6FE557AE96}</author>
+    <author>tc={50512406-1CC6-4565-9B77-F05E7EAE91AD}</author>
+    <author>tc={C1F2DFD1-A430-4890-A638-2486ED63CD17}</author>
+    <author>tc={4C420710-A9DB-42EE-B058-CA59688F3B86}</author>
+    <author>tc={DA6386B9-1FD4-419C-B1E6-2F4E1CB7CD71}</author>
+    <author>tc={AEE4803A-8ED7-4A0D-8FC8-D16FFEAD89F8}</author>
+    <author>tc={BA08210C-B7BC-4987-9939-E431144246CC}</author>
+    <author>tc={CEA60AD4-58B0-4A8D-B7A6-F45D2F5FD83B}</author>
+    <author>tc={A772F140-AD77-4F14-A0CA-D2CD7AC79D91}</author>
+    <author>tc={BCE21385-98BE-4BEA-ADF4-3EEBF80D504C}</author>
+    <author>tc={34EE0504-7808-474C-8C56-6BE9AD951A47}</author>
+    <author>tc={4714F8D3-78A5-4D15-95EC-73F897501234}</author>
+    <author>tc={BEC48103-4F21-465C-B878-6A362A258000}</author>
+    <author>tc={D169EA82-9331-4B93-B5DB-1236B7C7D343}</author>
+    <author>tc={271D7E9C-3D49-4294-B48D-FCCCECDC01DE}</author>
+    <author>tc={0E88173D-1B6E-44EB-A6B9-8124F1E99ADF}</author>
+    <author>tc={AF8A0F6A-C550-4837-A29B-CFB5CE37D6B5}</author>
+    <author>tc={CCA9BBA6-5E87-4F5D-B513-96E58D1D55D8}</author>
+    <author>tc={A8193393-567D-4FB1-8C10-8DE8516EA36F}</author>
+    <author>tc={F51FF2AF-1BC0-424B-8EF5-66E28532DE1F}</author>
+    <author>tc={86E0457B-BF6B-41DF-AA9C-13E48880862A}</author>
+    <author>tc={3CF118FD-8949-4324-89C1-907E716D08B2}</author>
+    <author>tc={E10383B7-2BD9-4C18-B5C9-318A318E246E}</author>
+    <author>tc={BD0CA3F6-892E-4F88-8410-D6864381D1C6}</author>
+    <author>tc={923A4E5C-3372-4240-89EA-15C1F093AF41}</author>
+    <author>tc={0376D20D-F711-42E1-9D6D-21C15A7C509D}</author>
+    <author>tc={35883730-4232-493F-B275-864B7CF9086A}</author>
+    <author>tc={EA8FE9C6-2D25-4B90-A56B-AEA4CB9C9214}</author>
+    <author>tc={21355403-593A-474E-8965-4879B24CBFE0}</author>
+    <author>tc={338EAC44-897B-4346-9E19-EFA43384781E}</author>
+    <author>tc={8FE1819E-0BEE-4464-AB1C-ADA246A4ACAC}</author>
+    <author>tc={630C4277-0F09-49CC-90D7-89CD79ED4150}</author>
+    <author>tc={8DA8A712-8A17-414E-A30C-BF3B285B86A0}</author>
+    <author>tc={B52E8732-89FA-4C4D-B4DD-62BFB5AE57F4}</author>
+    <author>tc={4C7C81D2-2274-400B-90BC-3AEC5ED46DFC}</author>
+    <author>tc={65D18A92-7EDC-487D-9F58-FCAF8BEB2730}</author>
+    <author>tc={31E81C72-2707-473D-8B66-5D07BC647E41}</author>
+    <author>tc={D9EA80F6-EBED-484B-9B74-3FCC53D5C5FF}</author>
+    <author>tc={79AC39A9-ECDA-4D79-830A-A14066B9D6E9}</author>
+    <author>tc={ECC3531B-A123-4346-8600-942D8E905BFA}</author>
+    <author>tc={1BDB793F-810B-4DB4-AFB5-59F2E798C70E}</author>
+    <author>tc={82FB3759-6DA0-4A12-92A1-09908ECDDC4F}</author>
+    <author>tc={1C038F2A-9667-4044-AD01-66BFB79D212F}</author>
+    <author>tc={92021650-A28A-44BE-B200-18038E6B548F}</author>
+    <author>tc={6F32BCA3-890A-4030-9F7B-6253C18398DA}</author>
+    <author>tc={6328544A-A105-4DEA-A47F-F3A50FEEF063}</author>
+    <author>tc={B9F37386-8589-4F8C-866B-3569CAC1C64C}</author>
+    <author>tc={72ABFD34-9472-43AA-BE20-CEEC9BE7083B}</author>
+    <author>tc={3B2D0EC1-7ABB-42C7-BB93-D05F9DB7799F}</author>
+    <author>tc={196BD3E2-312E-4A5F-AE8C-FD75B44A4D77}</author>
+    <author>tc={A864D4D3-48D8-4F07-8338-DD6C186A0DB1}</author>
+    <author>tc={C21EAAA1-9677-428A-8975-0EE797D2FD3E}</author>
+    <author>tc={D0B86361-B267-469B-A913-0ED48C80B9B0}</author>
+    <author>tc={82727AEF-4CE7-416B-8A72-28535D4CDAFE}</author>
+    <author>tc={C771EE25-DBDE-412D-A7C3-B5A36FA4E03E}</author>
+    <author>tc={F5FF36FF-16D8-4D90-A0F4-C7FC396E4741}</author>
+    <author>tc={453E0200-CBB6-4ED3-909C-DB413B9E4134}</author>
+    <author>tc={50123A26-4948-411F-94BB-B861DE890CE7}</author>
+    <author>tc={9FCC5101-B6A3-4CB7-B9D6-6CE1E7063281}</author>
+    <author>tc={7B796589-9FAD-439C-ACEB-1121FDBE7AB4}</author>
+    <author>tc={783A25C7-6779-4AAC-8913-E3E01C8644A8}</author>
+    <author>tc={3133F592-E218-40B5-A909-8363689D7F62}</author>
+    <author>tc={27561DAC-AD42-4E8E-B1A7-481E5A33F5F1}</author>
+    <author>tc={ACBF3C48-384A-4624-9FD4-2642750D6EA2}</author>
+    <author>tc={B98B5302-3608-4131-B7FC-2FB1FD18C20B}</author>
+    <author>tc={F6C408AE-946D-4F18-B174-FB8BE5162B3D}</author>
+    <author>tc={A27919A6-6C60-4493-9EE5-8CBA8D5B41BC}</author>
+    <author>tc={82C3863C-7A2F-4AA4-A210-F29E147E7CFF}</author>
+    <author>tc={DCB6335D-714E-431B-83ED-90AE2374745C}</author>
+    <author>tc={3D4905E5-FD6D-4403-8BE9-BF98C15BCC5F}</author>
+    <author>tc={4B692865-6B4E-42F0-8D9A-C1DA5C4342D3}</author>
+    <author>tc={7D5D6B88-96CD-4D89-AA5C-E071AE4C447B}</author>
+    <author>tc={20ED06F7-69CE-4EAD-AF35-ACA3E0F76812}</author>
+  </authors>
+  <commentList>
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{72BF5544-6E4C-4260-861A-7DF0C0773E58}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Y1</t>
+      </text>
+    </comment>
+    <comment ref="K9" authorId="1" shapeId="0" xr:uid="{07FFC8DB-00CB-441D-81E9-CEF80015BDB8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_T1</t>
+      </text>
+    </comment>
+    <comment ref="L9" authorId="2" shapeId="0" xr:uid="{F97D81D6-3435-445F-9756-060110178598}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_T1</t>
+      </text>
+    </comment>
+    <comment ref="N9" authorId="3" shapeId="0" xr:uid="{EB4B2C77-9F1F-4170-9D0B-9709DFF32126}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_N1</t>
+      </text>
+    </comment>
+    <comment ref="O9" authorId="4" shapeId="0" xr:uid="{C5245D0F-4CAF-4FB0-A6D5-91B4CD388C89}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_N1</t>
+      </text>
+    </comment>
+    <comment ref="Q9" authorId="5" shapeId="0" xr:uid="{50E10842-8EFF-4D34-8A51-123726BE6F6B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    L1</t>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="6" shapeId="0" xr:uid="{DAB148A7-F441-46DA-8DC3-DE6FE557AE96}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P2</t>
+      </text>
+    </comment>
+    <comment ref="N10" authorId="7" shapeId="0" xr:uid="{50512406-1CC6-4565-9B77-F05E7EAE91AD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P2</t>
+      </text>
+    </comment>
+    <comment ref="M11" authorId="8" shapeId="0" xr:uid="{C1F2DFD1-A430-4890-A638-2486ED63CD17}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P2</t>
+      </text>
+    </comment>
+    <comment ref="N11" authorId="9" shapeId="0" xr:uid="{4C420710-A9DB-42EE-B058-CA59688F3B86}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P2</t>
+      </text>
+    </comment>
+    <comment ref="M13" authorId="10" shapeId="0" xr:uid="{DA6386B9-1FD4-419C-B1E6-2F4E1CB7CD71}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P5</t>
+      </text>
+    </comment>
+    <comment ref="N13" authorId="11" shapeId="0" xr:uid="{AEE4803A-8ED7-4A0D-8FC8-D16FFEAD89F8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P5</t>
+      </text>
+    </comment>
+    <comment ref="M14" authorId="12" shapeId="0" xr:uid="{BA08210C-B7BC-4987-9939-E431144246CC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P5</t>
+      </text>
+    </comment>
+    <comment ref="N14" authorId="13" shapeId="0" xr:uid="{CEA60AD4-58B0-4A8D-B7A6-F45D2F5FD83B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P5</t>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="14" shapeId="0" xr:uid="{A772F140-AD77-4F14-A0CA-D2CD7AC79D91}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD8</t>
+      </text>
+    </comment>
+    <comment ref="C16" authorId="15" shapeId="0" xr:uid="{BCE21385-98BE-4BEA-ADF4-3EEBF80D504C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD8</t>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="16" shapeId="0" xr:uid="{34EE0504-7808-474C-8C56-6BE9AD951A47}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD8</t>
+      </text>
+    </comment>
+    <comment ref="Y16" authorId="17" shapeId="0" xr:uid="{4714F8D3-78A5-4D15-95EC-73F897501234}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A8</t>
+      </text>
+    </comment>
+    <comment ref="Z16" authorId="18" shapeId="0" xr:uid="{BEC48103-4F21-465C-B878-6A362A258000}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A8</t>
+      </text>
+    </comment>
+    <comment ref="AA16" authorId="19" shapeId="0" xr:uid="{D169EA82-9331-4B93-B5DB-1236B7C7D343}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A8</t>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="20" shapeId="0" xr:uid="{271D7E9C-3D49-4294-B48D-FCCCECDC01DE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD8</t>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="21" shapeId="0" xr:uid="{0E88173D-1B6E-44EB-A6B9-8124F1E99ADF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD8</t>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="22" shapeId="0" xr:uid="{AF8A0F6A-C550-4837-A29B-CFB5CE37D6B5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD8</t>
+      </text>
+    </comment>
+    <comment ref="Y17" authorId="23" shapeId="0" xr:uid="{CCA9BBA6-5E87-4F5D-B513-96E58D1D55D8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A8</t>
+      </text>
+    </comment>
+    <comment ref="Z17" authorId="24" shapeId="0" xr:uid="{A8193393-567D-4FB1-8C10-8DE8516EA36F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A8</t>
+      </text>
+    </comment>
+    <comment ref="AA17" authorId="25" shapeId="0" xr:uid="{F51FF2AF-1BC0-424B-8EF5-66E28532DE1F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A8</t>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="26" shapeId="0" xr:uid="{86E0457B-BF6B-41DF-AA9C-13E48880862A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD11</t>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="27" shapeId="0" xr:uid="{3CF118FD-8949-4324-89C1-907E716D08B2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD11</t>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="28" shapeId="0" xr:uid="{E10383B7-2BD9-4C18-B5C9-318A318E246E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD11</t>
+      </text>
+    </comment>
+    <comment ref="Y19" authorId="29" shapeId="0" xr:uid="{BD0CA3F6-892E-4F88-8410-D6864381D1C6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A11</t>
+      </text>
+    </comment>
+    <comment ref="Z19" authorId="30" shapeId="0" xr:uid="{923A4E5C-3372-4240-89EA-15C1F093AF41}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A11</t>
+      </text>
+    </comment>
+    <comment ref="AA19" authorId="31" shapeId="0" xr:uid="{0376D20D-F711-42E1-9D6D-21C15A7C509D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A11</t>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="32" shapeId="0" xr:uid="{35883730-4232-493F-B275-864B7CF9086A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD11</t>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="33" shapeId="0" xr:uid="{EA8FE9C6-2D25-4B90-A56B-AEA4CB9C9214}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD11</t>
+      </text>
+    </comment>
+    <comment ref="D20" authorId="34" shapeId="0" xr:uid="{21355403-593A-474E-8965-4879B24CBFE0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD11</t>
+      </text>
+    </comment>
+    <comment ref="Y20" authorId="35" shapeId="0" xr:uid="{338EAC44-897B-4346-9E19-EFA43384781E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A11</t>
+      </text>
+    </comment>
+    <comment ref="Z20" authorId="36" shapeId="0" xr:uid="{8FE1819E-0BEE-4464-AB1C-ADA246A4ACAC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A11</t>
+      </text>
+    </comment>
+    <comment ref="AA20" authorId="37" shapeId="0" xr:uid="{630C4277-0F09-49CC-90D7-89CD79ED4150}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A11</t>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="38" shapeId="0" xr:uid="{8DA8A712-8A17-414E-A30C-BF3B285B86A0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD14</t>
+      </text>
+    </comment>
+    <comment ref="C22" authorId="39" shapeId="0" xr:uid="{B52E8732-89FA-4C4D-B4DD-62BFB5AE57F4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD14</t>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="40" shapeId="0" xr:uid="{4C7C81D2-2274-400B-90BC-3AEC5ED46DFC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD14</t>
+      </text>
+    </comment>
+    <comment ref="Y22" authorId="41" shapeId="0" xr:uid="{65D18A92-7EDC-487D-9F58-FCAF8BEB2730}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    GATE_LINK</t>
+      </text>
+    </comment>
+    <comment ref="Z22" authorId="42" shapeId="0" xr:uid="{31E81C72-2707-473D-8B66-5D07BC647E41}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    GATE_LINK</t>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="43" shapeId="0" xr:uid="{D9EA80F6-EBED-484B-9B74-3FCC53D5C5FF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD14</t>
+      </text>
+    </comment>
+    <comment ref="C23" authorId="44" shapeId="0" xr:uid="{79AC39A9-ECDA-4D79-830A-A14066B9D6E9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD14</t>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="45" shapeId="0" xr:uid="{ECC3531B-A123-4346-8600-942D8E905BFA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD14</t>
+      </text>
+    </comment>
+    <comment ref="Y23" authorId="46" shapeId="0" xr:uid="{1BDB793F-810B-4DB4-AFB5-59F2E798C70E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    GATE_LINK</t>
+      </text>
+    </comment>
+    <comment ref="Z23" authorId="47" shapeId="0" xr:uid="{82FB3759-6DA0-4A12-92A1-09908ECDDC4F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    GATE_LINK</t>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="48" shapeId="0" xr:uid="{1C038F2A-9667-4044-AD01-66BFB79D212F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD17</t>
+      </text>
+    </comment>
+    <comment ref="C25" authorId="49" shapeId="0" xr:uid="{92021650-A28A-44BE-B200-18038E6B548F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD17</t>
+      </text>
+    </comment>
+    <comment ref="D25" authorId="50" shapeId="0" xr:uid="{6F32BCA3-890A-4030-9F7B-6253C18398DA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD17</t>
+      </text>
+    </comment>
+    <comment ref="Y25" authorId="51" shapeId="0" xr:uid="{6328544A-A105-4DEA-A47F-F3A50FEEF063}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    VDD_LINK</t>
+      </text>
+    </comment>
+    <comment ref="Z25" authorId="52" shapeId="0" xr:uid="{B9F37386-8589-4F8C-866B-3569CAC1C64C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    VDD_LINK</t>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="53" shapeId="0" xr:uid="{72ABFD34-9472-43AA-BE20-CEEC9BE7083B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD17</t>
+      </text>
+    </comment>
+    <comment ref="C26" authorId="54" shapeId="0" xr:uid="{3B2D0EC1-7ABB-42C7-BB93-D05F9DB7799F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD17</t>
+      </text>
+    </comment>
+    <comment ref="D26" authorId="55" shapeId="0" xr:uid="{196BD3E2-312E-4A5F-AE8C-FD75B44A4D77}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD17</t>
+      </text>
+    </comment>
+    <comment ref="Y26" authorId="56" shapeId="0" xr:uid="{A864D4D3-48D8-4F07-8338-DD6C186A0DB1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    VDD_LINK</t>
+      </text>
+    </comment>
+    <comment ref="Z26" authorId="57" shapeId="0" xr:uid="{C21EAAA1-9677-428A-8975-0EE797D2FD3E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    VDD_LINK</t>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="58" shapeId="0" xr:uid="{D0B86361-B267-469B-A913-0ED48C80B9B0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AF20</t>
+      </text>
+    </comment>
+    <comment ref="AA28" authorId="59" shapeId="0" xr:uid="{82727AEF-4CE7-416B-8A72-28535D4CDAFE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A20</t>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="60" shapeId="0" xr:uid="{C771EE25-DBDE-412D-A7C3-B5A36FA4E03E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AF20</t>
+      </text>
+    </comment>
+    <comment ref="L29" authorId="61" shapeId="0" xr:uid="{F5FF36FF-16D8-4D90-A0F4-C7FC396E4741}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R21</t>
+      </text>
+    </comment>
+    <comment ref="M29" authorId="62" shapeId="0" xr:uid="{453E0200-CBB6-4ED3-909C-DB413B9E4134}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R21</t>
+      </text>
+    </comment>
+    <comment ref="AA29" authorId="63" shapeId="0" xr:uid="{50123A26-4948-411F-94BB-B861DE890CE7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A20</t>
+      </text>
+    </comment>
+    <comment ref="L30" authorId="64" shapeId="0" xr:uid="{9FCC5101-B6A3-4CB7-B9D6-6CE1E7063281}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R21</t>
+      </text>
+    </comment>
+    <comment ref="M30" authorId="65" shapeId="0" xr:uid="{7B796589-9FAD-439C-ACEB-1121FDBE7AB4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R21</t>
+      </text>
+    </comment>
+    <comment ref="B31" authorId="66" shapeId="0" xr:uid="{783A25C7-6779-4AAC-8913-E3E01C8644A8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AF23</t>
+      </text>
+    </comment>
+    <comment ref="AA31" authorId="67" shapeId="0" xr:uid="{3133F592-E218-40B5-A909-8363689D7F62}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A23</t>
+      </text>
+    </comment>
+    <comment ref="B32" authorId="68" shapeId="0" xr:uid="{27561DAC-AD42-4E8E-B1A7-481E5A33F5F1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AF23</t>
+      </text>
+    </comment>
+    <comment ref="L32" authorId="69" shapeId="0" xr:uid="{ACBF3C48-384A-4624-9FD4-2642750D6EA2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R24</t>
+      </text>
+    </comment>
+    <comment ref="M32" authorId="70" shapeId="0" xr:uid="{B98B5302-3608-4131-B7FC-2FB1FD18C20B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R24</t>
+      </text>
+    </comment>
+    <comment ref="AA32" authorId="71" shapeId="0" xr:uid="{F6C408AE-946D-4F18-B174-FB8BE5162B3D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A23</t>
+      </text>
+    </comment>
+    <comment ref="L33" authorId="72" shapeId="0" xr:uid="{A27919A6-6C60-4493-9EE5-8CBA8D5B41BC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R24</t>
+      </text>
+    </comment>
+    <comment ref="M33" authorId="73" shapeId="0" xr:uid="{82C3863C-7A2F-4AA4-A210-F29E147E7CFF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R24</t>
+      </text>
+    </comment>
+    <comment ref="K34" authorId="74" shapeId="0" xr:uid="{DCB6335D-714E-431B-83ED-90AE2374745C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_T26</t>
+      </text>
+    </comment>
+    <comment ref="L34" authorId="75" shapeId="0" xr:uid="{3D4905E5-FD6D-4403-8BE9-BF98C15BCC5F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_T26</t>
+      </text>
+    </comment>
+    <comment ref="N34" authorId="76" shapeId="0" xr:uid="{4B692865-6B4E-42F0-8D9A-C1DA5C4342D3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_N26</t>
+      </text>
+    </comment>
+    <comment ref="O34" authorId="77" shapeId="0" xr:uid="{7D5D6B88-96CD-4D89-AA5C-E071AE4C447B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_N26</t>
+      </text>
+    </comment>
+    <comment ref="Q34" authorId="78" shapeId="0" xr:uid="{20ED06F7-69CE-4EAD-AF35-ACA3E0F76812}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    L26</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="126">
   <si>
     <t>name</t>
   </si>
@@ -415,7 +1136,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -465,8 +1186,26 @@
       <name val="Comic Sans MS"/>
       <family val="4"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -569,8 +1308,62 @@
         <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FFF8CBAD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FFBDD7EE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF0066CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FFDF0015"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -804,11 +1597,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1105,6 +1965,108 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1179,6 +2141,7 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FFE07070"/>
       <color rgb="FFDF0015"/>
       <color rgb="FFBDD7EE"/>
@@ -1194,6 +2157,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Olen, Carl (Nokia - US)" id="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" userId="S::carl.olen@nokia-bell-labs.com::4757c402-796e-42cf-aeaa-1493fc214845" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1457,6 +2426,248 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H9" dT="2020-05-15T20:56:53.35" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{72BF5544-6E4C-4260-861A-7DF0C0773E58}">
+    <text>Y1</text>
+  </threadedComment>
+  <threadedComment ref="K9" dT="2020-05-15T20:54:58.15" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{07FFC8DB-00CB-441D-81E9-CEF80015BDB8}">
+    <text>NetU2_T1</text>
+  </threadedComment>
+  <threadedComment ref="L9" dT="2020-05-15T20:54:49.29" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{F97D81D6-3435-445F-9756-060110178598}">
+    <text>NetU2_T1</text>
+  </threadedComment>
+  <threadedComment ref="N9" dT="2020-05-15T20:52:23.87" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{EB4B2C77-9F1F-4170-9D0B-9709DFF32126}">
+    <text>NetU2_N1</text>
+  </threadedComment>
+  <threadedComment ref="O9" dT="2020-05-15T20:52:16.80" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{C5245D0F-4CAF-4FB0-A6D5-91B4CD388C89}">
+    <text>NetU2_N1</text>
+  </threadedComment>
+  <threadedComment ref="Q9" dT="2020-05-15T20:51:25.87" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{50E10842-8EFF-4D34-8A51-123726BE6F6B}">
+    <text>L1</text>
+  </threadedComment>
+  <threadedComment ref="M10" dT="2020-05-15T20:53:26.00" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{DAB148A7-F441-46DA-8DC3-DE6FE557AE96}">
+    <text>NetU2_P2</text>
+  </threadedComment>
+  <threadedComment ref="N10" dT="2020-05-15T20:53:43.70" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{50512406-1CC6-4565-9B77-F05E7EAE91AD}">
+    <text>NetU2_P2</text>
+  </threadedComment>
+  <threadedComment ref="M11" dT="2020-05-15T20:53:33.09" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{C1F2DFD1-A430-4890-A638-2486ED63CD17}">
+    <text>NetU2_P2</text>
+  </threadedComment>
+  <threadedComment ref="N11" dT="2020-05-15T20:53:51.71" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{4C420710-A9DB-42EE-B058-CA59688F3B86}">
+    <text>NetU2_P2</text>
+  </threadedComment>
+  <threadedComment ref="M13" dT="2020-05-15T20:41:11.70" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{DA6386B9-1FD4-419C-B1E6-2F4E1CB7CD71}">
+    <text>NetU2_P5</text>
+  </threadedComment>
+  <threadedComment ref="N13" dT="2020-05-15T20:41:25.62" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{AEE4803A-8ED7-4A0D-8FC8-D16FFEAD89F8}">
+    <text>NetU2_P5</text>
+  </threadedComment>
+  <threadedComment ref="M14" dT="2020-05-15T20:41:18.39" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{BA08210C-B7BC-4987-9939-E431144246CC}">
+    <text>NetU2_P5</text>
+  </threadedComment>
+  <threadedComment ref="N14" dT="2020-05-15T20:41:32.16" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{CEA60AD4-58B0-4A8D-B7A6-F45D2F5FD83B}">
+    <text>NetU2_P5</text>
+  </threadedComment>
+  <threadedComment ref="B16" dT="2020-05-15T20:35:50.09" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{A772F140-AD77-4F14-A0CA-D2CD7AC79D91}">
+    <text>NetU2_AD8</text>
+  </threadedComment>
+  <threadedComment ref="C16" dT="2020-05-15T20:36:04.68" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{BCE21385-98BE-4BEA-ADF4-3EEBF80D504C}">
+    <text>NetU2_AD8</text>
+  </threadedComment>
+  <threadedComment ref="D16" dT="2020-05-15T20:36:19.20" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{34EE0504-7808-474C-8C56-6BE9AD951A47}">
+    <text>NetU2_AD8</text>
+  </threadedComment>
+  <threadedComment ref="Y16" dT="2020-05-15T20:46:02.29" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{4714F8D3-78A5-4D15-95EC-73F897501234}">
+    <text>NetU2_A8</text>
+  </threadedComment>
+  <threadedComment ref="Z16" dT="2020-05-15T20:46:18.92" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{BEC48103-4F21-465C-B878-6A362A258000}">
+    <text>NetU2_A8</text>
+  </threadedComment>
+  <threadedComment ref="AA16" dT="2020-05-15T20:46:38.89" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{D169EA82-9331-4B93-B5DB-1236B7C7D343}">
+    <text>NetU2_A8</text>
+  </threadedComment>
+  <threadedComment ref="B17" dT="2020-05-15T20:35:57.05" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{271D7E9C-3D49-4294-B48D-FCCCECDC01DE}">
+    <text>NetU2_AD8</text>
+  </threadedComment>
+  <threadedComment ref="C17" dT="2020-05-15T20:36:11.63" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{0E88173D-1B6E-44EB-A6B9-8124F1E99ADF}">
+    <text>NetU2_AD8</text>
+  </threadedComment>
+  <threadedComment ref="D17" dT="2020-05-15T20:36:32.64" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{AF8A0F6A-C550-4837-A29B-CFB5CE37D6B5}">
+    <text>NetU2_AD8</text>
+  </threadedComment>
+  <threadedComment ref="Y17" dT="2020-05-15T20:46:11.27" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{CCA9BBA6-5E87-4F5D-B513-96E58D1D55D8}">
+    <text>NetU2_A8</text>
+  </threadedComment>
+  <threadedComment ref="Z17" dT="2020-05-15T20:46:26.93" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{A8193393-567D-4FB1-8C10-8DE8516EA36F}">
+    <text>NetU2_A8</text>
+  </threadedComment>
+  <threadedComment ref="AA17" dT="2020-05-15T20:46:45.92" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{F51FF2AF-1BC0-424B-8EF5-66E28532DE1F}">
+    <text>NetU2_A8</text>
+  </threadedComment>
+  <threadedComment ref="B19" dT="2020-05-15T20:30:44.32" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{86E0457B-BF6B-41DF-AA9C-13E48880862A}">
+    <text>NetU2_AD11</text>
+  </threadedComment>
+  <threadedComment ref="C19" dT="2020-05-15T20:30:58.35" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{3CF118FD-8949-4324-89C1-907E716D08B2}">
+    <text>NetU2_AD11</text>
+  </threadedComment>
+  <threadedComment ref="D19" dT="2020-05-15T20:31:11.27" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{E10383B7-2BD9-4C18-B5C9-318A318E246E}">
+    <text>NetU2_AD11</text>
+  </threadedComment>
+  <threadedComment ref="Y19" dT="2020-05-15T20:20:41.48" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{BD0CA3F6-892E-4F88-8410-D6864381D1C6}">
+    <text>NetU2_A11</text>
+  </threadedComment>
+  <threadedComment ref="Z19" dT="2020-05-15T20:20:10.90" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{923A4E5C-3372-4240-89EA-15C1F093AF41}">
+    <text>NetU2_A11</text>
+  </threadedComment>
+  <threadedComment ref="AA19" dT="2020-05-15T20:19:54.58" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{0376D20D-F711-42E1-9D6D-21C15A7C509D}">
+    <text>NetU2_A11</text>
+  </threadedComment>
+  <threadedComment ref="B20" dT="2020-05-15T20:30:51.21" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{35883730-4232-493F-B275-864B7CF9086A}">
+    <text>NetU2_AD11</text>
+  </threadedComment>
+  <threadedComment ref="C20" dT="2020-05-15T20:31:04.40" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{EA8FE9C6-2D25-4B90-A56B-AEA4CB9C9214}">
+    <text>NetU2_AD11</text>
+  </threadedComment>
+  <threadedComment ref="D20" dT="2020-05-15T20:31:17.84" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{21355403-593A-474E-8965-4879B24CBFE0}">
+    <text>NetU2_AD11</text>
+  </threadedComment>
+  <threadedComment ref="Y20" dT="2020-05-15T20:20:50.23" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{338EAC44-897B-4346-9E19-EFA43384781E}">
+    <text>NetU2_A11</text>
+  </threadedComment>
+  <threadedComment ref="Z20" dT="2020-05-15T20:20:18.73" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{8FE1819E-0BEE-4464-AB1C-ADA246A4ACAC}">
+    <text>NetU2_A11</text>
+  </threadedComment>
+  <threadedComment ref="AA20" dT="2020-05-15T20:20:03.70" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{630C4277-0F09-49CC-90D7-89CD79ED4150}">
+    <text>NetU2_A11</text>
+  </threadedComment>
+  <threadedComment ref="B22" dT="2020-05-15T20:32:13.93" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{8DA8A712-8A17-414E-A30C-BF3B285B86A0}">
+    <text>NetU2_AD14</text>
+  </threadedComment>
+  <threadedComment ref="C22" dT="2020-05-15T20:32:30.57" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{B52E8732-89FA-4C4D-B4DD-62BFB5AE57F4}">
+    <text>NetU2_AD14</text>
+  </threadedComment>
+  <threadedComment ref="D22" dT="2020-05-15T20:32:48.07" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{4C7C81D2-2274-400B-90BC-3AEC5ED46DFC}">
+    <text>NetU2_AD14</text>
+  </threadedComment>
+  <threadedComment ref="Y22" dT="2020-05-15T20:16:19.78" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{65D18A92-7EDC-487D-9F58-FCAF8BEB2730}">
+    <text>GATE_LINK</text>
+  </threadedComment>
+  <threadedComment ref="Z22" dT="2020-05-15T20:16:34.72" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{31E81C72-2707-473D-8B66-5D07BC647E41}">
+    <text>GATE_LINK</text>
+  </threadedComment>
+  <threadedComment ref="B23" dT="2020-05-15T20:32:21.08" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{D9EA80F6-EBED-484B-9B74-3FCC53D5C5FF}">
+    <text>NetU2_AD14</text>
+  </threadedComment>
+  <threadedComment ref="C23" dT="2020-05-15T20:32:37.61" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{79AC39A9-ECDA-4D79-830A-A14066B9D6E9}">
+    <text>NetU2_AD14</text>
+  </threadedComment>
+  <threadedComment ref="D23" dT="2020-05-15T20:32:54.75" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{ECC3531B-A123-4346-8600-942D8E905BFA}">
+    <text>NetU2_AD14</text>
+  </threadedComment>
+  <threadedComment ref="Y23" dT="2020-05-15T20:16:26.48" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{1BDB793F-810B-4DB4-AFB5-59F2E798C70E}">
+    <text>GATE_LINK</text>
+  </threadedComment>
+  <threadedComment ref="Z23" dT="2020-05-15T20:16:42.30" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{82FB3759-6DA0-4A12-92A1-09908ECDDC4F}">
+    <text>GATE_LINK</text>
+  </threadedComment>
+  <threadedComment ref="B25" dT="2020-05-15T20:04:43.01" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{1C038F2A-9667-4044-AD01-66BFB79D212F}">
+    <text>NetU2_AD17</text>
+  </threadedComment>
+  <threadedComment ref="C25" dT="2020-05-15T20:05:02.07" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{92021650-A28A-44BE-B200-18038E6B548F}">
+    <text>NetU2_AD17</text>
+  </threadedComment>
+  <threadedComment ref="D25" dT="2020-05-15T20:05:28.71" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{6F32BCA3-890A-4030-9F7B-6253C18398DA}">
+    <text>NetU2_AD17</text>
+  </threadedComment>
+  <threadedComment ref="Y25" dT="2020-05-15T20:12:22.99" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{6328544A-A105-4DEA-A47F-F3A50FEEF063}">
+    <text>VDD_LINK</text>
+  </threadedComment>
+  <threadedComment ref="Z25" dT="2020-05-15T20:12:42.14" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{B9F37386-8589-4F8C-866B-3569CAC1C64C}">
+    <text>VDD_LINK</text>
+  </threadedComment>
+  <threadedComment ref="B26" dT="2020-05-15T20:04:54.79" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{72ABFD34-9472-43AA-BE20-CEEC9BE7083B}">
+    <text>NetU2_AD17</text>
+  </threadedComment>
+  <threadedComment ref="C26" dT="2020-05-15T20:05:10.11" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{3B2D0EC1-7ABB-42C7-BB93-D05F9DB7799F}">
+    <text>NetU2_AD17</text>
+  </threadedComment>
+  <threadedComment ref="D26" dT="2020-05-15T20:05:37.06" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{196BD3E2-312E-4A5F-AE8C-FD75B44A4D77}">
+    <text>NetU2_AD17</text>
+  </threadedComment>
+  <threadedComment ref="Y26" dT="2020-05-15T20:12:31.13" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{A864D4D3-48D8-4F07-8338-DD6C186A0DB1}">
+    <text>VDD_LINK</text>
+  </threadedComment>
+  <threadedComment ref="Z26" dT="2020-05-15T20:12:49.17" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{C21EAAA1-9677-428A-8975-0EE797D2FD3E}">
+    <text>VDD_LINK</text>
+  </threadedComment>
+  <threadedComment ref="B28" dT="2020-05-15T19:59:04.10" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{D0B86361-B267-469B-A913-0ED48C80B9B0}">
+    <text>NetU2_AF20</text>
+  </threadedComment>
+  <threadedComment ref="AA28" dT="2020-05-15T19:48:01.53" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{82727AEF-4CE7-416B-8A72-28535D4CDAFE}">
+    <text>NetU2_A20</text>
+  </threadedComment>
+  <threadedComment ref="B29" dT="2020-05-15T19:59:12.64" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{C771EE25-DBDE-412D-A7C3-B5A36FA4E03E}">
+    <text>NetU2_AF20</text>
+  </threadedComment>
+  <threadedComment ref="L29" dT="2020-05-15T19:51:44.10" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{F5FF36FF-16D8-4D90-A0F4-C7FC396E4741}">
+    <text>NetU2_R21</text>
+  </threadedComment>
+  <threadedComment ref="M29" dT="2020-05-15T19:51:17.38" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{453E0200-CBB6-4ED3-909C-DB413B9E4134}">
+    <text>NetU2_R21</text>
+  </threadedComment>
+  <threadedComment ref="AA29" dT="2020-05-15T19:48:17.56" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{50123A26-4948-411F-94BB-B861DE890CE7}">
+    <text>NetU2_A20</text>
+  </threadedComment>
+  <threadedComment ref="L30" dT="2020-05-15T19:51:34.24" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{9FCC5101-B6A3-4CB7-B9D6-6CE1E7063281}">
+    <text>NetU2_R21</text>
+  </threadedComment>
+  <threadedComment ref="M30" dT="2020-05-15T19:51:25.29" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{7B796589-9FAD-439C-ACEB-1121FDBE7AB4}">
+    <text>NetU2_R21</text>
+  </threadedComment>
+  <threadedComment ref="B31" dT="2020-05-15T19:58:08.91" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{783A25C7-6779-4AAC-8913-E3E01C8644A8}">
+    <text>NetU2_AF23</text>
+  </threadedComment>
+  <threadedComment ref="AA31" dT="2020-05-15T19:45:57.55" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{3133F592-E218-40B5-A909-8363689D7F62}">
+    <text>NetU2_A23</text>
+  </threadedComment>
+  <threadedComment ref="B32" dT="2020-05-15T19:58:17.96" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{27561DAC-AD42-4E8E-B1A7-481E5A33F5F1}">
+    <text>NetU2_AF23</text>
+  </threadedComment>
+  <threadedComment ref="L32" dT="2020-05-15T19:53:02.98" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{ACBF3C48-384A-4624-9FD4-2642750D6EA2}">
+    <text>NetU2_R24</text>
+  </threadedComment>
+  <threadedComment ref="M32" dT="2020-05-15T19:52:38.06" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{B98B5302-3608-4131-B7FC-2FB1FD18C20B}">
+    <text>NetU2_R24</text>
+  </threadedComment>
+  <threadedComment ref="AA32" dT="2020-05-15T19:46:25.09" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{F6C408AE-946D-4F18-B174-FB8BE5162B3D}">
+    <text>NetU2_A23</text>
+  </threadedComment>
+  <threadedComment ref="L33" dT="2020-05-15T19:52:55.05" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{A27919A6-6C60-4493-9EE5-8CBA8D5B41BC}">
+    <text>NetU2_R24</text>
+  </threadedComment>
+  <threadedComment ref="M33" dT="2020-05-15T19:52:47.25" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{82C3863C-7A2F-4AA4-A210-F29E147E7CFF}">
+    <text>NetU2_R24</text>
+  </threadedComment>
+  <threadedComment ref="K34" dT="2020-05-15T18:49:03.85" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{DCB6335D-714E-431B-83ED-90AE2374745C}">
+    <text>NetU2_T26</text>
+  </threadedComment>
+  <threadedComment ref="L34" dT="2020-05-15T18:50:01.29" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{3D4905E5-FD6D-4403-8BE9-BF98C15BCC5F}">
+    <text>NetU2_T26</text>
+  </threadedComment>
+  <threadedComment ref="N34" dT="2020-05-15T18:51:24.80" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{4B692865-6B4E-42F0-8D9A-C1DA5C4342D3}">
+    <text>NetU2_N26</text>
+  </threadedComment>
+  <threadedComment ref="O34" dT="2020-05-15T18:53:37.25" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{7D5D6B88-96CD-4D89-AA5C-E071AE4C447B}">
+    <text>NetU2_N26</text>
+  </threadedComment>
+  <threadedComment ref="Q34" dT="2020-05-15T18:54:31.42" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{20ED06F7-69CE-4EAD-AF35-ACA3E0F76812}">
+    <text>L26</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AM49"/>
@@ -6613,8 +7824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F1D2C4-C567-4531-BCF2-31E88F3EC739}">
   <dimension ref="A2:AL34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A8" zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
+      <selection activeCell="AU26" sqref="AU26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6625,6 +7836,11 @@
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="H6" s="22">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12416,4 +13632,3048 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E75085E-B800-4513-AA14-6BE0CE50106A}">
+  <dimension ref="A2:AL34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A8" sqref="A8"/>
+      <selection pane="topRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="AF26" sqref="AF26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="H6" s="22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="98"/>
+      <c r="B8" s="99" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="99" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="99" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="99" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="99" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="99" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="99" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" s="99" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="99" t="s">
+        <v>117</v>
+      </c>
+      <c r="K8" s="99" t="s">
+        <v>116</v>
+      </c>
+      <c r="L8" s="99" t="s">
+        <v>115</v>
+      </c>
+      <c r="M8" s="99" t="s">
+        <v>114</v>
+      </c>
+      <c r="N8" s="99" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="99" t="s">
+        <v>112</v>
+      </c>
+      <c r="P8" s="99" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q8" s="99" t="s">
+        <v>110</v>
+      </c>
+      <c r="R8" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="S8" s="99" t="s">
+        <v>108</v>
+      </c>
+      <c r="T8" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="U8" s="99" t="s">
+        <v>106</v>
+      </c>
+      <c r="V8" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="W8" s="99" t="s">
+        <v>104</v>
+      </c>
+      <c r="X8" s="99" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y8" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z8" s="99" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA8" s="99" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK8" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL8" s="22">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="99">
+        <v>1</v>
+      </c>
+      <c r="B9" s="109" t="str">
+        <f>LEFT(Full!AA11,(FIND(";",Full!AA11,1)-1))</f>
+        <v>NC</v>
+      </c>
+      <c r="C9" s="104" t="str">
+        <f>LEFT(Full!Z11,(FIND(";",Full!Z11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D9" s="105" t="str">
+        <f>LEFT(Full!Y11,(FIND(";",Full!Y11,1)-1))</f>
+        <v>ANT_1_N</v>
+      </c>
+      <c r="E9" s="105" t="str">
+        <f>LEFT(Full!X11,(FIND(";",Full!X11,1)-1))</f>
+        <v>ANT_1_P</v>
+      </c>
+      <c r="F9" s="104" t="str">
+        <f>LEFT(Full!W11,(FIND(";",Full!W11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G9" s="104" t="str">
+        <f>LEFT(Full!V11,(FIND(";",Full!V11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H9" s="47" t="str">
+        <f>LEFT(Full!U11,(FIND(";",Full!U11,1)-1))</f>
+        <v>IREF_ANALOG</v>
+      </c>
+      <c r="I9" s="104" t="str">
+        <f>LEFT(Full!T11,(FIND(";",Full!T11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J9" s="104" t="str">
+        <f>LEFT(Full!S11,(FIND(";",Full!S11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K9" s="131" t="str">
+        <f>LEFT(Full!R11,(FIND(";",Full!R11,1)-1))</f>
+        <v>LINK_BM_RX_0_N</v>
+      </c>
+      <c r="L9" s="131" t="str">
+        <f>LEFT(Full!Q11,(FIND(";",Full!Q11,1)-1))</f>
+        <v>LINK_BM_RX_0_P</v>
+      </c>
+      <c r="M9" s="104" t="str">
+        <f>LEFT(Full!P11,(FIND(";",Full!P11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N9" s="101" t="str">
+        <f>LEFT(Full!O11,(FIND(";",Full!O11,1)-1))</f>
+        <v>LINK_BM_TX_0_N</v>
+      </c>
+      <c r="O9" s="101" t="str">
+        <f>LEFT(Full!N11,(FIND(";",Full!N11,1)-1))</f>
+        <v>LINK_BM_TX_0_P</v>
+      </c>
+      <c r="P9" s="104" t="str">
+        <f>LEFT(Full!M11,(FIND(";",Full!M11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q9" s="100" t="str">
+        <f>LEFT(Full!L11,(FIND(";",Full!L11,1)-1))</f>
+        <v>SERDES_SUPPLY_PROBE_0</v>
+      </c>
+      <c r="R9" s="104" t="str">
+        <f>LEFT(Full!K11,(FIND(";",Full!K11,1)-1))</f>
+        <v>RESET</v>
+      </c>
+      <c r="S9" s="104" t="str">
+        <f>LEFT(Full!J11,(FIND(";",Full!J11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T9" s="108" t="str">
+        <f>LEFT(Full!I11,(FIND(";",Full!I11,1)-1))</f>
+        <v>LO_OVERRIDE_N</v>
+      </c>
+      <c r="U9" s="108" t="str">
+        <f>LEFT(Full!H11,(FIND(";",Full!H11,1)-1))</f>
+        <v>LO_OVERRIDE_P</v>
+      </c>
+      <c r="V9" s="124" t="str">
+        <f>LEFT(Full!G11,(FIND(";",Full!G11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W9" s="104" t="str">
+        <f>LEFT(Full!F11,(FIND(";",Full!F11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X9" s="105" t="str">
+        <f>LEFT(Full!E11,(FIND(";",Full!E11,1)-1))</f>
+        <v>ANT_0_N</v>
+      </c>
+      <c r="Y9" s="105" t="str">
+        <f>LEFT(Full!D11,(FIND(";",Full!D11,1)-1))</f>
+        <v>ANT_0_P</v>
+      </c>
+      <c r="Z9" s="104" t="str">
+        <f>LEFT(Full!C11,(FIND(";",Full!C11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA9" s="109" t="str">
+        <f>LEFT(Full!B11,(FIND(";",Full!B11,1)-1))</f>
+        <v>NC</v>
+      </c>
+      <c r="AK9" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL9" s="22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="99">
+        <v>2</v>
+      </c>
+      <c r="B10" s="104" t="str">
+        <f>LEFT(Full!AA12,(FIND(";",Full!AA12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C10" s="103" t="str">
+        <f>LEFT(Full!Z12,(FIND(";",Full!Z12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="D10" s="103" t="str">
+        <f>LEFT(Full!Y12,(FIND(";",Full!Y12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="E10" s="102" t="str">
+        <f>LEFT(Full!X12,(FIND(";",Full!X12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="F10" s="102" t="str">
+        <f>LEFT(Full!W12,(FIND(";",Full!W12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="G10" s="112" t="str">
+        <f>LEFT(Full!V12,(FIND(";",Full!V12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H10" s="112" t="str">
+        <f>LEFT(Full!U12,(FIND(";",Full!U12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I10" s="104" t="str">
+        <f>LEFT(Full!T12,(FIND(";",Full!T12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J10" s="104" t="str">
+        <f>LEFT(Full!S12,(FIND(";",Full!S12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K10" s="104" t="str">
+        <f>LEFT(Full!R12,(FIND(";",Full!R12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L10" s="104" t="str">
+        <f>LEFT(Full!Q12,(FIND(";",Full!Q12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M10" s="115" t="str">
+        <f>LEFT(Full!P12,(FIND(";",Full!P12,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="N10" s="115" t="str">
+        <f>LEFT(Full!O12,(FIND(";",Full!O12,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="O10" s="104" t="str">
+        <f>LEFT(Full!N12,(FIND(";",Full!N12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P10" s="104" t="str">
+        <f>LEFT(Full!M12,(FIND(";",Full!M12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q10" s="104" t="str">
+        <f>LEFT(Full!L12,(FIND(";",Full!L12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R10" s="104" t="str">
+        <f>LEFT(Full!K12,(FIND(";",Full!K12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S10" s="103" t="str">
+        <f>LEFT(Full!J12,(FIND(";",Full!J12,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T10" s="103" t="str">
+        <f>LEFT(Full!I12,(FIND(";",Full!I12,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U10" s="102" t="str">
+        <f>LEFT(Full!H12,(FIND(";",Full!H12,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="V10" s="102" t="str">
+        <f>LEFT(Full!G12,(FIND(";",Full!G12,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="W10" s="103" t="str">
+        <f>LEFT(Full!F12,(FIND(";",Full!F12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="X10" s="103" t="str">
+        <f>LEFT(Full!E12,(FIND(";",Full!E12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Y10" s="102" t="str">
+        <f>LEFT(Full!D12,(FIND(";",Full!D12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Z10" s="130" t="str">
+        <f>LEFT(Full!C12,(FIND(";",Full!C12,1)-1))</f>
+        <v>NC</v>
+      </c>
+      <c r="AA10" s="104" t="str">
+        <f>LEFT(Full!B12,(FIND(";",Full!B12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AK10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL10" s="22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="99">
+        <v>3</v>
+      </c>
+      <c r="B11" s="104" t="str">
+        <f>LEFT(Full!AA13,(FIND(";",Full!AA13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C11" s="103" t="str">
+        <f>LEFT(Full!Z13,(FIND(";",Full!Z13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="D11" s="103" t="str">
+        <f>LEFT(Full!Y13,(FIND(";",Full!Y13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="E11" s="102" t="str">
+        <f>LEFT(Full!X13,(FIND(";",Full!X13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="F11" s="102" t="str">
+        <f>LEFT(Full!W13,(FIND(";",Full!W13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="G11" s="112" t="str">
+        <f>LEFT(Full!V13,(FIND(";",Full!V13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H11" s="112" t="str">
+        <f>LEFT(Full!U13,(FIND(";",Full!U13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I11" s="104" t="str">
+        <f>LEFT(Full!T13,(FIND(";",Full!T13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J11" s="104" t="str">
+        <f>LEFT(Full!S13,(FIND(";",Full!S13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K11" s="104" t="str">
+        <f>LEFT(Full!R13,(FIND(";",Full!R13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L11" s="104" t="str">
+        <f>LEFT(Full!Q13,(FIND(";",Full!Q13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M11" s="115" t="str">
+        <f>LEFT(Full!P13,(FIND(";",Full!P13,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="N11" s="115" t="str">
+        <f>LEFT(Full!O13,(FIND(";",Full!O13,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="O11" s="104" t="str">
+        <f>LEFT(Full!N13,(FIND(";",Full!N13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P11" s="104" t="str">
+        <f>LEFT(Full!M13,(FIND(";",Full!M13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q11" s="104" t="str">
+        <f>LEFT(Full!L13,(FIND(";",Full!L13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R11" s="104" t="str">
+        <f>LEFT(Full!K13,(FIND(";",Full!K13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S11" s="103" t="str">
+        <f>LEFT(Full!J13,(FIND(";",Full!J13,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T11" s="103" t="str">
+        <f>LEFT(Full!I13,(FIND(";",Full!I13,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U11" s="102" t="str">
+        <f>LEFT(Full!H13,(FIND(";",Full!H13,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="V11" s="102" t="str">
+        <f>LEFT(Full!G13,(FIND(";",Full!G13,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="W11" s="103" t="str">
+        <f>LEFT(Full!F13,(FIND(";",Full!F13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="X11" s="103" t="str">
+        <f>LEFT(Full!E13,(FIND(";",Full!E13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Y11" s="102" t="str">
+        <f>LEFT(Full!D13,(FIND(";",Full!D13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Z11" s="102" t="str">
+        <f>LEFT(Full!C13,(FIND(";",Full!C13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="AA11" s="125" t="str">
+        <f>LEFT(Full!B13,(FIND(";",Full!B13,1)-1))</f>
+        <v>SCAN_IN</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="99">
+        <v>4</v>
+      </c>
+      <c r="B12" s="104" t="str">
+        <f>LEFT(Full!AA14,(FIND(";",Full!AA14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C12" s="104" t="str">
+        <f>LEFT(Full!Z14,(FIND(";",Full!Z14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D12" s="104" t="str">
+        <f>LEFT(Full!Y14,(FIND(";",Full!Y14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E12" s="112" t="str">
+        <f>LEFT(Full!X14,(FIND(";",Full!X14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F12" s="112" t="str">
+        <f>LEFT(Full!W14,(FIND(";",Full!W14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G12" s="104" t="str">
+        <f>LEFT(Full!V14,(FIND(";",Full!V14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H12" s="104" t="str">
+        <f>LEFT(Full!U14,(FIND(";",Full!U14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I12" s="112" t="str">
+        <f>LEFT(Full!T14,(FIND(";",Full!T14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J12" s="112" t="str">
+        <f>LEFT(Full!S14,(FIND(";",Full!S14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K12" s="104" t="str">
+        <f>LEFT(Full!R14,(FIND(";",Full!R14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L12" s="116" t="str">
+        <f>LEFT(Full!Q14,(FIND(";",Full!Q14,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="M12" s="116" t="str">
+        <f>LEFT(Full!P14,(FIND(";",Full!P14,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="N12" s="116" t="str">
+        <f>LEFT(Full!O14,(FIND(";",Full!O14,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="O12" s="104" t="str">
+        <f>LEFT(Full!N14,(FIND(";",Full!N14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P12" s="104" t="str">
+        <f>LEFT(Full!M14,(FIND(";",Full!M14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q12" s="112" t="str">
+        <f>LEFT(Full!L14,(FIND(";",Full!L14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R12" s="112" t="str">
+        <f>LEFT(Full!K14,(FIND(";",Full!K14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S12" s="104" t="str">
+        <f>LEFT(Full!J14,(FIND(";",Full!J14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T12" s="104" t="str">
+        <f>LEFT(Full!I14,(FIND(";",Full!I14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U12" s="112" t="str">
+        <f>LEFT(Full!H14,(FIND(";",Full!H14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V12" s="112" t="str">
+        <f>LEFT(Full!G14,(FIND(";",Full!G14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W12" s="104" t="str">
+        <f>LEFT(Full!F14,(FIND(";",Full!F14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X12" s="104" t="str">
+        <f>LEFT(Full!E14,(FIND(";",Full!E14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y12" s="112" t="str">
+        <f>LEFT(Full!D14,(FIND(";",Full!D14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Z12" s="129" t="str">
+        <f>LEFT(Full!C14,(FIND(";",Full!C14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA12" s="104" t="str">
+        <f>LEFT(Full!B14,(FIND(";",Full!B14,1)-1))</f>
+        <v>SCAN_EN</v>
+      </c>
+      <c r="AK12" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL12" s="22">
+        <f>(2*AL8+AL8*(AL10-1))</f>
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="99">
+        <v>5</v>
+      </c>
+      <c r="B13" s="104" t="str">
+        <f>LEFT(Full!AA15,(FIND(";",Full!AA15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C13" s="104" t="str">
+        <f>LEFT(Full!Z15,(FIND(";",Full!Z15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D13" s="104" t="str">
+        <f>LEFT(Full!Y15,(FIND(";",Full!Y15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E13" s="112" t="str">
+        <f>LEFT(Full!X15,(FIND(";",Full!X15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F13" s="112" t="str">
+        <f>LEFT(Full!W15,(FIND(";",Full!W15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G13" s="104" t="str">
+        <f>LEFT(Full!V15,(FIND(";",Full!V15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H13" s="104" t="str">
+        <f>LEFT(Full!U15,(FIND(";",Full!U15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I13" s="112" t="str">
+        <f>LEFT(Full!T15,(FIND(";",Full!T15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J13" s="112" t="str">
+        <f>LEFT(Full!S15,(FIND(";",Full!S15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K13" s="104" t="str">
+        <f>LEFT(Full!R15,(FIND(";",Full!R15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L13" s="104" t="str">
+        <f>LEFT(Full!Q15,(FIND(";",Full!Q15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M13" s="115" t="str">
+        <f>LEFT(Full!P15,(FIND(";",Full!P15,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="N13" s="126" t="str">
+        <f>LEFT(Full!O15,(FIND(";",Full!O15,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="O13" s="104" t="str">
+        <f>LEFT(Full!N15,(FIND(";",Full!N15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P13" s="104" t="str">
+        <f>LEFT(Full!M15,(FIND(";",Full!M15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q13" s="112" t="str">
+        <f>LEFT(Full!L15,(FIND(";",Full!L15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R13" s="112" t="str">
+        <f>LEFT(Full!K15,(FIND(";",Full!K15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S13" s="104" t="str">
+        <f>LEFT(Full!J15,(FIND(";",Full!J15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T13" s="104" t="str">
+        <f>LEFT(Full!I15,(FIND(";",Full!I15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U13" s="112" t="str">
+        <f>LEFT(Full!H15,(FIND(";",Full!H15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V13" s="112" t="str">
+        <f>LEFT(Full!G15,(FIND(";",Full!G15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W13" s="104" t="str">
+        <f>LEFT(Full!F15,(FIND(";",Full!F15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X13" s="104" t="str">
+        <f>LEFT(Full!E15,(FIND(";",Full!E15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y13" s="112" t="str">
+        <f>LEFT(Full!D15,(FIND(";",Full!D15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Z13" s="129" t="str">
+        <f>LEFT(Full!C15,(FIND(";",Full!C15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA13" s="104" t="str">
+        <f>LEFT(Full!B15,(FIND(";",Full!B15,1)-1))</f>
+        <v>SCAN_CLK</v>
+      </c>
+      <c r="AK13" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL13" s="22">
+        <f>(2*AL8+AL8*(AL9-1))</f>
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="99">
+        <v>6</v>
+      </c>
+      <c r="B14" s="104" t="str">
+        <f>LEFT(Full!AA16,(FIND(";",Full!AA16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C14" s="104" t="str">
+        <f>LEFT(Full!Z16,(FIND(";",Full!Z16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D14" s="104" t="str">
+        <f>LEFT(Full!Y16,(FIND(";",Full!Y16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E14" s="104" t="str">
+        <f>LEFT(Full!X16,(FIND(";",Full!X16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F14" s="104" t="str">
+        <f>LEFT(Full!W16,(FIND(";",Full!W16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G14" s="112" t="str">
+        <f>LEFT(Full!V16,(FIND(";",Full!V16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H14" s="112" t="str">
+        <f>LEFT(Full!U16,(FIND(";",Full!U16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I14" s="104" t="str">
+        <f>LEFT(Full!T16,(FIND(";",Full!T16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J14" s="104" t="str">
+        <f>LEFT(Full!S16,(FIND(";",Full!S16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K14" s="104" t="str">
+        <f>LEFT(Full!R16,(FIND(";",Full!R16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L14" s="104" t="str">
+        <f>LEFT(Full!Q16,(FIND(";",Full!Q16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M14" s="115" t="str">
+        <f>LEFT(Full!P16,(FIND(";",Full!P16,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="N14" s="115" t="str">
+        <f>LEFT(Full!O16,(FIND(";",Full!O16,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="O14" s="121" t="str">
+        <f>LEFT(Full!N16,(FIND(";",Full!N16,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="P14" s="121" t="str">
+        <f>LEFT(Full!M16,(FIND(";",Full!M16,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Q14" s="121" t="str">
+        <f>LEFT(Full!L16,(FIND(";",Full!L16,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R14" s="121" t="str">
+        <f>LEFT(Full!K16,(FIND(";",Full!K16,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S14" s="112" t="str">
+        <f>LEFT(Full!J16,(FIND(";",Full!J16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T14" s="112" t="str">
+        <f>LEFT(Full!I16,(FIND(";",Full!I16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U14" s="104" t="str">
+        <f>LEFT(Full!H16,(FIND(";",Full!H16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V14" s="104" t="str">
+        <f>LEFT(Full!G16,(FIND(";",Full!G16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W14" s="112" t="str">
+        <f>LEFT(Full!F16,(FIND(";",Full!F16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X14" s="112" t="str">
+        <f>LEFT(Full!E16,(FIND(";",Full!E16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y14" s="104" t="str">
+        <f>LEFT(Full!D16,(FIND(";",Full!D16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Z14" s="117" t="str">
+        <f>LEFT(Full!C16,(FIND(";",Full!C16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA14" s="104" t="str">
+        <f>LEFT(Full!B16,(FIND(";",Full!B16,1)-1))</f>
+        <v>SCAN_OUT</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="99">
+        <v>7</v>
+      </c>
+      <c r="B15" s="125" t="str">
+        <f>LEFT(Full!AA17,(FIND(";",Full!AA17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C15" s="132" t="str">
+        <f>LEFT(Full!Z17,(FIND(";",Full!Z17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D15" s="133" t="str">
+        <f>LEFT(Full!Y17,(FIND(";",Full!Y17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E15" s="127" t="str">
+        <f>LEFT(Full!X17,(FIND(";",Full!X17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F15" s="125" t="str">
+        <f>LEFT(Full!W17,(FIND(";",Full!W17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G15" s="128" t="str">
+        <f>LEFT(Full!V17,(FIND(";",Full!V17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H15" s="128" t="str">
+        <f>LEFT(Full!U17,(FIND(";",Full!U17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I15" s="124" t="str">
+        <f>LEFT(Full!T17,(FIND(";",Full!T17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J15" s="124" t="str">
+        <f>LEFT(Full!S17,(FIND(";",Full!S17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K15" s="124" t="str">
+        <f>LEFT(Full!R17,(FIND(";",Full!R17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L15" s="116" t="str">
+        <f>LEFT(Full!Q17,(FIND(";",Full!Q17,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="M15" s="116" t="str">
+        <f>LEFT(Full!P17,(FIND(";",Full!P17,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="N15" s="116" t="str">
+        <f>LEFT(Full!O17,(FIND(";",Full!O17,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="O15" s="102" t="str">
+        <f>LEFT(Full!N17,(FIND(";",Full!N17,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="P15" s="102" t="str">
+        <f>LEFT(Full!M17,(FIND(";",Full!M17,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Q15" s="102" t="str">
+        <f>LEFT(Full!L17,(FIND(";",Full!L17,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R15" s="102" t="str">
+        <f>LEFT(Full!K17,(FIND(";",Full!K17,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S15" s="112" t="str">
+        <f>LEFT(Full!J17,(FIND(";",Full!J17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T15" s="112" t="str">
+        <f>LEFT(Full!I17,(FIND(";",Full!I17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U15" s="104" t="str">
+        <f>LEFT(Full!H17,(FIND(";",Full!H17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V15" s="104" t="str">
+        <f>LEFT(Full!G17,(FIND(";",Full!G17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W15" s="112" t="str">
+        <f>LEFT(Full!F17,(FIND(";",Full!F17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X15" s="112" t="str">
+        <f>LEFT(Full!E17,(FIND(";",Full!E17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y15" s="104" t="str">
+        <f>LEFT(Full!D17,(FIND(";",Full!D17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Z15" s="104" t="str">
+        <f>LEFT(Full!C17,(FIND(";",Full!C17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA15" s="104" t="str">
+        <f>LEFT(Full!B17,(FIND(";",Full!B17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="99">
+        <v>8</v>
+      </c>
+      <c r="B16" s="101" t="str">
+        <f>LEFT(Full!AA18,(FIND(";",Full!AA18,1)-1))</f>
+        <v>LINK_BM_TX_1_P</v>
+      </c>
+      <c r="C16" s="115" t="str">
+        <f>LEFT(Full!Z18,(FIND(";",Full!Z18,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="D16" s="126" t="str">
+        <f>LEFT(Full!Y18,(FIND(";",Full!Y18,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="E16" s="104" t="str">
+        <f>LEFT(Full!X18,(FIND(";",Full!X18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F16" s="104" t="str">
+        <f>LEFT(Full!W18,(FIND(";",Full!W18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G16" s="104" t="str">
+        <f>LEFT(Full!V18,(FIND(";",Full!V18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H16" s="104" t="str">
+        <f>LEFT(Full!U18,(FIND(";",Full!U18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I16" s="103" t="str">
+        <f>LEFT(Full!T18,(FIND(";",Full!T18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J16" s="103" t="str">
+        <f>LEFT(Full!S18,(FIND(";",Full!S18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K16" s="102" t="str">
+        <f>LEFT(Full!R18,(FIND(";",Full!R18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="L16" s="102" t="str">
+        <f>LEFT(Full!Q18,(FIND(";",Full!Q18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="M16" s="112" t="str">
+        <f>LEFT(Full!P18,(FIND(";",Full!P18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N16" s="112" t="str">
+        <f>LEFT(Full!O18,(FIND(";",Full!O18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O16" s="104" t="str">
+        <f>LEFT(Full!N18,(FIND(";",Full!N18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P16" s="104" t="str">
+        <f>LEFT(Full!M18,(FIND(";",Full!M18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q16" s="103" t="str">
+        <f>LEFT(Full!L18,(FIND(";",Full!L18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R16" s="103" t="str">
+        <f>LEFT(Full!K18,(FIND(";",Full!K18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S16" s="121" t="str">
+        <f>LEFT(Full!J18,(FIND(";",Full!J18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T16" s="102" t="str">
+        <f>LEFT(Full!I18,(FIND(";",Full!I18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U16" s="112" t="str">
+        <f>LEFT(Full!H18,(FIND(";",Full!H18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V16" s="112" t="str">
+        <f>LEFT(Full!G18,(FIND(";",Full!G18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W16" s="104" t="str">
+        <f>LEFT(Full!F18,(FIND(";",Full!F18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X16" s="104" t="str">
+        <f>LEFT(Full!E18,(FIND(";",Full!E18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y16" s="115" t="str">
+        <f>LEFT(Full!D18,(FIND(";",Full!D18,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="Z16" s="115" t="str">
+        <f>LEFT(Full!C18,(FIND(";",Full!C18,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="AA16" s="101" t="str">
+        <f>LEFT(Full!B18,(FIND(";",Full!B18,1)-1))</f>
+        <v>LINK_BM_RX_3_P</v>
+      </c>
+      <c r="AK16" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL16" s="22">
+        <f t="shared" ref="AL16:AL21" si="0">COUNTIF($B$9:$AC$34, AK16)</f>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="99">
+        <v>9</v>
+      </c>
+      <c r="B17" s="101" t="str">
+        <f>LEFT(Full!AA19,(FIND(";",Full!AA19,1)-1))</f>
+        <v>LINK_BM_TX_1_N</v>
+      </c>
+      <c r="C17" s="115" t="str">
+        <f>LEFT(Full!Z19,(FIND(";",Full!Z19,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="D17" s="126" t="str">
+        <f>LEFT(Full!Y19,(FIND(";",Full!Y19,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="E17" s="104" t="str">
+        <f>LEFT(Full!X19,(FIND(";",Full!X19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F17" s="104" t="str">
+        <f>LEFT(Full!W19,(FIND(";",Full!W19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G17" s="104" t="str">
+        <f>LEFT(Full!V19,(FIND(";",Full!V19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H17" s="104" t="str">
+        <f>LEFT(Full!U19,(FIND(";",Full!U19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I17" s="103" t="str">
+        <f>LEFT(Full!T19,(FIND(";",Full!T19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J17" s="103" t="str">
+        <f>LEFT(Full!S19,(FIND(";",Full!S19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K17" s="102" t="str">
+        <f>LEFT(Full!R19,(FIND(";",Full!R19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="L17" s="102" t="str">
+        <f>LEFT(Full!Q19,(FIND(";",Full!Q19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="M17" s="112" t="str">
+        <f>LEFT(Full!P19,(FIND(";",Full!P19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N17" s="112" t="str">
+        <f>LEFT(Full!O19,(FIND(";",Full!O19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O17" s="104" t="str">
+        <f>LEFT(Full!N19,(FIND(";",Full!N19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P17" s="104" t="str">
+        <f>LEFT(Full!M19,(FIND(";",Full!M19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q17" s="103" t="str">
+        <f>LEFT(Full!L19,(FIND(";",Full!L19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R17" s="103" t="str">
+        <f>LEFT(Full!K19,(FIND(";",Full!K19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S17" s="102" t="str">
+        <f>LEFT(Full!J19,(FIND(";",Full!J19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T17" s="102" t="str">
+        <f>LEFT(Full!I19,(FIND(";",Full!I19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U17" s="112" t="str">
+        <f>LEFT(Full!H19,(FIND(";",Full!H19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V17" s="112" t="str">
+        <f>LEFT(Full!G19,(FIND(";",Full!G19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W17" s="104" t="str">
+        <f>LEFT(Full!F19,(FIND(";",Full!F19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X17" s="104" t="str">
+        <f>LEFT(Full!E19,(FIND(";",Full!E19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y17" s="115" t="str">
+        <f>LEFT(Full!D19,(FIND(";",Full!D19,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="Z17" s="115" t="str">
+        <f>LEFT(Full!C19,(FIND(";",Full!C19,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="AA17" s="101" t="str">
+        <f>LEFT(Full!B19,(FIND(";",Full!B19,1)-1))</f>
+        <v>LINK_BM_RX_3_N</v>
+      </c>
+      <c r="AK17" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL17" s="22">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="99">
+        <v>10</v>
+      </c>
+      <c r="B18" s="104" t="str">
+        <f>LEFT(Full!AA20,(FIND(";",Full!AA20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C18" s="116" t="str">
+        <f>LEFT(Full!Z20,(FIND(";",Full!Z20,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="D18" s="116" t="str">
+        <f>LEFT(Full!Y20,(FIND(";",Full!Y20,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="E18" s="116" t="str">
+        <f>LEFT(Full!X20,(FIND(";",Full!X20,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="F18" s="104" t="str">
+        <f>LEFT(Full!W20,(FIND(";",Full!W20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G18" s="112" t="str">
+        <f>LEFT(Full!V20,(FIND(";",Full!V20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H18" s="112" t="str">
+        <f>LEFT(Full!U20,(FIND(";",Full!U20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I18" s="104" t="str">
+        <f>LEFT(Full!T20,(FIND(";",Full!T20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J18" s="104" t="str">
+        <f>LEFT(Full!S20,(FIND(";",Full!S20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K18" s="103" t="str">
+        <f>LEFT(Full!R20,(FIND(";",Full!R20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L18" s="103" t="str">
+        <f>LEFT(Full!Q20,(FIND(";",Full!Q20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M18" s="102" t="str">
+        <f>LEFT(Full!P20,(FIND(";",Full!P20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N18" s="102" t="str">
+        <f>LEFT(Full!O20,(FIND(";",Full!O20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O18" s="103" t="str">
+        <f>LEFT(Full!N20,(FIND(";",Full!N20,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="P18" s="103" t="str">
+        <f>LEFT(Full!M20,(FIND(";",Full!M20,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="Q18" s="102" t="str">
+        <f>LEFT(Full!L20,(FIND(";",Full!L20,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="R18" s="102" t="str">
+        <f>LEFT(Full!K20,(FIND(";",Full!K20,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="S18" s="112" t="str">
+        <f>LEFT(Full!J20,(FIND(";",Full!J20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T18" s="112" t="str">
+        <f>LEFT(Full!I20,(FIND(";",Full!I20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U18" s="104" t="str">
+        <f>LEFT(Full!H20,(FIND(";",Full!H20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V18" s="104" t="str">
+        <f>LEFT(Full!G20,(FIND(";",Full!G20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W18" s="104" t="str">
+        <f>LEFT(Full!F20,(FIND(";",Full!F20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X18" s="57" t="str">
+        <f>LEFT(Full!E20,(FIND(";",Full!E20,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Y18" s="57" t="str">
+        <f>LEFT(Full!D20,(FIND(";",Full!D20,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Z18" s="57" t="str">
+        <f>LEFT(Full!C20,(FIND(";",Full!C20,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="AA18" s="104" t="str">
+        <f>LEFT(Full!B20,(FIND(";",Full!B20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AK18" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL18" s="22">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="99">
+        <v>11</v>
+      </c>
+      <c r="B19" s="101" t="str">
+        <f>LEFT(Full!AA21,(FIND(";",Full!AA21,1)-1))</f>
+        <v>LINK_BM_RX_1_P</v>
+      </c>
+      <c r="C19" s="115" t="str">
+        <f>LEFT(Full!Z21,(FIND(";",Full!Z21,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="D19" s="115" t="str">
+        <f>LEFT(Full!Y21,(FIND(";",Full!Y21,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="E19" s="125" t="str">
+        <f>LEFT(Full!X21,(FIND(";",Full!X21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F19" s="104" t="str">
+        <f>LEFT(Full!W21,(FIND(";",Full!W21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G19" s="112" t="str">
+        <f>LEFT(Full!V21,(FIND(";",Full!V21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H19" s="112" t="str">
+        <f>LEFT(Full!U21,(FIND(";",Full!U21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I19" s="104" t="str">
+        <f>LEFT(Full!T21,(FIND(";",Full!T21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J19" s="104" t="str">
+        <f>LEFT(Full!S21,(FIND(";",Full!S21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K19" s="103" t="str">
+        <f>LEFT(Full!R21,(FIND(";",Full!R21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L19" s="103" t="str">
+        <f>LEFT(Full!Q21,(FIND(";",Full!Q21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M19" s="104" t="str">
+        <f>LEFT(Full!P21,(FIND(";",Full!P21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N19" s="104" t="str">
+        <f>LEFT(Full!O21,(FIND(";",Full!O21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O19" s="103" t="str">
+        <f>LEFT(Full!N21,(FIND(";",Full!N21,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="P19" s="103" t="str">
+        <f>LEFT(Full!M21,(FIND(";",Full!M21,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="Q19" s="102" t="str">
+        <f>LEFT(Full!L21,(FIND(";",Full!L21,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="R19" s="102" t="str">
+        <f>LEFT(Full!K21,(FIND(";",Full!K21,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="S19" s="112" t="str">
+        <f>LEFT(Full!J21,(FIND(";",Full!J21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T19" s="112" t="str">
+        <f>LEFT(Full!I21,(FIND(";",Full!I21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U19" s="104" t="str">
+        <f>LEFT(Full!H21,(FIND(";",Full!H21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V19" s="104" t="str">
+        <f>LEFT(Full!G21,(FIND(";",Full!G21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W19" s="104" t="str">
+        <f>LEFT(Full!F21,(FIND(";",Full!F21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X19" s="104" t="str">
+        <f>LEFT(Full!E21,(FIND(";",Full!E21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y19" s="115" t="str">
+        <f>LEFT(Full!D21,(FIND(";",Full!D21,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="Z19" s="115" t="str">
+        <f>LEFT(Full!C21,(FIND(";",Full!C21,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="AA19" s="101" t="str">
+        <f>LEFT(Full!B21,(FIND(";",Full!B21,1)-1))</f>
+        <v>LINK_BM_TX_3_P</v>
+      </c>
+      <c r="AK19" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL19" s="22">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="99">
+        <v>12</v>
+      </c>
+      <c r="B20" s="101" t="str">
+        <f>LEFT(Full!AA22,(FIND(";",Full!AA22,1)-1))</f>
+        <v>LINK_BM_RX_1_N</v>
+      </c>
+      <c r="C20" s="115" t="str">
+        <f>LEFT(Full!Z22,(FIND(";",Full!Z22,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="D20" s="115" t="str">
+        <f>LEFT(Full!Y22,(FIND(";",Full!Y22,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="E20" s="124" t="str">
+        <f>LEFT(Full!X22,(FIND(";",Full!X22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F20" s="104" t="str">
+        <f>LEFT(Full!W22,(FIND(";",Full!W22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G20" s="121" t="str">
+        <f>LEFT(Full!V22,(FIND(";",Full!V22,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="H20" s="121" t="str">
+        <f>LEFT(Full!U22,(FIND(";",Full!U22,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="I20" s="120" t="str">
+        <f>LEFT(Full!T22,(FIND(";",Full!T22,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J20" s="103" t="str">
+        <f>LEFT(Full!S22,(FIND(";",Full!S22,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K20" s="104" t="str">
+        <f>LEFT(Full!R22,(FIND(";",Full!R22,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="L20" s="102" t="str">
+        <f>LEFT(Full!Q22,(FIND(";",Full!Q22,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="M20" s="112" t="str">
+        <f>LEFT(Full!P22,(FIND(";",Full!P22,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="N20" s="103" t="str">
+        <f>LEFT(Full!O22,(FIND(";",Full!O22,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="O20" s="104" t="str">
+        <f>LEFT(Full!N22,(FIND(";",Full!N22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P20" s="104" t="str">
+        <f>LEFT(Full!M22,(FIND(";",Full!M22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q20" s="112" t="str">
+        <f>LEFT(Full!L22,(FIND(";",Full!L22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R20" s="112" t="str">
+        <f>LEFT(Full!K22,(FIND(";",Full!K22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S20" s="104" t="str">
+        <f>LEFT(Full!J22,(FIND(";",Full!J22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T20" s="104" t="str">
+        <f>LEFT(Full!I22,(FIND(";",Full!I22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U20" s="112" t="str">
+        <f>LEFT(Full!H22,(FIND(";",Full!H22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V20" s="112" t="str">
+        <f>LEFT(Full!G22,(FIND(";",Full!G22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W20" s="104" t="str">
+        <f>LEFT(Full!F22,(FIND(";",Full!F22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X20" s="104" t="str">
+        <f>LEFT(Full!E22,(FIND(";",Full!E22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y20" s="115" t="str">
+        <f>LEFT(Full!D22,(FIND(";",Full!D22,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="Z20" s="115" t="str">
+        <f>LEFT(Full!C22,(FIND(";",Full!C22,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="AA20" s="101" t="str">
+        <f>LEFT(Full!B22,(FIND(";",Full!B22,1)-1))</f>
+        <v>LINK_BM_TX_3_N</v>
+      </c>
+      <c r="AK20" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL20" s="22">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="99">
+        <v>13</v>
+      </c>
+      <c r="B21" s="104" t="str">
+        <f>LEFT(Full!AA23,(FIND(";",Full!AA23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C21" s="116" t="str">
+        <f>LEFT(Full!Z23,(FIND(";",Full!Z23,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="D21" s="116" t="str">
+        <f>LEFT(Full!Y23,(FIND(";",Full!Y23,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="E21" s="116" t="str">
+        <f>LEFT(Full!X23,(FIND(";",Full!X23,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="F21" s="104" t="str">
+        <f>LEFT(Full!W23,(FIND(";",Full!W23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G21" s="102" t="str">
+        <f>LEFT(Full!V23,(FIND(";",Full!V23,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="H21" s="102" t="str">
+        <f>LEFT(Full!U23,(FIND(";",Full!U23,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="I21" s="103" t="str">
+        <f>LEFT(Full!T23,(FIND(";",Full!T23,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J21" s="103" t="str">
+        <f>LEFT(Full!S23,(FIND(";",Full!S23,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K21" s="104" t="str">
+        <f>LEFT(Full!R23,(FIND(";",Full!R23,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="L21" s="102" t="str">
+        <f>LEFT(Full!Q23,(FIND(";",Full!Q23,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="M21" s="103" t="str">
+        <f>LEFT(Full!P23,(FIND(";",Full!P23,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="N21" s="103" t="str">
+        <f>LEFT(Full!O23,(FIND(";",Full!O23,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="O21" s="104" t="str">
+        <f>LEFT(Full!N23,(FIND(";",Full!N23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P21" s="104" t="str">
+        <f>LEFT(Full!M23,(FIND(";",Full!M23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q21" s="112" t="str">
+        <f>LEFT(Full!L23,(FIND(";",Full!L23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R21" s="112" t="str">
+        <f>LEFT(Full!K23,(FIND(";",Full!K23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S21" s="104" t="str">
+        <f>LEFT(Full!J23,(FIND(";",Full!J23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T21" s="104" t="str">
+        <f>LEFT(Full!I23,(FIND(";",Full!I23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U21" s="112" t="str">
+        <f>LEFT(Full!H23,(FIND(";",Full!H23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V21" s="112" t="str">
+        <f>LEFT(Full!G23,(FIND(";",Full!G23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W21" s="104" t="str">
+        <f>LEFT(Full!F23,(FIND(";",Full!F23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X21" s="116" t="str">
+        <f>LEFT(Full!E23,(FIND(";",Full!E23,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Y21" s="116" t="str">
+        <f>LEFT(Full!D23,(FIND(";",Full!D23,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Z21" s="116" t="str">
+        <f>LEFT(Full!C23,(FIND(";",Full!C23,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="AA21" s="104" t="str">
+        <f>LEFT(Full!B23,(FIND(";",Full!B23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AK21" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL21" s="22">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="99">
+        <v>14</v>
+      </c>
+      <c r="B22" s="101" t="str">
+        <f>LEFT(Full!AA24,(FIND(";",Full!AA24,1)-1))</f>
+        <v>LINK_CM_TX_0_P</v>
+      </c>
+      <c r="C22" s="115" t="str">
+        <f>LEFT(Full!Z24,(FIND(";",Full!Z24,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="D22" s="115" t="str">
+        <f>LEFT(Full!Y24,(FIND(";",Full!Y24,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="E22" s="125" t="str">
+        <f>LEFT(Full!X24,(FIND(";",Full!X24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F22" s="104" t="str">
+        <f>LEFT(Full!W24,(FIND(";",Full!W24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G22" s="112" t="str">
+        <f>LEFT(Full!V24,(FIND(";",Full!V24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H22" s="112" t="str">
+        <f>LEFT(Full!U24,(FIND(";",Full!U24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I22" s="104" t="str">
+        <f>LEFT(Full!T24,(FIND(";",Full!T24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J22" s="104" t="str">
+        <f>LEFT(Full!S24,(FIND(";",Full!S24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K22" s="103" t="str">
+        <f>LEFT(Full!R24,(FIND(";",Full!R24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="L22" s="103" t="str">
+        <f>LEFT(Full!Q24,(FIND(";",Full!Q24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="M22" s="102" t="str">
+        <f>LEFT(Full!P24,(FIND(";",Full!P24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="N22" s="102" t="str">
+        <f>LEFT(Full!O24,(FIND(";",Full!O24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="O22" s="112" t="str">
+        <f>LEFT(Full!N24,(FIND(";",Full!N24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="P22" s="103" t="str">
+        <f>LEFT(Full!M24,(FIND(";",Full!M24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="Q22" s="102" t="str">
+        <f>LEFT(Full!L24,(FIND(";",Full!L24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="R22" s="102" t="str">
+        <f>LEFT(Full!K24,(FIND(";",Full!K24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="S22" s="123" t="str">
+        <f>LEFT(Full!J24,(FIND(";",Full!J24,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T22" s="123" t="str">
+        <f>LEFT(Full!I24,(FIND(";",Full!I24,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U22" s="102" t="str">
+        <f>LEFT(Full!H24,(FIND(";",Full!H24,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="V22" s="102" t="str">
+        <f>LEFT(Full!G24,(FIND(";",Full!G24,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="W22" s="104" t="str">
+        <f>LEFT(Full!F24,(FIND(";",Full!F24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X22" s="104" t="str">
+        <f>LEFT(Full!E24,(FIND(";",Full!E24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y22" s="50" t="str">
+        <f>LEFT(Full!D24,(FIND(";",Full!D24,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="Z22" s="49" t="str">
+        <f>LEFT(Full!C24,(FIND(";",Full!C24,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="AA22" s="105" t="str">
+        <f>LEFT(Full!B24,(FIND(";",Full!B24,1)-1))</f>
+        <v>LINK_CM_RX_1_P</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="99">
+        <v>15</v>
+      </c>
+      <c r="B23" s="101" t="str">
+        <f>LEFT(Full!AA25,(FIND(";",Full!AA25,1)-1))</f>
+        <v>LINK_CM_TX_0_N</v>
+      </c>
+      <c r="C23" s="115" t="str">
+        <f>LEFT(Full!Z25,(FIND(";",Full!Z25,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="D23" s="115" t="str">
+        <f>LEFT(Full!Y25,(FIND(";",Full!Y25,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="E23" s="104" t="str">
+        <f>LEFT(Full!X25,(FIND(";",Full!X25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F23" s="104" t="str">
+        <f>LEFT(Full!W25,(FIND(";",Full!W25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G23" s="112" t="str">
+        <f>LEFT(Full!V25,(FIND(";",Full!V25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H23" s="112" t="str">
+        <f>LEFT(Full!U25,(FIND(";",Full!U25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I23" s="104" t="str">
+        <f>LEFT(Full!T25,(FIND(";",Full!T25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J23" s="104" t="str">
+        <f>LEFT(Full!S25,(FIND(";",Full!S25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K23" s="103" t="str">
+        <f>LEFT(Full!R25,(FIND(";",Full!R25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="L23" s="103" t="str">
+        <f>LEFT(Full!Q25,(FIND(";",Full!Q25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="M23" s="102" t="str">
+        <f>LEFT(Full!P25,(FIND(";",Full!P25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="N23" s="102" t="str">
+        <f>LEFT(Full!O25,(FIND(";",Full!O25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="O23" s="103" t="str">
+        <f>LEFT(Full!N25,(FIND(";",Full!N25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="P23" s="103" t="str">
+        <f>LEFT(Full!M25,(FIND(";",Full!M25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="Q23" s="102" t="str">
+        <f>LEFT(Full!L25,(FIND(";",Full!L25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="R23" s="102" t="str">
+        <f>LEFT(Full!K25,(FIND(";",Full!K25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="S23" s="123" t="str">
+        <f>LEFT(Full!J25,(FIND(";",Full!J25,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T23" s="123" t="str">
+        <f>LEFT(Full!I25,(FIND(";",Full!I25,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U23" s="102" t="str">
+        <f>LEFT(Full!H25,(FIND(";",Full!H25,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="V23" s="102" t="str">
+        <f>LEFT(Full!G25,(FIND(";",Full!G25,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="W23" s="104" t="str">
+        <f>LEFT(Full!F25,(FIND(";",Full!F25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X23" s="104" t="str">
+        <f>LEFT(Full!E25,(FIND(";",Full!E25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y23" s="64" t="str">
+        <f>LEFT(Full!D25,(FIND(";",Full!D25,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="Z23" s="63" t="str">
+        <f>LEFT(Full!C25,(FIND(";",Full!C25,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="AA23" s="105" t="str">
+        <f>LEFT(Full!B25,(FIND(";",Full!B25,1)-1))</f>
+        <v>LINK_CM_RX_1_N</v>
+      </c>
+      <c r="AK23" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL23" s="22">
+        <f>COUNTIF($B$9:$AC$34, AK23)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="99">
+        <v>16</v>
+      </c>
+      <c r="B24" s="104" t="str">
+        <f>LEFT(Full!AA26,(FIND(";",Full!AA26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C24" s="116" t="str">
+        <f>LEFT(Full!Z26,(FIND(";",Full!Z26,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="D24" s="116" t="str">
+        <f>LEFT(Full!Y26,(FIND(";",Full!Y26,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="E24" s="116" t="str">
+        <f>LEFT(Full!X26,(FIND(";",Full!X26,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="F24" s="104" t="str">
+        <f>LEFT(Full!W26,(FIND(";",Full!W26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G24" s="102" t="str">
+        <f>LEFT(Full!V26,(FIND(";",Full!V26,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="H24" s="102" t="str">
+        <f>LEFT(Full!U26,(FIND(";",Full!U26,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="I24" s="103" t="str">
+        <f>LEFT(Full!T26,(FIND(";",Full!T26,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J24" s="103" t="str">
+        <f>LEFT(Full!S26,(FIND(";",Full!S26,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K24" s="104" t="str">
+        <f>LEFT(Full!R26,(FIND(";",Full!R26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L24" s="104" t="str">
+        <f>LEFT(Full!Q26,(FIND(";",Full!Q26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M24" s="112" t="str">
+        <f>LEFT(Full!P26,(FIND(";",Full!P26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N24" s="112" t="str">
+        <f>LEFT(Full!O26,(FIND(";",Full!O26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O24" s="104" t="str">
+        <f>LEFT(Full!N26,(FIND(";",Full!N26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P24" s="104" t="str">
+        <f>LEFT(Full!M26,(FIND(";",Full!M26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q24" s="112" t="str">
+        <f>LEFT(Full!L26,(FIND(";",Full!L26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R24" s="112" t="str">
+        <f>LEFT(Full!K26,(FIND(";",Full!K26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S24" s="104" t="str">
+        <f>LEFT(Full!J26,(FIND(";",Full!J26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T24" s="104" t="str">
+        <f>LEFT(Full!I26,(FIND(";",Full!I26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U24" s="112" t="str">
+        <f>LEFT(Full!H26,(FIND(";",Full!H26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V24" s="112" t="str">
+        <f>LEFT(Full!G26,(FIND(";",Full!G26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W24" s="104" t="str">
+        <f>LEFT(Full!F26,(FIND(";",Full!F26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X24" s="116" t="str">
+        <f>LEFT(Full!E26,(FIND(";",Full!E26,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Y24" s="116" t="str">
+        <f>LEFT(Full!D26,(FIND(";",Full!D26,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Z24" s="116" t="str">
+        <f>LEFT(Full!C26,(FIND(";",Full!C26,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="AA24" s="104" t="str">
+        <f>LEFT(Full!B26,(FIND(";",Full!B26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AK24" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL24" s="22">
+        <f>COUNTIF($B$9:$AC$34, AK24)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="99">
+        <v>17</v>
+      </c>
+      <c r="B25" s="101" t="str">
+        <f>LEFT(Full!AA27,(FIND(";",Full!AA27,1)-1))</f>
+        <v>LINK_CM_RX_0_P</v>
+      </c>
+      <c r="C25" s="115" t="str">
+        <f>LEFT(Full!Z27,(FIND(";",Full!Z27,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="D25" s="115" t="str">
+        <f>LEFT(Full!Y27,(FIND(";",Full!Y27,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="E25" s="104" t="str">
+        <f>LEFT(Full!X27,(FIND(";",Full!X27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F25" s="117" t="str">
+        <f>LEFT(Full!W27,(FIND(";",Full!W27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G25" s="102" t="str">
+        <f>LEFT(Full!V27,(FIND(";",Full!V27,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="H25" s="102" t="str">
+        <f>LEFT(Full!U27,(FIND(";",Full!U27,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="I25" s="103" t="str">
+        <f>LEFT(Full!T27,(FIND(";",Full!T27,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J25" s="103" t="str">
+        <f>LEFT(Full!S27,(FIND(";",Full!S27,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K25" s="104" t="str">
+        <f>LEFT(Full!R27,(FIND(";",Full!R27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L25" s="104" t="str">
+        <f>LEFT(Full!Q27,(FIND(";",Full!Q27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M25" s="112" t="str">
+        <f>LEFT(Full!P27,(FIND(";",Full!P27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N25" s="112" t="str">
+        <f>LEFT(Full!O27,(FIND(";",Full!O27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O25" s="104" t="str">
+        <f>LEFT(Full!N27,(FIND(";",Full!N27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P25" s="104" t="str">
+        <f>LEFT(Full!M27,(FIND(";",Full!M27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q25" s="112" t="str">
+        <f>LEFT(Full!L27,(FIND(";",Full!L27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R25" s="112" t="str">
+        <f>LEFT(Full!K27,(FIND(";",Full!K27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S25" s="104" t="str">
+        <f>LEFT(Full!J27,(FIND(";",Full!J27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T25" s="104" t="str">
+        <f>LEFT(Full!I27,(FIND(";",Full!I27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U25" s="112" t="str">
+        <f>LEFT(Full!H27,(FIND(";",Full!H27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V25" s="112" t="str">
+        <f>LEFT(Full!G27,(FIND(";",Full!G27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W25" s="104" t="str">
+        <f>LEFT(Full!F27,(FIND(";",Full!F27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X25" s="104" t="str">
+        <f>LEFT(Full!E27,(FIND(";",Full!E27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y25" s="115" t="str">
+        <f>LEFT(Full!D27,(FIND(";",Full!D27,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="Z25" s="115" t="str">
+        <f>LEFT(Full!C27,(FIND(";",Full!C27,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="AA25" s="105" t="str">
+        <f>LEFT(Full!B27,(FIND(";",Full!B27,1)-1))</f>
+        <v>LINK_CM_TX_1_P</v>
+      </c>
+      <c r="AK25" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="AL25" s="22">
+        <f>AL9*AL10-AL23-AL24</f>
+        <v>635</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="99">
+        <v>18</v>
+      </c>
+      <c r="B26" s="101" t="str">
+        <f>LEFT(Full!AA28,(FIND(";",Full!AA28,1)-1))</f>
+        <v>LINK_CM_RX_0_N</v>
+      </c>
+      <c r="C26" s="115" t="str">
+        <f>LEFT(Full!Z28,(FIND(";",Full!Z28,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="D26" s="115" t="str">
+        <f>LEFT(Full!Y28,(FIND(";",Full!Y28,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="E26" s="104" t="str">
+        <f>LEFT(Full!X28,(FIND(";",Full!X28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F26" s="104" t="str">
+        <f>LEFT(Full!W28,(FIND(";",Full!W28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G26" s="112" t="str">
+        <f>LEFT(Full!V28,(FIND(";",Full!V28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H26" s="112" t="str">
+        <f>LEFT(Full!U28,(FIND(";",Full!U28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I26" s="104" t="str">
+        <f>LEFT(Full!T28,(FIND(";",Full!T28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J26" s="104" t="str">
+        <f>LEFT(Full!S28,(FIND(";",Full!S28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K26" s="120" t="str">
+        <f>LEFT(Full!R28,(FIND(";",Full!R28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="L26" s="120" t="str">
+        <f>LEFT(Full!Q28,(FIND(";",Full!Q28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="M26" s="121" t="str">
+        <f>LEFT(Full!P28,(FIND(";",Full!P28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="N26" s="121" t="str">
+        <f>LEFT(Full!O28,(FIND(";",Full!O28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="O26" s="120" t="str">
+        <f>LEFT(Full!N28,(FIND(";",Full!N28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="P26" s="120" t="str">
+        <f>LEFT(Full!M28,(FIND(";",Full!M28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Q26" s="121" t="str">
+        <f>LEFT(Full!L28,(FIND(";",Full!L28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R26" s="121" t="str">
+        <f>LEFT(Full!K28,(FIND(";",Full!K28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S26" s="112" t="str">
+        <f>LEFT(Full!J28,(FIND(";",Full!J28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T26" s="112" t="str">
+        <f>LEFT(Full!I28,(FIND(";",Full!I28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U26" s="104" t="str">
+        <f>LEFT(Full!H28,(FIND(";",Full!H28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V26" s="104" t="str">
+        <f>LEFT(Full!G28,(FIND(";",Full!G28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W26" s="104" t="str">
+        <f>LEFT(Full!F28,(FIND(";",Full!F28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X26" s="104" t="str">
+        <f>LEFT(Full!E28,(FIND(";",Full!E28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y26" s="115" t="str">
+        <f>LEFT(Full!D28,(FIND(";",Full!D28,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="Z26" s="115" t="str">
+        <f>LEFT(Full!C28,(FIND(";",Full!C28,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="AA26" s="105" t="str">
+        <f>LEFT(Full!B28,(FIND(";",Full!B28,1)-1))</f>
+        <v>LINK_CM_TX_1_N</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="99">
+        <v>19</v>
+      </c>
+      <c r="B27" s="104" t="str">
+        <f>LEFT(Full!AA29,(FIND(";",Full!AA29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C27" s="116" t="str">
+        <f>LEFT(Full!Z29,(FIND(";",Full!Z29,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="D27" s="116" t="str">
+        <f>LEFT(Full!Y29,(FIND(";",Full!Y29,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="E27" s="119" t="str">
+        <f>LEFT(Full!X29,(FIND(";",Full!X29,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="F27" s="104" t="str">
+        <f>LEFT(Full!W29,(FIND(";",Full!W29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G27" s="112" t="str">
+        <f>LEFT(Full!V29,(FIND(";",Full!V29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H27" s="112" t="str">
+        <f>LEFT(Full!U29,(FIND(";",Full!U29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I27" s="104" t="str">
+        <f>LEFT(Full!T29,(FIND(";",Full!T29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J27" s="104" t="str">
+        <f>LEFT(Full!S29,(FIND(";",Full!S29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K27" s="103" t="str">
+        <f>LEFT(Full!R29,(FIND(";",Full!R29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="L27" s="103" t="str">
+        <f>LEFT(Full!Q29,(FIND(";",Full!Q29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="M27" s="102" t="str">
+        <f>LEFT(Full!P29,(FIND(";",Full!P29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="N27" s="102" t="str">
+        <f>LEFT(Full!O29,(FIND(";",Full!O29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="O27" s="103" t="str">
+        <f>LEFT(Full!N29,(FIND(";",Full!N29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="P27" s="103" t="str">
+        <f>LEFT(Full!M29,(FIND(";",Full!M29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Q27" s="102" t="str">
+        <f>LEFT(Full!L29,(FIND(";",Full!L29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R27" s="102" t="str">
+        <f>LEFT(Full!K29,(FIND(";",Full!K29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S27" s="112" t="str">
+        <f>LEFT(Full!J29,(FIND(";",Full!J29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T27" s="112" t="str">
+        <f>LEFT(Full!I29,(FIND(";",Full!I29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U27" s="104" t="str">
+        <f>LEFT(Full!H29,(FIND(";",Full!H29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V27" s="104" t="str">
+        <f>LEFT(Full!G29,(FIND(";",Full!G29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W27" s="104" t="str">
+        <f>LEFT(Full!F29,(FIND(";",Full!F29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X27" s="122" t="str">
+        <f>LEFT(Full!E29,(FIND(";",Full!E29,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Y27" s="116" t="str">
+        <f>LEFT(Full!D29,(FIND(";",Full!D29,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Z27" s="116" t="str">
+        <f>LEFT(Full!C29,(FIND(";",Full!C29,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="AA27" s="104" t="str">
+        <f>LEFT(Full!B29,(FIND(";",Full!B29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="99">
+        <v>20</v>
+      </c>
+      <c r="B28" s="100" t="str">
+        <f>LEFT(Full!AA30,(FIND(";",Full!AA30,1)-1))</f>
+        <v>REF_SERDES_CM0_P</v>
+      </c>
+      <c r="C28" s="104" t="str">
+        <f>LEFT(Full!Z30,(FIND(";",Full!Z30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D28" s="104" t="str">
+        <f>LEFT(Full!Y30,(FIND(";",Full!Y30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E28" s="112" t="str">
+        <f>LEFT(Full!X30,(FIND(";",Full!X30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F28" s="112" t="str">
+        <f>LEFT(Full!W30,(FIND(";",Full!W30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G28" s="104" t="str">
+        <f>LEFT(Full!V30,(FIND(";",Full!V30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H28" s="104" t="str">
+        <f>LEFT(Full!U30,(FIND(";",Full!U30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I28" s="103" t="str">
+        <f>LEFT(Full!T30,(FIND(";",Full!T30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J28" s="103" t="str">
+        <f>LEFT(Full!S30,(FIND(";",Full!S30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K28" s="102" t="str">
+        <f>LEFT(Full!R30,(FIND(";",Full!R30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="L28" s="116" t="str">
+        <f>LEFT(Full!Q30,(FIND(";",Full!Q30,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="M28" s="116" t="str">
+        <f>LEFT(Full!P30,(FIND(";",Full!P30,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="N28" s="116" t="str">
+        <f>LEFT(Full!O30,(FIND(";",Full!O30,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="O28" s="104" t="str">
+        <f>LEFT(Full!N30,(FIND(";",Full!N30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P28" s="104" t="str">
+        <f>LEFT(Full!M30,(FIND(";",Full!M30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q28" s="103" t="str">
+        <f>LEFT(Full!L30,(FIND(";",Full!L30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R28" s="103" t="str">
+        <f>LEFT(Full!K30,(FIND(";",Full!K30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S28" s="102" t="str">
+        <f>LEFT(Full!J30,(FIND(";",Full!J30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T28" s="102" t="str">
+        <f>LEFT(Full!I30,(FIND(";",Full!I30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U28" s="112" t="str">
+        <f>LEFT(Full!H30,(FIND(";",Full!H30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V28" s="112" t="str">
+        <f>LEFT(Full!G30,(FIND(";",Full!G30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W28" s="104" t="str">
+        <f>LEFT(Full!F30,(FIND(";",Full!F30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X28" s="104" t="str">
+        <f>LEFT(Full!E30,(FIND(";",Full!E30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y28" s="112" t="str">
+        <f>LEFT(Full!D30,(FIND(";",Full!D30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Z28" s="112" t="str">
+        <f>LEFT(Full!C30,(FIND(";",Full!C30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA28" s="100" t="str">
+        <f>LEFT(Full!B30,(FIND(";",Full!B30,1)-1))</f>
+        <v>REF_SERDES_CM1_P</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="99">
+        <v>21</v>
+      </c>
+      <c r="B29" s="100" t="str">
+        <f>LEFT(Full!AA31,(FIND(";",Full!AA31,1)-1))</f>
+        <v>REF_SERDES_CM0_N</v>
+      </c>
+      <c r="C29" s="104" t="str">
+        <f>LEFT(Full!Z31,(FIND(";",Full!Z31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D29" s="104" t="str">
+        <f>LEFT(Full!Y31,(FIND(";",Full!Y31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E29" s="112" t="str">
+        <f>LEFT(Full!X31,(FIND(";",Full!X31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F29" s="112" t="str">
+        <f>LEFT(Full!W31,(FIND(";",Full!W31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G29" s="104" t="str">
+        <f>LEFT(Full!V31,(FIND(";",Full!V31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H29" s="104" t="str">
+        <f>LEFT(Full!U31,(FIND(";",Full!U31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I29" s="103" t="str">
+        <f>LEFT(Full!T31,(FIND(";",Full!T31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J29" s="103" t="str">
+        <f>LEFT(Full!S31,(FIND(";",Full!S31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K29" s="102" t="str">
+        <f>LEFT(Full!R31,(FIND(";",Full!R31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="L29" s="115" t="str">
+        <f>LEFT(Full!Q31,(FIND(";",Full!Q31,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="M29" s="115" t="str">
+        <f>LEFT(Full!P31,(FIND(";",Full!P31,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="N29" s="104" t="str">
+        <f>LEFT(Full!O31,(FIND(";",Full!O31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O29" s="104" t="str">
+        <f>LEFT(Full!N31,(FIND(";",Full!N31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P29" s="104" t="str">
+        <f>LEFT(Full!M31,(FIND(";",Full!M31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q29" s="103" t="str">
+        <f>LEFT(Full!L31,(FIND(";",Full!L31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R29" s="103" t="str">
+        <f>LEFT(Full!K31,(FIND(";",Full!K31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S29" s="102" t="str">
+        <f>LEFT(Full!J31,(FIND(";",Full!J31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T29" s="102" t="str">
+        <f>LEFT(Full!I31,(FIND(";",Full!I31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U29" s="112" t="str">
+        <f>LEFT(Full!H31,(FIND(";",Full!H31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V29" s="112" t="str">
+        <f>LEFT(Full!G31,(FIND(";",Full!G31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W29" s="104" t="str">
+        <f>LEFT(Full!F31,(FIND(";",Full!F31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X29" s="104" t="str">
+        <f>LEFT(Full!E31,(FIND(";",Full!E31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y29" s="112" t="str">
+        <f>LEFT(Full!D31,(FIND(";",Full!D31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Z29" s="112" t="str">
+        <f>LEFT(Full!C31,(FIND(";",Full!C31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA29" s="100" t="str">
+        <f>LEFT(Full!B31,(FIND(";",Full!B31,1)-1))</f>
+        <v>REF_SERDES_CM1_N</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="99">
+        <v>22</v>
+      </c>
+      <c r="B30" s="104" t="str">
+        <f>LEFT(Full!AA32,(FIND(";",Full!AA32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C30" s="112" t="str">
+        <f>LEFT(Full!Z32,(FIND(";",Full!Z32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D30" s="112" t="str">
+        <f>LEFT(Full!Y32,(FIND(";",Full!Y32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E30" s="104" t="str">
+        <f>LEFT(Full!X32,(FIND(";",Full!X32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F30" s="104" t="str">
+        <f>LEFT(Full!W32,(FIND(";",Full!W32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G30" s="112" t="str">
+        <f>LEFT(Full!V32,(FIND(";",Full!V32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H30" s="112" t="str">
+        <f>LEFT(Full!U32,(FIND(";",Full!U32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I30" s="113" t="str">
+        <f>LEFT(Full!T32,(FIND(";",Full!T32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J30" s="104" t="str">
+        <f>LEFT(Full!S32,(FIND(";",Full!S32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K30" s="104" t="str">
+        <f>LEFT(Full!R32,(FIND(";",Full!R32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L30" s="115" t="str">
+        <f>LEFT(Full!Q32,(FIND(";",Full!Q32,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="M30" s="115" t="str">
+        <f>LEFT(Full!P32,(FIND(";",Full!P32,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="N30" s="104" t="str">
+        <f>LEFT(Full!O32,(FIND(";",Full!O32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O30" s="104" t="str">
+        <f>LEFT(Full!N32,(FIND(";",Full!N32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P30" s="104" t="str">
+        <f>LEFT(Full!M32,(FIND(";",Full!M32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q30" s="113" t="str">
+        <f>LEFT(Full!L32,(FIND(";",Full!L32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R30" s="104" t="str">
+        <f>LEFT(Full!K32,(FIND(";",Full!K32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S30" s="112" t="str">
+        <f>LEFT(Full!J32,(FIND(";",Full!J32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T30" s="112" t="str">
+        <f>LEFT(Full!I32,(FIND(";",Full!I32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U30" s="104" t="str">
+        <f>LEFT(Full!H32,(FIND(";",Full!H32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V30" s="104" t="str">
+        <f>LEFT(Full!G32,(FIND(";",Full!G32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W30" s="103" t="str">
+        <f>LEFT(Full!F32,(FIND(";",Full!F32,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="X30" s="103" t="str">
+        <f>LEFT(Full!E32,(FIND(";",Full!E32,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Y30" s="102" t="str">
+        <f>LEFT(Full!D32,(FIND(";",Full!D32,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Z30" s="102" t="str">
+        <f>LEFT(Full!C32,(FIND(";",Full!C32,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="AA30" s="104" t="str">
+        <f>LEFT(Full!B32,(FIND(";",Full!B32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="99">
+        <v>23</v>
+      </c>
+      <c r="B31" s="118" t="str">
+        <f>LEFT(Full!AA33,(FIND(";",Full!AA33,1)-1))</f>
+        <v>REF_DIG_N</v>
+      </c>
+      <c r="C31" s="112" t="str">
+        <f>LEFT(Full!Z33,(FIND(";",Full!Z33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D31" s="112" t="str">
+        <f>LEFT(Full!Y33,(FIND(";",Full!Y33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E31" s="104" t="str">
+        <f>LEFT(Full!X33,(FIND(";",Full!X33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F31" s="104" t="str">
+        <f>LEFT(Full!W33,(FIND(";",Full!W33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G31" s="112" t="str">
+        <f>LEFT(Full!V33,(FIND(";",Full!V33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H31" s="112" t="str">
+        <f>LEFT(Full!U33,(FIND(";",Full!U33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I31" s="113" t="str">
+        <f>LEFT(Full!T33,(FIND(";",Full!T33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J31" s="104" t="str">
+        <f>LEFT(Full!S33,(FIND(";",Full!S33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K31" s="104" t="str">
+        <f>LEFT(Full!R33,(FIND(";",Full!R33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L31" s="116" t="str">
+        <f>LEFT(Full!Q33,(FIND(";",Full!Q33,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="M31" s="116" t="str">
+        <f>LEFT(Full!P33,(FIND(";",Full!P33,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="N31" s="116" t="str">
+        <f>LEFT(Full!O33,(FIND(";",Full!O33,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="O31" s="104" t="str">
+        <f>LEFT(Full!N33,(FIND(";",Full!N33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P31" s="104" t="str">
+        <f>LEFT(Full!M33,(FIND(";",Full!M33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q31" s="113" t="str">
+        <f>LEFT(Full!L33,(FIND(";",Full!L33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R31" s="104" t="str">
+        <f>LEFT(Full!K33,(FIND(";",Full!K33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S31" s="112" t="str">
+        <f>LEFT(Full!J33,(FIND(";",Full!J33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T31" s="112" t="str">
+        <f>LEFT(Full!I33,(FIND(";",Full!I33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U31" s="104" t="str">
+        <f>LEFT(Full!H33,(FIND(";",Full!H33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V31" s="104" t="str">
+        <f>LEFT(Full!G33,(FIND(";",Full!G33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W31" s="103" t="str">
+        <f>LEFT(Full!F33,(FIND(";",Full!F33,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="X31" s="103" t="str">
+        <f>LEFT(Full!E33,(FIND(";",Full!E33,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Y31" s="102" t="str">
+        <f>LEFT(Full!D33,(FIND(";",Full!D33,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Z31" s="102" t="str">
+        <f>LEFT(Full!C33,(FIND(";",Full!C33,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="AA31" s="100" t="str">
+        <f>LEFT(Full!B33,(FIND(";",Full!B33,1)-1))</f>
+        <v>REF_LO_N</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="99">
+        <v>24</v>
+      </c>
+      <c r="B32" s="118" t="str">
+        <f>LEFT(Full!AA34,(FIND(";",Full!AA34,1)-1))</f>
+        <v>REF_DIG_P</v>
+      </c>
+      <c r="C32" s="102" t="str">
+        <f>LEFT(Full!Z34,(FIND(";",Full!Z34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="D32" s="102" t="str">
+        <f>LEFT(Full!Y34,(FIND(";",Full!Y34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="E32" s="103" t="str">
+        <f>LEFT(Full!X34,(FIND(";",Full!X34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="F32" s="103" t="str">
+        <f>LEFT(Full!W34,(FIND(";",Full!W34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="G32" s="104" t="str">
+        <f>LEFT(Full!V34,(FIND(";",Full!V34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H32" s="104" t="str">
+        <f>LEFT(Full!U34,(FIND(";",Full!U34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I32" s="112" t="str">
+        <f>LEFT(Full!T34,(FIND(";",Full!T34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J32" s="112" t="str">
+        <f>LEFT(Full!S34,(FIND(";",Full!S34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K32" s="104" t="str">
+        <f>LEFT(Full!R34,(FIND(";",Full!R34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L32" s="115" t="str">
+        <f>LEFT(Full!Q34,(FIND(";",Full!Q34,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="M32" s="115" t="str">
+        <f>LEFT(Full!P34,(FIND(";",Full!P34,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="N32" s="104" t="str">
+        <f>LEFT(Full!O34,(FIND(";",Full!O34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O32" s="104" t="str">
+        <f>LEFT(Full!N34,(FIND(";",Full!N34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P32" s="104" t="str">
+        <f>LEFT(Full!M34,(FIND(";",Full!M34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q32" s="114" t="str">
+        <f>LEFT(Full!L34,(FIND(";",Full!L34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R32" s="112" t="str">
+        <f>LEFT(Full!K34,(FIND(";",Full!K34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S32" s="104" t="str">
+        <f>LEFT(Full!J34,(FIND(";",Full!J34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T32" s="104" t="str">
+        <f>LEFT(Full!I34,(FIND(";",Full!I34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U32" s="112" t="str">
+        <f>LEFT(Full!H34,(FIND(";",Full!H34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V32" s="112" t="str">
+        <f>LEFT(Full!G34,(FIND(";",Full!G34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W32" s="110" t="str">
+        <f>LEFT(Full!F34,(FIND(";",Full!F34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="X32" s="102" t="str">
+        <f>LEFT(Full!E34,(FIND(";",Full!E34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Y32" s="103" t="str">
+        <f>LEFT(Full!D34,(FIND(";",Full!D34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Z32" s="103" t="str">
+        <f>LEFT(Full!C34,(FIND(";",Full!C34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="AA32" s="100" t="str">
+        <f>LEFT(Full!B34,(FIND(";",Full!B34,1)-1))</f>
+        <v>REF_LO_P</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="99">
+        <v>25</v>
+      </c>
+      <c r="B33" s="104" t="str">
+        <f>LEFT(Full!AA35,(FIND(";",Full!AA35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C33" s="106" t="str">
+        <f>LEFT(Full!Z35,(FIND(";",Full!Z35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="D33" s="106" t="str">
+        <f>LEFT(Full!Y35,(FIND(";",Full!Y35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="E33" s="103" t="str">
+        <f>LEFT(Full!X35,(FIND(";",Full!X35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="F33" s="103" t="str">
+        <f>LEFT(Full!W35,(FIND(";",Full!W35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="G33" s="104" t="str">
+        <f>LEFT(Full!V35,(FIND(";",Full!V35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H33" s="104" t="str">
+        <f>LEFT(Full!U35,(FIND(";",Full!U35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I33" s="112" t="str">
+        <f>LEFT(Full!T35,(FIND(";",Full!T35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J33" s="112" t="str">
+        <f>LEFT(Full!S35,(FIND(";",Full!S35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K33" s="104" t="str">
+        <f>LEFT(Full!R35,(FIND(";",Full!R35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L33" s="115" t="str">
+        <f>LEFT(Full!Q35,(FIND(";",Full!Q35,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="M33" s="115" t="str">
+        <f>LEFT(Full!P35,(FIND(";",Full!P35,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="N33" s="104" t="str">
+        <f>LEFT(Full!O35,(FIND(";",Full!O35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O33" s="104" t="str">
+        <f>LEFT(Full!N35,(FIND(";",Full!N35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P33" s="104" t="str">
+        <f>LEFT(Full!M35,(FIND(";",Full!M35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q33" s="114" t="str">
+        <f>LEFT(Full!L35,(FIND(";",Full!L35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R33" s="112" t="str">
+        <f>LEFT(Full!K35,(FIND(";",Full!K35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S33" s="104" t="str">
+        <f>LEFT(Full!J35,(FIND(";",Full!J35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T33" s="104" t="str">
+        <f>LEFT(Full!I35,(FIND(";",Full!I35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U33" s="112" t="str">
+        <f>LEFT(Full!H35,(FIND(";",Full!H35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V33" s="112" t="str">
+        <f>LEFT(Full!G35,(FIND(";",Full!G35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W33" s="111" t="str">
+        <f>LEFT(Full!F35,(FIND(";",Full!F35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="X33" s="106" t="str">
+        <f>LEFT(Full!E35,(FIND(";",Full!E35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Y33" s="107" t="str">
+        <f>LEFT(Full!D35,(FIND(";",Full!D35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Z33" s="107" t="str">
+        <f>LEFT(Full!C35,(FIND(";",Full!C35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="AA33" s="104" t="str">
+        <f>LEFT(Full!B35,(FIND(";",Full!B35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="99">
+        <v>26</v>
+      </c>
+      <c r="B34" s="109" t="str">
+        <f>LEFT(Full!AA36,(FIND(";",Full!AA36,1)-1))</f>
+        <v>NC</v>
+      </c>
+      <c r="C34" s="104" t="str">
+        <f>LEFT(Full!Z36,(FIND(";",Full!Z36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D34" s="105" t="str">
+        <f>LEFT(Full!Y36,(FIND(";",Full!Y36,1)-1))</f>
+        <v>ANT_2_N</v>
+      </c>
+      <c r="E34" s="105" t="str">
+        <f>LEFT(Full!X36,(FIND(";",Full!X36,1)-1))</f>
+        <v>ANT_2_P</v>
+      </c>
+      <c r="F34" s="104" t="str">
+        <f>LEFT(Full!W36,(FIND(";",Full!W36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G34" s="104" t="str">
+        <f>LEFT(Full!V36,(FIND(";",Full!V36,1)-1))</f>
+        <v>CLK_DIG_OVERRIDE_N</v>
+      </c>
+      <c r="H34" s="104" t="str">
+        <f>LEFT(Full!U36,(FIND(";",Full!U36,1)-1))</f>
+        <v>CLK_DIG_OVERRIDE_P</v>
+      </c>
+      <c r="I34" s="104" t="str">
+        <f>LEFT(Full!T36,(FIND(";",Full!T36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J34" s="104" t="str">
+        <f>LEFT(Full!S36,(FIND(";",Full!S36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K34" s="101" t="str">
+        <f>LEFT(Full!R36,(FIND(";",Full!R36,1)-1))</f>
+        <v>LINK_BM_TX_2_N</v>
+      </c>
+      <c r="L34" s="101" t="str">
+        <f>LEFT(Full!Q36,(FIND(";",Full!Q36,1)-1))</f>
+        <v>LINK_BM_TX_2_P</v>
+      </c>
+      <c r="M34" s="104" t="str">
+        <f>LEFT(Full!P36,(FIND(";",Full!P36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N34" s="101" t="str">
+        <f>LEFT(Full!O36,(FIND(";",Full!O36,1)-1))</f>
+        <v>LINK_BM_RX_2_N</v>
+      </c>
+      <c r="O34" s="101" t="str">
+        <f>LEFT(Full!N36,(FIND(";",Full!N36,1)-1))</f>
+        <v>LINK_BM_RX_2_P</v>
+      </c>
+      <c r="P34" s="104" t="str">
+        <f>LEFT(Full!M36,(FIND(";",Full!M36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q34" s="100" t="str">
+        <f>LEFT(Full!L36,(FIND(";",Full!L36,1)-1))</f>
+        <v>SERDES_SUPPLY_PROBE_2</v>
+      </c>
+      <c r="R34" s="104" t="str">
+        <f>LEFT(Full!K36,(FIND(";",Full!K36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S34" s="104" t="str">
+        <f>LEFT(Full!J36,(FIND(";",Full!J36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T34" s="108" t="str">
+        <f>LEFT(Full!I36,(FIND(";",Full!I36,1)-1))</f>
+        <v>ANA_MUX_N</v>
+      </c>
+      <c r="U34" s="108" t="str">
+        <f>LEFT(Full!H36,(FIND(";",Full!H36,1)-1))</f>
+        <v>ANA_MUX_P</v>
+      </c>
+      <c r="V34" s="104" t="str">
+        <f>LEFT(Full!G36,(FIND(";",Full!G36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W34" s="104" t="str">
+        <f>LEFT(Full!F36,(FIND(";",Full!F36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X34" s="105" t="str">
+        <f>LEFT(Full!E36,(FIND(";",Full!E36,1)-1))</f>
+        <v>ANT_3_N</v>
+      </c>
+      <c r="Y34" s="105" t="str">
+        <f>LEFT(Full!D36,(FIND(";",Full!D36,1)-1))</f>
+        <v>ANT_3_P</v>
+      </c>
+      <c r="Z34" s="104" t="str">
+        <f>LEFT(Full!C36,(FIND(";",Full!C36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA34" s="109" t="str">
+        <f>LEFT(Full!B36,(FIND(";",Full!B36,1)-1))</f>
+        <v>NC</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Solved the Component 3D models issue.
</commit_message>
<xml_diff>
--- a/Files_for_TestPlan_TestReports/FADER2_bumps.xlsx
+++ b/Files_for_TestPlan_TestReports/FADER2_bumps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caolen\Nokia\Fader2.5\fader25_pcb\Files_for_TestPlan_TestReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4807E160-1154-40C2-81D5-B168F491B0A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1F85C6-A12D-4DF2-9F92-D13A3E6A36F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="240" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="240" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="BUMP_DOWN" sheetId="4" r:id="rId3"/>
     <sheet name="Bare_for_export" sheetId="3" r:id="rId4"/>
     <sheet name="BUMP_DOWN_check" sheetId="5" r:id="rId5"/>
+    <sheet name="BumpNets" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -751,8 +752,728 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={BDE5BDA6-CB32-4CC0-B89C-A155A6BDE68C}</author>
+    <author>tc={29E01679-7890-4367-9C9E-CD815055852D}</author>
+    <author>tc={F8A1A964-95D9-40B3-B898-FAC2FCADFBAA}</author>
+    <author>tc={81EDBE8E-5C69-4009-B4B1-F7B4BD4286E5}</author>
+    <author>tc={003BB8F6-F217-4B0D-AC8F-6E961F9FBFBB}</author>
+    <author>tc={14AF6259-1B7F-4DDD-9815-EA02E1523C1A}</author>
+    <author>tc={FF5668BB-6ADB-4287-B3A7-98790E7A8DCC}</author>
+    <author>tc={5E47CD91-1403-4769-AA85-A1AA9DA9F8F9}</author>
+    <author>tc={E28CCF30-320B-4F7B-A341-C109A1778D26}</author>
+    <author>tc={88CA8277-5748-4E24-BB52-3B8614C3D04B}</author>
+    <author>tc={87530752-9619-45E6-BDE4-D93FBA3907C7}</author>
+    <author>tc={6F75D3C3-A306-43FD-897F-5964BA6813C9}</author>
+    <author>tc={4B6B9B29-F8DC-45BE-9B47-19569749182E}</author>
+    <author>tc={B51C33CC-1AB2-47E4-A860-828989CA44E4}</author>
+    <author>tc={39A8F800-FBAF-4771-858F-5E85EFFF802C}</author>
+    <author>tc={3F2BC4E4-D9E7-4A92-AB26-BBA961BFD784}</author>
+    <author>tc={AC9A66B2-D393-4DCD-895C-49B4753B39DA}</author>
+    <author>tc={26DD7C9B-9752-4FFA-A7B8-376E6F8E7A8A}</author>
+    <author>tc={2D0765EC-F349-4AB8-930F-ADEB31E5B2BE}</author>
+    <author>tc={7FE67145-F7AC-4E55-BD98-6A5264CD942D}</author>
+    <author>tc={D25EA8B3-9788-4A16-9701-31D5D9F3C44E}</author>
+    <author>tc={521D1DA4-659B-4E31-99E2-D2971D787465}</author>
+    <author>tc={4238F18B-FEE2-48B3-92A0-25D9218D1F32}</author>
+    <author>tc={6DA30A73-DEF3-4FD9-823B-FE567719B845}</author>
+    <author>tc={EA39886B-7F5E-4ED1-B04F-C3115DAFEA63}</author>
+    <author>tc={55B1F6BC-FAD0-4B60-B366-AC975894A81D}</author>
+    <author>tc={034D7C97-052D-4827-A188-7091E6AFA86E}</author>
+    <author>tc={50F729DE-08A8-4F38-BF3C-C7F31B3C8FDE}</author>
+    <author>tc={52A123F1-85C3-4DA8-8ADF-E9A7163388AF}</author>
+    <author>tc={62B8E12F-2A49-4A08-8E2C-9C398A8CF3D6}</author>
+    <author>tc={2701B0F1-F89C-4E52-AE43-CBF640EA1DEA}</author>
+    <author>tc={F83C8C57-D2F2-4EBE-89A7-0837BA91C144}</author>
+    <author>tc={CB92F0D1-BA93-4BE7-B6D9-EE932BADD1F7}</author>
+    <author>tc={887C81DC-D3D9-4535-A120-A4A01995D652}</author>
+    <author>tc={7A8759AA-A0EA-44B8-8EB3-C6C82B350FE4}</author>
+    <author>tc={71765772-9431-4CE7-84C1-5E0C0B9E1733}</author>
+    <author>tc={5091BB0F-049F-4F56-93D0-A9D6F05E201B}</author>
+    <author>tc={81C75C56-9F0A-43C3-A863-1CDFED55584A}</author>
+    <author>tc={E3F5A2C1-4B66-42F6-9CB9-1DBB461F76E2}</author>
+    <author>tc={66D21BE1-9AE2-4141-BA67-7A173A43690F}</author>
+    <author>tc={EBF86732-58B3-40FD-879E-4E993913DC1B}</author>
+    <author>tc={983EF7DB-3186-4A50-97C4-8B55ADBC824E}</author>
+    <author>tc={10278EE9-2EC6-48F2-8908-9FE64E180CF1}</author>
+    <author>tc={1551E8A3-72F6-4797-B5EA-0ACFB26201D7}</author>
+    <author>tc={97FFD680-B771-4B27-8A22-162952EDF013}</author>
+    <author>tc={FFBECB4B-872F-48E1-93EF-63FD9C23A7F9}</author>
+    <author>tc={3C0015A2-1FB2-4D74-95DF-3E1189A4AA7F}</author>
+    <author>tc={7D72F398-6F0A-4BBF-99D1-E302D27FEAA8}</author>
+    <author>tc={F032D927-A854-468A-AAAB-331E18C71AE3}</author>
+    <author>tc={E2B9FD76-C3F4-42E0-B3FD-2AFCB60612F0}</author>
+    <author>tc={3DEB9FD6-F649-4570-8F24-A916A062B55C}</author>
+    <author>tc={936C452D-DA9E-4FFC-81EC-D34A738C3AB4}</author>
+    <author>tc={47A9B048-8522-4BEC-B384-EB5546BAAF5E}</author>
+    <author>tc={0C8B3908-F02B-4DE1-876B-71DB3FCDD509}</author>
+    <author>tc={E77ADBBB-DB0D-4326-B7A0-917D3DDE787F}</author>
+    <author>tc={2DCF5F9B-C09D-4872-9486-3970C9B68DB4}</author>
+    <author>tc={14D3DEA3-1C33-4287-8607-7E557D5EBBC6}</author>
+    <author>tc={53DD59EB-42BB-4394-BC5A-0B10F5A5E179}</author>
+    <author>tc={4F85480C-B7C0-49F6-B23B-057A003A9EAC}</author>
+    <author>tc={FDB59AA9-BE08-4F1B-95F7-0B1D4EB3E22F}</author>
+    <author>tc={117480FE-DB3B-4255-BB6D-253687A9CDA7}</author>
+    <author>tc={C84C240C-30E6-4FEE-88D6-658F9448035E}</author>
+    <author>tc={F7FA3E23-FD82-4317-9736-9EB5FBACE6E8}</author>
+    <author>tc={A7010E83-C9E2-4C24-B934-C6CC100EF3AC}</author>
+    <author>tc={E6D8FCBA-D9EE-45C7-9F39-82068746AAAE}</author>
+    <author>tc={AA8E01F2-9E73-420C-A338-34DA08CFA35A}</author>
+    <author>tc={BEAEC392-1188-4750-AF2E-ECE53D04F183}</author>
+    <author>tc={0FE15E43-9ECE-4F64-8DC8-EC906B725029}</author>
+    <author>tc={E57DF2AA-1538-4E2A-A288-61B46383AE88}</author>
+    <author>tc={D9E26C60-9355-47A1-8D3A-9C897A3832B6}</author>
+    <author>tc={C36DEBFD-9502-4F3E-BA22-514A04B38603}</author>
+    <author>tc={DA1E4AF7-DE87-4A65-A6AE-3586575164E0}</author>
+    <author>tc={3E71FC0C-F4A1-4410-9932-1D337F50B03E}</author>
+    <author>tc={ECC6D9B6-BDC8-4DDD-AF49-3883110FD668}</author>
+    <author>tc={C9AF7EDA-1E04-466D-A5A3-40DCFFC8B3A8}</author>
+    <author>tc={C1C571C0-90A9-4017-9975-8D9392542D91}</author>
+    <author>tc={28FF81FB-128B-4B9F-8F44-50CF3A945ABE}</author>
+    <author>tc={D14371A0-F488-42FF-B49E-78F3D68E5D0B}</author>
+    <author>tc={AA787274-6F90-46B1-BC5F-74913F1F994C}</author>
+  </authors>
+  <commentList>
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{BDE5BDA6-CB32-4CC0-B89C-A155A6BDE68C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Y1</t>
+      </text>
+    </comment>
+    <comment ref="K9" authorId="1" shapeId="0" xr:uid="{29E01679-7890-4367-9C9E-CD815055852D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_T1</t>
+      </text>
+    </comment>
+    <comment ref="L9" authorId="2" shapeId="0" xr:uid="{F8A1A964-95D9-40B3-B898-FAC2FCADFBAA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_T1</t>
+      </text>
+    </comment>
+    <comment ref="N9" authorId="3" shapeId="0" xr:uid="{81EDBE8E-5C69-4009-B4B1-F7B4BD4286E5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_N1</t>
+      </text>
+    </comment>
+    <comment ref="O9" authorId="4" shapeId="0" xr:uid="{003BB8F6-F217-4B0D-AC8F-6E961F9FBFBB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_N1</t>
+      </text>
+    </comment>
+    <comment ref="Q9" authorId="5" shapeId="0" xr:uid="{14AF6259-1B7F-4DDD-9815-EA02E1523C1A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    L1</t>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="6" shapeId="0" xr:uid="{FF5668BB-6ADB-4287-B3A7-98790E7A8DCC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P2</t>
+      </text>
+    </comment>
+    <comment ref="N10" authorId="7" shapeId="0" xr:uid="{5E47CD91-1403-4769-AA85-A1AA9DA9F8F9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P2</t>
+      </text>
+    </comment>
+    <comment ref="M11" authorId="8" shapeId="0" xr:uid="{E28CCF30-320B-4F7B-A341-C109A1778D26}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P2</t>
+      </text>
+    </comment>
+    <comment ref="N11" authorId="9" shapeId="0" xr:uid="{88CA8277-5748-4E24-BB52-3B8614C3D04B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P2</t>
+      </text>
+    </comment>
+    <comment ref="M13" authorId="10" shapeId="0" xr:uid="{87530752-9619-45E6-BDE4-D93FBA3907C7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P5</t>
+      </text>
+    </comment>
+    <comment ref="N13" authorId="11" shapeId="0" xr:uid="{6F75D3C3-A306-43FD-897F-5964BA6813C9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P5</t>
+      </text>
+    </comment>
+    <comment ref="M14" authorId="12" shapeId="0" xr:uid="{4B6B9B29-F8DC-45BE-9B47-19569749182E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P5</t>
+      </text>
+    </comment>
+    <comment ref="N14" authorId="13" shapeId="0" xr:uid="{B51C33CC-1AB2-47E4-A860-828989CA44E4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_P5</t>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="14" shapeId="0" xr:uid="{39A8F800-FBAF-4771-858F-5E85EFFF802C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD8</t>
+      </text>
+    </comment>
+    <comment ref="C16" authorId="15" shapeId="0" xr:uid="{3F2BC4E4-D9E7-4A92-AB26-BBA961BFD784}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD8</t>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="16" shapeId="0" xr:uid="{AC9A66B2-D393-4DCD-895C-49B4753B39DA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD8</t>
+      </text>
+    </comment>
+    <comment ref="Y16" authorId="17" shapeId="0" xr:uid="{26DD7C9B-9752-4FFA-A7B8-376E6F8E7A8A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A8</t>
+      </text>
+    </comment>
+    <comment ref="Z16" authorId="18" shapeId="0" xr:uid="{2D0765EC-F349-4AB8-930F-ADEB31E5B2BE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A8</t>
+      </text>
+    </comment>
+    <comment ref="AA16" authorId="19" shapeId="0" xr:uid="{7FE67145-F7AC-4E55-BD98-6A5264CD942D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A8</t>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="20" shapeId="0" xr:uid="{D25EA8B3-9788-4A16-9701-31D5D9F3C44E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD8</t>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="21" shapeId="0" xr:uid="{521D1DA4-659B-4E31-99E2-D2971D787465}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD8</t>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="22" shapeId="0" xr:uid="{4238F18B-FEE2-48B3-92A0-25D9218D1F32}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD8</t>
+      </text>
+    </comment>
+    <comment ref="Y17" authorId="23" shapeId="0" xr:uid="{6DA30A73-DEF3-4FD9-823B-FE567719B845}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A8</t>
+      </text>
+    </comment>
+    <comment ref="Z17" authorId="24" shapeId="0" xr:uid="{EA39886B-7F5E-4ED1-B04F-C3115DAFEA63}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A8</t>
+      </text>
+    </comment>
+    <comment ref="AA17" authorId="25" shapeId="0" xr:uid="{55B1F6BC-FAD0-4B60-B366-AC975894A81D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A8</t>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="26" shapeId="0" xr:uid="{034D7C97-052D-4827-A188-7091E6AFA86E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD11</t>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="27" shapeId="0" xr:uid="{50F729DE-08A8-4F38-BF3C-C7F31B3C8FDE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD11</t>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="28" shapeId="0" xr:uid="{52A123F1-85C3-4DA8-8ADF-E9A7163388AF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD11</t>
+      </text>
+    </comment>
+    <comment ref="Y19" authorId="29" shapeId="0" xr:uid="{62B8E12F-2A49-4A08-8E2C-9C398A8CF3D6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A11</t>
+      </text>
+    </comment>
+    <comment ref="Z19" authorId="30" shapeId="0" xr:uid="{2701B0F1-F89C-4E52-AE43-CBF640EA1DEA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A11</t>
+      </text>
+    </comment>
+    <comment ref="AA19" authorId="31" shapeId="0" xr:uid="{F83C8C57-D2F2-4EBE-89A7-0837BA91C144}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A11</t>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="32" shapeId="0" xr:uid="{CB92F0D1-BA93-4BE7-B6D9-EE932BADD1F7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD11</t>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="33" shapeId="0" xr:uid="{887C81DC-D3D9-4535-A120-A4A01995D652}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD11</t>
+      </text>
+    </comment>
+    <comment ref="D20" authorId="34" shapeId="0" xr:uid="{7A8759AA-A0EA-44B8-8EB3-C6C82B350FE4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD11</t>
+      </text>
+    </comment>
+    <comment ref="Y20" authorId="35" shapeId="0" xr:uid="{71765772-9431-4CE7-84C1-5E0C0B9E1733}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A11</t>
+      </text>
+    </comment>
+    <comment ref="Z20" authorId="36" shapeId="0" xr:uid="{5091BB0F-049F-4F56-93D0-A9D6F05E201B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A11</t>
+      </text>
+    </comment>
+    <comment ref="AA20" authorId="37" shapeId="0" xr:uid="{81C75C56-9F0A-43C3-A863-1CDFED55584A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A11</t>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="38" shapeId="0" xr:uid="{E3F5A2C1-4B66-42F6-9CB9-1DBB461F76E2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD14</t>
+      </text>
+    </comment>
+    <comment ref="C22" authorId="39" shapeId="0" xr:uid="{66D21BE1-9AE2-4141-BA67-7A173A43690F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD14</t>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="40" shapeId="0" xr:uid="{EBF86732-58B3-40FD-879E-4E993913DC1B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD14</t>
+      </text>
+    </comment>
+    <comment ref="Y22" authorId="41" shapeId="0" xr:uid="{983EF7DB-3186-4A50-97C4-8B55ADBC824E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    GATE_LINK</t>
+      </text>
+    </comment>
+    <comment ref="Z22" authorId="42" shapeId="0" xr:uid="{10278EE9-2EC6-48F2-8908-9FE64E180CF1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    GATE_LINK</t>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="43" shapeId="0" xr:uid="{1551E8A3-72F6-4797-B5EA-0ACFB26201D7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD14</t>
+      </text>
+    </comment>
+    <comment ref="C23" authorId="44" shapeId="0" xr:uid="{97FFD680-B771-4B27-8A22-162952EDF013}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD14</t>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="45" shapeId="0" xr:uid="{FFBECB4B-872F-48E1-93EF-63FD9C23A7F9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD14</t>
+      </text>
+    </comment>
+    <comment ref="Y23" authorId="46" shapeId="0" xr:uid="{3C0015A2-1FB2-4D74-95DF-3E1189A4AA7F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    GATE_LINK</t>
+      </text>
+    </comment>
+    <comment ref="Z23" authorId="47" shapeId="0" xr:uid="{7D72F398-6F0A-4BBF-99D1-E302D27FEAA8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    GATE_LINK</t>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="48" shapeId="0" xr:uid="{F032D927-A854-468A-AAAB-331E18C71AE3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD17</t>
+      </text>
+    </comment>
+    <comment ref="C25" authorId="49" shapeId="0" xr:uid="{E2B9FD76-C3F4-42E0-B3FD-2AFCB60612F0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD17</t>
+      </text>
+    </comment>
+    <comment ref="D25" authorId="50" shapeId="0" xr:uid="{3DEB9FD6-F649-4570-8F24-A916A062B55C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD17</t>
+      </text>
+    </comment>
+    <comment ref="Y25" authorId="51" shapeId="0" xr:uid="{936C452D-DA9E-4FFC-81EC-D34A738C3AB4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    VDD_LINK</t>
+      </text>
+    </comment>
+    <comment ref="Z25" authorId="52" shapeId="0" xr:uid="{47A9B048-8522-4BEC-B384-EB5546BAAF5E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    VDD_LINK</t>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="53" shapeId="0" xr:uid="{0C8B3908-F02B-4DE1-876B-71DB3FCDD509}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD17</t>
+      </text>
+    </comment>
+    <comment ref="C26" authorId="54" shapeId="0" xr:uid="{E77ADBBB-DB0D-4326-B7A0-917D3DDE787F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD17</t>
+      </text>
+    </comment>
+    <comment ref="D26" authorId="55" shapeId="0" xr:uid="{2DCF5F9B-C09D-4872-9486-3970C9B68DB4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AD17</t>
+      </text>
+    </comment>
+    <comment ref="Y26" authorId="56" shapeId="0" xr:uid="{14D3DEA3-1C33-4287-8607-7E557D5EBBC6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    VDD_LINK</t>
+      </text>
+    </comment>
+    <comment ref="Z26" authorId="57" shapeId="0" xr:uid="{53DD59EB-42BB-4394-BC5A-0B10F5A5E179}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    VDD_LINK</t>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="58" shapeId="0" xr:uid="{4F85480C-B7C0-49F6-B23B-057A003A9EAC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AF20</t>
+      </text>
+    </comment>
+    <comment ref="AA28" authorId="59" shapeId="0" xr:uid="{FDB59AA9-BE08-4F1B-95F7-0B1D4EB3E22F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A20</t>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="60" shapeId="0" xr:uid="{117480FE-DB3B-4255-BB6D-253687A9CDA7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AF20</t>
+      </text>
+    </comment>
+    <comment ref="L29" authorId="61" shapeId="0" xr:uid="{C84C240C-30E6-4FEE-88D6-658F9448035E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R21</t>
+      </text>
+    </comment>
+    <comment ref="M29" authorId="62" shapeId="0" xr:uid="{F7FA3E23-FD82-4317-9736-9EB5FBACE6E8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R21</t>
+      </text>
+    </comment>
+    <comment ref="AA29" authorId="63" shapeId="0" xr:uid="{A7010E83-C9E2-4C24-B934-C6CC100EF3AC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A20</t>
+      </text>
+    </comment>
+    <comment ref="L30" authorId="64" shapeId="0" xr:uid="{E6D8FCBA-D9EE-45C7-9F39-82068746AAAE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R21</t>
+      </text>
+    </comment>
+    <comment ref="M30" authorId="65" shapeId="0" xr:uid="{AA8E01F2-9E73-420C-A338-34DA08CFA35A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R21</t>
+      </text>
+    </comment>
+    <comment ref="B31" authorId="66" shapeId="0" xr:uid="{BEAEC392-1188-4750-AF2E-ECE53D04F183}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AF23</t>
+      </text>
+    </comment>
+    <comment ref="AA31" authorId="67" shapeId="0" xr:uid="{0FE15E43-9ECE-4F64-8DC8-EC906B725029}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A23</t>
+      </text>
+    </comment>
+    <comment ref="B32" authorId="68" shapeId="0" xr:uid="{E57DF2AA-1538-4E2A-A288-61B46383AE88}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_AF23</t>
+      </text>
+    </comment>
+    <comment ref="L32" authorId="69" shapeId="0" xr:uid="{D9E26C60-9355-47A1-8D3A-9C897A3832B6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R24</t>
+      </text>
+    </comment>
+    <comment ref="M32" authorId="70" shapeId="0" xr:uid="{C36DEBFD-9502-4F3E-BA22-514A04B38603}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R24</t>
+      </text>
+    </comment>
+    <comment ref="AA32" authorId="71" shapeId="0" xr:uid="{DA1E4AF7-DE87-4A65-A6AE-3586575164E0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_A23</t>
+      </text>
+    </comment>
+    <comment ref="L33" authorId="72" shapeId="0" xr:uid="{3E71FC0C-F4A1-4410-9932-1D337F50B03E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R24</t>
+      </text>
+    </comment>
+    <comment ref="M33" authorId="73" shapeId="0" xr:uid="{ECC6D9B6-BDC8-4DDD-AF49-3883110FD668}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_R24</t>
+      </text>
+    </comment>
+    <comment ref="K34" authorId="74" shapeId="0" xr:uid="{C9AF7EDA-1E04-466D-A5A3-40DCFFC8B3A8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_T26</t>
+      </text>
+    </comment>
+    <comment ref="L34" authorId="75" shapeId="0" xr:uid="{C1C571C0-90A9-4017-9975-8D9392542D91}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_T26</t>
+      </text>
+    </comment>
+    <comment ref="N34" authorId="76" shapeId="0" xr:uid="{28FF81FB-128B-4B9F-8F44-50CF3A945ABE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_N26</t>
+      </text>
+    </comment>
+    <comment ref="O34" authorId="77" shapeId="0" xr:uid="{D14371A0-F488-42FF-B49E-78F3D68E5D0B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NetU2_N26</t>
+      </text>
+    </comment>
+    <comment ref="Q34" authorId="78" shapeId="0" xr:uid="{AA787274-6F90-46B1-BC5F-74913F1F994C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    L26</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="132">
   <si>
     <t>name</t>
   </si>
@@ -1131,6 +1852,24 @@
   <si>
     <t>AF</t>
   </si>
+  <si>
+    <t>VDD_BM0</t>
+  </si>
+  <si>
+    <t>VDD_BM1</t>
+  </si>
+  <si>
+    <t>VDD_BM3</t>
+  </si>
+  <si>
+    <t>VDD_BM2</t>
+  </si>
+  <si>
+    <t>VDD_LINK_CM0</t>
+  </si>
+  <si>
+    <t>VDD_LINK_CM1</t>
+  </si>
 </sst>
 </file>
 
@@ -1193,19 +1932,20 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="55">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1360,6 +2100,174 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
         <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FFDF0015"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6666FF"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6666FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0099FF"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0099FF"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0099FF"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0099FF"/>
+        <bgColor rgb="FF0066CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0099FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD08B00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD08B00"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1668,7 +2576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2046,7 +2954,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2061,10 +2969,125 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="41" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="42" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="43" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="44" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="49" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="49" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="49" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="49" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="51" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="52" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="52" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="53" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="53" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="54" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2142,10 +3165,15 @@
     </indexedColors>
     <mruColors>
       <color rgb="FF00FF00"/>
-      <color rgb="FFE07070"/>
-      <color rgb="FFDF0015"/>
-      <color rgb="FFBDD7EE"/>
-      <color rgb="FF3366FF"/>
+      <color rgb="FFD08B00"/>
+      <color rgb="FF996600"/>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FFFF6600"/>
+      <color rgb="FF0099FF"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FF6666FF"/>
+      <color rgb="FFFF7C80"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2668,6 +3696,248 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H9" dT="2020-05-15T20:56:53.35" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{BDE5BDA6-CB32-4CC0-B89C-A155A6BDE68C}">
+    <text>Y1</text>
+  </threadedComment>
+  <threadedComment ref="K9" dT="2020-05-15T20:54:58.15" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{29E01679-7890-4367-9C9E-CD815055852D}">
+    <text>NetU2_T1</text>
+  </threadedComment>
+  <threadedComment ref="L9" dT="2020-05-15T20:54:49.29" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{F8A1A964-95D9-40B3-B898-FAC2FCADFBAA}">
+    <text>NetU2_T1</text>
+  </threadedComment>
+  <threadedComment ref="N9" dT="2020-05-15T20:52:23.87" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{81EDBE8E-5C69-4009-B4B1-F7B4BD4286E5}">
+    <text>NetU2_N1</text>
+  </threadedComment>
+  <threadedComment ref="O9" dT="2020-05-15T20:52:16.80" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{003BB8F6-F217-4B0D-AC8F-6E961F9FBFBB}">
+    <text>NetU2_N1</text>
+  </threadedComment>
+  <threadedComment ref="Q9" dT="2020-05-15T20:51:25.87" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{14AF6259-1B7F-4DDD-9815-EA02E1523C1A}">
+    <text>L1</text>
+  </threadedComment>
+  <threadedComment ref="M10" dT="2020-05-15T20:53:26.00" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{FF5668BB-6ADB-4287-B3A7-98790E7A8DCC}">
+    <text>NetU2_P2</text>
+  </threadedComment>
+  <threadedComment ref="N10" dT="2020-05-15T20:53:43.70" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{5E47CD91-1403-4769-AA85-A1AA9DA9F8F9}">
+    <text>NetU2_P2</text>
+  </threadedComment>
+  <threadedComment ref="M11" dT="2020-05-15T20:53:33.09" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{E28CCF30-320B-4F7B-A341-C109A1778D26}">
+    <text>NetU2_P2</text>
+  </threadedComment>
+  <threadedComment ref="N11" dT="2020-05-15T20:53:51.71" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{88CA8277-5748-4E24-BB52-3B8614C3D04B}">
+    <text>NetU2_P2</text>
+  </threadedComment>
+  <threadedComment ref="M13" dT="2020-05-15T20:41:11.70" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{87530752-9619-45E6-BDE4-D93FBA3907C7}">
+    <text>NetU2_P5</text>
+  </threadedComment>
+  <threadedComment ref="N13" dT="2020-05-15T20:41:25.62" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{6F75D3C3-A306-43FD-897F-5964BA6813C9}">
+    <text>NetU2_P5</text>
+  </threadedComment>
+  <threadedComment ref="M14" dT="2020-05-15T20:41:18.39" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{4B6B9B29-F8DC-45BE-9B47-19569749182E}">
+    <text>NetU2_P5</text>
+  </threadedComment>
+  <threadedComment ref="N14" dT="2020-05-15T20:41:32.16" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{B51C33CC-1AB2-47E4-A860-828989CA44E4}">
+    <text>NetU2_P5</text>
+  </threadedComment>
+  <threadedComment ref="B16" dT="2020-05-15T20:35:50.09" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{39A8F800-FBAF-4771-858F-5E85EFFF802C}">
+    <text>NetU2_AD8</text>
+  </threadedComment>
+  <threadedComment ref="C16" dT="2020-05-15T20:36:04.68" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{3F2BC4E4-D9E7-4A92-AB26-BBA961BFD784}">
+    <text>NetU2_AD8</text>
+  </threadedComment>
+  <threadedComment ref="D16" dT="2020-05-15T20:36:19.20" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{AC9A66B2-D393-4DCD-895C-49B4753B39DA}">
+    <text>NetU2_AD8</text>
+  </threadedComment>
+  <threadedComment ref="Y16" dT="2020-05-15T20:46:02.29" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{26DD7C9B-9752-4FFA-A7B8-376E6F8E7A8A}">
+    <text>NetU2_A8</text>
+  </threadedComment>
+  <threadedComment ref="Z16" dT="2020-05-15T20:46:18.92" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{2D0765EC-F349-4AB8-930F-ADEB31E5B2BE}">
+    <text>NetU2_A8</text>
+  </threadedComment>
+  <threadedComment ref="AA16" dT="2020-05-15T20:46:38.89" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{7FE67145-F7AC-4E55-BD98-6A5264CD942D}">
+    <text>NetU2_A8</text>
+  </threadedComment>
+  <threadedComment ref="B17" dT="2020-05-15T20:35:57.05" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{D25EA8B3-9788-4A16-9701-31D5D9F3C44E}">
+    <text>NetU2_AD8</text>
+  </threadedComment>
+  <threadedComment ref="C17" dT="2020-05-15T20:36:11.63" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{521D1DA4-659B-4E31-99E2-D2971D787465}">
+    <text>NetU2_AD8</text>
+  </threadedComment>
+  <threadedComment ref="D17" dT="2020-05-15T20:36:32.64" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{4238F18B-FEE2-48B3-92A0-25D9218D1F32}">
+    <text>NetU2_AD8</text>
+  </threadedComment>
+  <threadedComment ref="Y17" dT="2020-05-15T20:46:11.27" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{6DA30A73-DEF3-4FD9-823B-FE567719B845}">
+    <text>NetU2_A8</text>
+  </threadedComment>
+  <threadedComment ref="Z17" dT="2020-05-15T20:46:26.93" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{EA39886B-7F5E-4ED1-B04F-C3115DAFEA63}">
+    <text>NetU2_A8</text>
+  </threadedComment>
+  <threadedComment ref="AA17" dT="2020-05-15T20:46:45.92" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{55B1F6BC-FAD0-4B60-B366-AC975894A81D}">
+    <text>NetU2_A8</text>
+  </threadedComment>
+  <threadedComment ref="B19" dT="2020-05-15T20:30:44.32" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{034D7C97-052D-4827-A188-7091E6AFA86E}">
+    <text>NetU2_AD11</text>
+  </threadedComment>
+  <threadedComment ref="C19" dT="2020-05-15T20:30:58.35" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{50F729DE-08A8-4F38-BF3C-C7F31B3C8FDE}">
+    <text>NetU2_AD11</text>
+  </threadedComment>
+  <threadedComment ref="D19" dT="2020-05-15T20:31:11.27" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{52A123F1-85C3-4DA8-8ADF-E9A7163388AF}">
+    <text>NetU2_AD11</text>
+  </threadedComment>
+  <threadedComment ref="Y19" dT="2020-05-15T20:20:41.48" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{62B8E12F-2A49-4A08-8E2C-9C398A8CF3D6}">
+    <text>NetU2_A11</text>
+  </threadedComment>
+  <threadedComment ref="Z19" dT="2020-05-15T20:20:10.90" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{2701B0F1-F89C-4E52-AE43-CBF640EA1DEA}">
+    <text>NetU2_A11</text>
+  </threadedComment>
+  <threadedComment ref="AA19" dT="2020-05-15T20:19:54.58" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{F83C8C57-D2F2-4EBE-89A7-0837BA91C144}">
+    <text>NetU2_A11</text>
+  </threadedComment>
+  <threadedComment ref="B20" dT="2020-05-15T20:30:51.21" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{CB92F0D1-BA93-4BE7-B6D9-EE932BADD1F7}">
+    <text>NetU2_AD11</text>
+  </threadedComment>
+  <threadedComment ref="C20" dT="2020-05-15T20:31:04.40" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{887C81DC-D3D9-4535-A120-A4A01995D652}">
+    <text>NetU2_AD11</text>
+  </threadedComment>
+  <threadedComment ref="D20" dT="2020-05-15T20:31:17.84" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{7A8759AA-A0EA-44B8-8EB3-C6C82B350FE4}">
+    <text>NetU2_AD11</text>
+  </threadedComment>
+  <threadedComment ref="Y20" dT="2020-05-15T20:20:50.23" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{71765772-9431-4CE7-84C1-5E0C0B9E1733}">
+    <text>NetU2_A11</text>
+  </threadedComment>
+  <threadedComment ref="Z20" dT="2020-05-15T20:20:18.73" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{5091BB0F-049F-4F56-93D0-A9D6F05E201B}">
+    <text>NetU2_A11</text>
+  </threadedComment>
+  <threadedComment ref="AA20" dT="2020-05-15T20:20:03.70" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{81C75C56-9F0A-43C3-A863-1CDFED55584A}">
+    <text>NetU2_A11</text>
+  </threadedComment>
+  <threadedComment ref="B22" dT="2020-05-15T20:32:13.93" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{E3F5A2C1-4B66-42F6-9CB9-1DBB461F76E2}">
+    <text>NetU2_AD14</text>
+  </threadedComment>
+  <threadedComment ref="C22" dT="2020-05-15T20:32:30.57" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{66D21BE1-9AE2-4141-BA67-7A173A43690F}">
+    <text>NetU2_AD14</text>
+  </threadedComment>
+  <threadedComment ref="D22" dT="2020-05-15T20:32:48.07" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{EBF86732-58B3-40FD-879E-4E993913DC1B}">
+    <text>NetU2_AD14</text>
+  </threadedComment>
+  <threadedComment ref="Y22" dT="2020-05-15T20:16:19.78" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{983EF7DB-3186-4A50-97C4-8B55ADBC824E}">
+    <text>GATE_LINK</text>
+  </threadedComment>
+  <threadedComment ref="Z22" dT="2020-05-15T20:16:34.72" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{10278EE9-2EC6-48F2-8908-9FE64E180CF1}">
+    <text>GATE_LINK</text>
+  </threadedComment>
+  <threadedComment ref="B23" dT="2020-05-15T20:32:21.08" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{1551E8A3-72F6-4797-B5EA-0ACFB26201D7}">
+    <text>NetU2_AD14</text>
+  </threadedComment>
+  <threadedComment ref="C23" dT="2020-05-15T20:32:37.61" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{97FFD680-B771-4B27-8A22-162952EDF013}">
+    <text>NetU2_AD14</text>
+  </threadedComment>
+  <threadedComment ref="D23" dT="2020-05-15T20:32:54.75" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{FFBECB4B-872F-48E1-93EF-63FD9C23A7F9}">
+    <text>NetU2_AD14</text>
+  </threadedComment>
+  <threadedComment ref="Y23" dT="2020-05-15T20:16:26.48" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{3C0015A2-1FB2-4D74-95DF-3E1189A4AA7F}">
+    <text>GATE_LINK</text>
+  </threadedComment>
+  <threadedComment ref="Z23" dT="2020-05-15T20:16:42.30" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{7D72F398-6F0A-4BBF-99D1-E302D27FEAA8}">
+    <text>GATE_LINK</text>
+  </threadedComment>
+  <threadedComment ref="B25" dT="2020-05-15T20:04:43.01" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{F032D927-A854-468A-AAAB-331E18C71AE3}">
+    <text>NetU2_AD17</text>
+  </threadedComment>
+  <threadedComment ref="C25" dT="2020-05-15T20:05:02.07" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{E2B9FD76-C3F4-42E0-B3FD-2AFCB60612F0}">
+    <text>NetU2_AD17</text>
+  </threadedComment>
+  <threadedComment ref="D25" dT="2020-05-15T20:05:28.71" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{3DEB9FD6-F649-4570-8F24-A916A062B55C}">
+    <text>NetU2_AD17</text>
+  </threadedComment>
+  <threadedComment ref="Y25" dT="2020-05-15T20:12:22.99" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{936C452D-DA9E-4FFC-81EC-D34A738C3AB4}">
+    <text>VDD_LINK</text>
+  </threadedComment>
+  <threadedComment ref="Z25" dT="2020-05-15T20:12:42.14" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{47A9B048-8522-4BEC-B384-EB5546BAAF5E}">
+    <text>VDD_LINK</text>
+  </threadedComment>
+  <threadedComment ref="B26" dT="2020-05-15T20:04:54.79" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{0C8B3908-F02B-4DE1-876B-71DB3FCDD509}">
+    <text>NetU2_AD17</text>
+  </threadedComment>
+  <threadedComment ref="C26" dT="2020-05-15T20:05:10.11" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{E77ADBBB-DB0D-4326-B7A0-917D3DDE787F}">
+    <text>NetU2_AD17</text>
+  </threadedComment>
+  <threadedComment ref="D26" dT="2020-05-15T20:05:37.06" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{2DCF5F9B-C09D-4872-9486-3970C9B68DB4}">
+    <text>NetU2_AD17</text>
+  </threadedComment>
+  <threadedComment ref="Y26" dT="2020-05-15T20:12:31.13" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{14D3DEA3-1C33-4287-8607-7E557D5EBBC6}">
+    <text>VDD_LINK</text>
+  </threadedComment>
+  <threadedComment ref="Z26" dT="2020-05-15T20:12:49.17" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{53DD59EB-42BB-4394-BC5A-0B10F5A5E179}">
+    <text>VDD_LINK</text>
+  </threadedComment>
+  <threadedComment ref="B28" dT="2020-05-15T19:59:04.10" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{4F85480C-B7C0-49F6-B23B-057A003A9EAC}">
+    <text>NetU2_AF20</text>
+  </threadedComment>
+  <threadedComment ref="AA28" dT="2020-05-15T19:48:01.53" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{FDB59AA9-BE08-4F1B-95F7-0B1D4EB3E22F}">
+    <text>NetU2_A20</text>
+  </threadedComment>
+  <threadedComment ref="B29" dT="2020-05-15T19:59:12.64" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{117480FE-DB3B-4255-BB6D-253687A9CDA7}">
+    <text>NetU2_AF20</text>
+  </threadedComment>
+  <threadedComment ref="L29" dT="2020-05-15T19:51:44.10" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{C84C240C-30E6-4FEE-88D6-658F9448035E}">
+    <text>NetU2_R21</text>
+  </threadedComment>
+  <threadedComment ref="M29" dT="2020-05-15T19:51:17.38" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{F7FA3E23-FD82-4317-9736-9EB5FBACE6E8}">
+    <text>NetU2_R21</text>
+  </threadedComment>
+  <threadedComment ref="AA29" dT="2020-05-15T19:48:17.56" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{A7010E83-C9E2-4C24-B934-C6CC100EF3AC}">
+    <text>NetU2_A20</text>
+  </threadedComment>
+  <threadedComment ref="L30" dT="2020-05-15T19:51:34.24" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{E6D8FCBA-D9EE-45C7-9F39-82068746AAAE}">
+    <text>NetU2_R21</text>
+  </threadedComment>
+  <threadedComment ref="M30" dT="2020-05-15T19:51:25.29" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{AA8E01F2-9E73-420C-A338-34DA08CFA35A}">
+    <text>NetU2_R21</text>
+  </threadedComment>
+  <threadedComment ref="B31" dT="2020-05-15T19:58:08.91" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{BEAEC392-1188-4750-AF2E-ECE53D04F183}">
+    <text>NetU2_AF23</text>
+  </threadedComment>
+  <threadedComment ref="AA31" dT="2020-05-15T19:45:57.55" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{0FE15E43-9ECE-4F64-8DC8-EC906B725029}">
+    <text>NetU2_A23</text>
+  </threadedComment>
+  <threadedComment ref="B32" dT="2020-05-15T19:58:17.96" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{E57DF2AA-1538-4E2A-A288-61B46383AE88}">
+    <text>NetU2_AF23</text>
+  </threadedComment>
+  <threadedComment ref="L32" dT="2020-05-15T19:53:02.98" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{D9E26C60-9355-47A1-8D3A-9C897A3832B6}">
+    <text>NetU2_R24</text>
+  </threadedComment>
+  <threadedComment ref="M32" dT="2020-05-15T19:52:38.06" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{C36DEBFD-9502-4F3E-BA22-514A04B38603}">
+    <text>NetU2_R24</text>
+  </threadedComment>
+  <threadedComment ref="AA32" dT="2020-05-15T19:46:25.09" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{DA1E4AF7-DE87-4A65-A6AE-3586575164E0}">
+    <text>NetU2_A23</text>
+  </threadedComment>
+  <threadedComment ref="L33" dT="2020-05-15T19:52:55.05" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{3E71FC0C-F4A1-4410-9932-1D337F50B03E}">
+    <text>NetU2_R24</text>
+  </threadedComment>
+  <threadedComment ref="M33" dT="2020-05-15T19:52:47.25" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{ECC6D9B6-BDC8-4DDD-AF49-3883110FD668}">
+    <text>NetU2_R24</text>
+  </threadedComment>
+  <threadedComment ref="K34" dT="2020-05-15T18:49:03.85" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{C9AF7EDA-1E04-466D-A5A3-40DCFFC8B3A8}">
+    <text>NetU2_T26</text>
+  </threadedComment>
+  <threadedComment ref="L34" dT="2020-05-15T18:50:01.29" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{C1C571C0-90A9-4017-9975-8D9392542D91}">
+    <text>NetU2_T26</text>
+  </threadedComment>
+  <threadedComment ref="N34" dT="2020-05-15T18:51:24.80" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{28FF81FB-128B-4B9F-8F44-50CF3A945ABE}">
+    <text>NetU2_N26</text>
+  </threadedComment>
+  <threadedComment ref="O34" dT="2020-05-15T18:53:37.25" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{D14371A0-F488-42FF-B49E-78F3D68E5D0B}">
+    <text>NetU2_N26</text>
+  </threadedComment>
+  <threadedComment ref="Q34" dT="2020-05-15T18:54:31.42" personId="{0F2D2355-BB0C-4E28-9F0B-9D43E54862E0}" id="{AA787274-6F90-46B1-BC5F-74913F1F994C}">
+    <text>L26</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AM49"/>
@@ -13638,7 +14908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E75085E-B800-4513-AA14-6BE0CE50106A}">
   <dimension ref="A2:AL34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
       <selection pane="topRight" activeCell="B8" sqref="B8"/>
@@ -16676,4 +17946,3090 @@
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E832F835-A670-42B0-9E65-F328848494C0}">
+  <dimension ref="A2:AN34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F27" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A8" sqref="A8"/>
+      <selection pane="topRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="AX20" sqref="AX20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="29" width="9" style="22"/>
+    <col min="30" max="30" width="11.25" style="22" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="9" style="22"/>
+    <col min="33" max="33" width="14.375" style="22" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9" style="22"/>
+    <col min="35" max="35" width="14.375" style="22" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="9" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="H6" s="22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="98"/>
+      <c r="B8" s="99" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="99" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="99" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="99" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="99" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="99" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="99" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" s="99" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="99" t="s">
+        <v>117</v>
+      </c>
+      <c r="K8" s="99" t="s">
+        <v>116</v>
+      </c>
+      <c r="L8" s="99" t="s">
+        <v>115</v>
+      </c>
+      <c r="M8" s="99" t="s">
+        <v>114</v>
+      </c>
+      <c r="N8" s="99" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="99" t="s">
+        <v>112</v>
+      </c>
+      <c r="P8" s="99" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q8" s="99" t="s">
+        <v>110</v>
+      </c>
+      <c r="R8" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="S8" s="99" t="s">
+        <v>108</v>
+      </c>
+      <c r="T8" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="U8" s="99" t="s">
+        <v>106</v>
+      </c>
+      <c r="V8" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="W8" s="99" t="s">
+        <v>104</v>
+      </c>
+      <c r="X8" s="99" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y8" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z8" s="99" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA8" s="99" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD8" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE8" s="22">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="99">
+        <v>1</v>
+      </c>
+      <c r="B9" s="142" t="str">
+        <f>LEFT(Full!AA11,(FIND(";",Full!AA11,1)-1))</f>
+        <v>NC</v>
+      </c>
+      <c r="C9" s="104" t="str">
+        <f>LEFT(Full!Z11,(FIND(";",Full!Z11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D9" s="142" t="str">
+        <f>LEFT(Full!Y11,(FIND(";",Full!Y11,1)-1))</f>
+        <v>ANT_1_N</v>
+      </c>
+      <c r="E9" s="142" t="str">
+        <f>LEFT(Full!X11,(FIND(";",Full!X11,1)-1))</f>
+        <v>ANT_1_P</v>
+      </c>
+      <c r="F9" s="104" t="str">
+        <f>LEFT(Full!W11,(FIND(";",Full!W11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G9" s="104" t="str">
+        <f>LEFT(Full!V11,(FIND(";",Full!V11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H9" s="143" t="str">
+        <f>LEFT(Full!U11,(FIND(";",Full!U11,1)-1))</f>
+        <v>IREF_ANALOG</v>
+      </c>
+      <c r="I9" s="104" t="str">
+        <f>LEFT(Full!T11,(FIND(";",Full!T11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J9" s="104" t="str">
+        <f>LEFT(Full!S11,(FIND(";",Full!S11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K9" s="144" t="str">
+        <f>LEFT(Full!R11,(FIND(";",Full!R11,1)-1))</f>
+        <v>LINK_BM_RX_0_N</v>
+      </c>
+      <c r="L9" s="144" t="str">
+        <f>LEFT(Full!Q11,(FIND(";",Full!Q11,1)-1))</f>
+        <v>LINK_BM_RX_0_P</v>
+      </c>
+      <c r="M9" s="104" t="str">
+        <f>LEFT(Full!P11,(FIND(";",Full!P11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N9" s="142" t="str">
+        <f>LEFT(Full!O11,(FIND(";",Full!O11,1)-1))</f>
+        <v>LINK_BM_TX_0_N</v>
+      </c>
+      <c r="O9" s="142" t="str">
+        <f>LEFT(Full!N11,(FIND(";",Full!N11,1)-1))</f>
+        <v>LINK_BM_TX_0_P</v>
+      </c>
+      <c r="P9" s="104" t="str">
+        <f>LEFT(Full!M11,(FIND(";",Full!M11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q9" s="142" t="str">
+        <f>LEFT(Full!L11,(FIND(";",Full!L11,1)-1))</f>
+        <v>SERDES_SUPPLY_PROBE_0</v>
+      </c>
+      <c r="R9" s="142" t="str">
+        <f>LEFT(Full!K11,(FIND(";",Full!K11,1)-1))</f>
+        <v>RESET</v>
+      </c>
+      <c r="S9" s="104" t="str">
+        <f>LEFT(Full!J11,(FIND(";",Full!J11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T9" s="142" t="str">
+        <f>LEFT(Full!I11,(FIND(";",Full!I11,1)-1))</f>
+        <v>LO_OVERRIDE_N</v>
+      </c>
+      <c r="U9" s="142" t="str">
+        <f>LEFT(Full!H11,(FIND(";",Full!H11,1)-1))</f>
+        <v>LO_OVERRIDE_P</v>
+      </c>
+      <c r="V9" s="124" t="str">
+        <f>LEFT(Full!G11,(FIND(";",Full!G11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W9" s="104" t="str">
+        <f>LEFT(Full!F11,(FIND(";",Full!F11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X9" s="142" t="str">
+        <f>LEFT(Full!E11,(FIND(";",Full!E11,1)-1))</f>
+        <v>ANT_0_N</v>
+      </c>
+      <c r="Y9" s="142" t="str">
+        <f>LEFT(Full!D11,(FIND(";",Full!D11,1)-1))</f>
+        <v>ANT_0_P</v>
+      </c>
+      <c r="Z9" s="104" t="str">
+        <f>LEFT(Full!C11,(FIND(";",Full!C11,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA9" s="142" t="str">
+        <f>LEFT(Full!B11,(FIND(";",Full!B11,1)-1))</f>
+        <v>NC</v>
+      </c>
+      <c r="AD9" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE9" s="22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="99">
+        <v>2</v>
+      </c>
+      <c r="B10" s="104" t="str">
+        <f>LEFT(Full!AA12,(FIND(";",Full!AA12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C10" s="146" t="str">
+        <f>LEFT(Full!Z12,(FIND(";",Full!Z12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="D10" s="146" t="str">
+        <f>LEFT(Full!Y12,(FIND(";",Full!Y12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="E10" s="147" t="str">
+        <f>LEFT(Full!X12,(FIND(";",Full!X12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="F10" s="147" t="str">
+        <f>LEFT(Full!W12,(FIND(";",Full!W12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="G10" s="112" t="str">
+        <f>LEFT(Full!V12,(FIND(";",Full!V12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H10" s="112" t="str">
+        <f>LEFT(Full!U12,(FIND(";",Full!U12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I10" s="104" t="str">
+        <f>LEFT(Full!T12,(FIND(";",Full!T12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J10" s="104" t="str">
+        <f>LEFT(Full!S12,(FIND(";",Full!S12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K10" s="104" t="str">
+        <f>LEFT(Full!R12,(FIND(";",Full!R12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L10" s="104" t="str">
+        <f>LEFT(Full!Q12,(FIND(";",Full!Q12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M10" s="175" t="str">
+        <f>LEFT(Full!P12,(FIND(";",Full!P12,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="N10" s="175" t="str">
+        <f>LEFT(Full!O12,(FIND(";",Full!O12,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="O10" s="104" t="str">
+        <f>LEFT(Full!N12,(FIND(";",Full!N12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P10" s="104" t="str">
+        <f>LEFT(Full!M12,(FIND(";",Full!M12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q10" s="104" t="str">
+        <f>LEFT(Full!L12,(FIND(";",Full!L12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R10" s="104" t="str">
+        <f>LEFT(Full!K12,(FIND(";",Full!K12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S10" s="138" t="str">
+        <f>LEFT(Full!J12,(FIND(";",Full!J12,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T10" s="138" t="str">
+        <f>LEFT(Full!I12,(FIND(";",Full!I12,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U10" s="139" t="str">
+        <f>LEFT(Full!H12,(FIND(";",Full!H12,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="V10" s="139" t="str">
+        <f>LEFT(Full!G12,(FIND(";",Full!G12,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="W10" s="146" t="str">
+        <f>LEFT(Full!F12,(FIND(";",Full!F12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="X10" s="146" t="str">
+        <f>LEFT(Full!E12,(FIND(";",Full!E12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Y10" s="147" t="str">
+        <f>LEFT(Full!D12,(FIND(";",Full!D12,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Z10" s="144" t="str">
+        <f>LEFT(Full!C12,(FIND(";",Full!C12,1)-1))</f>
+        <v>NC</v>
+      </c>
+      <c r="AA10" s="104" t="str">
+        <f>LEFT(Full!B12,(FIND(";",Full!B12,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AD10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE10" s="22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="99">
+        <v>3</v>
+      </c>
+      <c r="B11" s="104" t="str">
+        <f>LEFT(Full!AA13,(FIND(";",Full!AA13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C11" s="146" t="str">
+        <f>LEFT(Full!Z13,(FIND(";",Full!Z13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="D11" s="146" t="str">
+        <f>LEFT(Full!Y13,(FIND(";",Full!Y13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="E11" s="147" t="str">
+        <f>LEFT(Full!X13,(FIND(";",Full!X13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="F11" s="147" t="str">
+        <f>LEFT(Full!W13,(FIND(";",Full!W13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="G11" s="112" t="str">
+        <f>LEFT(Full!V13,(FIND(";",Full!V13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H11" s="112" t="str">
+        <f>LEFT(Full!U13,(FIND(";",Full!U13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I11" s="104" t="str">
+        <f>LEFT(Full!T13,(FIND(";",Full!T13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J11" s="104" t="str">
+        <f>LEFT(Full!S13,(FIND(";",Full!S13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K11" s="104" t="str">
+        <f>LEFT(Full!R13,(FIND(";",Full!R13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L11" s="104" t="str">
+        <f>LEFT(Full!Q13,(FIND(";",Full!Q13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M11" s="175" t="str">
+        <f>LEFT(Full!P13,(FIND(";",Full!P13,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="N11" s="175" t="str">
+        <f>LEFT(Full!O13,(FIND(";",Full!O13,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="O11" s="104" t="str">
+        <f>LEFT(Full!N13,(FIND(";",Full!N13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P11" s="104" t="str">
+        <f>LEFT(Full!M13,(FIND(";",Full!M13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q11" s="104" t="str">
+        <f>LEFT(Full!L13,(FIND(";",Full!L13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R11" s="104" t="str">
+        <f>LEFT(Full!K13,(FIND(";",Full!K13,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S11" s="138" t="str">
+        <f>LEFT(Full!J13,(FIND(";",Full!J13,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T11" s="138" t="str">
+        <f>LEFT(Full!I13,(FIND(";",Full!I13,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U11" s="139" t="str">
+        <f>LEFT(Full!H13,(FIND(";",Full!H13,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="V11" s="139" t="str">
+        <f>LEFT(Full!G13,(FIND(";",Full!G13,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="W11" s="146" t="str">
+        <f>LEFT(Full!F13,(FIND(";",Full!F13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="X11" s="146" t="str">
+        <f>LEFT(Full!E13,(FIND(";",Full!E13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Y11" s="147" t="str">
+        <f>LEFT(Full!D13,(FIND(";",Full!D13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Z11" s="147" t="str">
+        <f>LEFT(Full!C13,(FIND(";",Full!C13,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="AA11" s="145" t="str">
+        <f>LEFT(Full!B13,(FIND(";",Full!B13,1)-1))</f>
+        <v>SCAN_IN</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="99">
+        <v>4</v>
+      </c>
+      <c r="B12" s="104" t="str">
+        <f>LEFT(Full!AA14,(FIND(";",Full!AA14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C12" s="104" t="str">
+        <f>LEFT(Full!Z14,(FIND(";",Full!Z14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D12" s="104" t="str">
+        <f>LEFT(Full!Y14,(FIND(";",Full!Y14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E12" s="112" t="str">
+        <f>LEFT(Full!X14,(FIND(";",Full!X14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F12" s="112" t="str">
+        <f>LEFT(Full!W14,(FIND(";",Full!W14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G12" s="104" t="str">
+        <f>LEFT(Full!V14,(FIND(";",Full!V14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H12" s="104" t="str">
+        <f>LEFT(Full!U14,(FIND(";",Full!U14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I12" s="112" t="str">
+        <f>LEFT(Full!T14,(FIND(";",Full!T14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J12" s="112" t="str">
+        <f>LEFT(Full!S14,(FIND(";",Full!S14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K12" s="104" t="str">
+        <f>LEFT(Full!R14,(FIND(";",Full!R14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L12" s="116" t="str">
+        <f>LEFT(Full!Q14,(FIND(";",Full!Q14,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="M12" s="116" t="str">
+        <f>LEFT(Full!P14,(FIND(";",Full!P14,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="N12" s="116" t="str">
+        <f>LEFT(Full!O14,(FIND(";",Full!O14,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="O12" s="104" t="str">
+        <f>LEFT(Full!N14,(FIND(";",Full!N14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P12" s="104" t="str">
+        <f>LEFT(Full!M14,(FIND(";",Full!M14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q12" s="112" t="str">
+        <f>LEFT(Full!L14,(FIND(";",Full!L14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R12" s="112" t="str">
+        <f>LEFT(Full!K14,(FIND(";",Full!K14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S12" s="104" t="str">
+        <f>LEFT(Full!J14,(FIND(";",Full!J14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T12" s="104" t="str">
+        <f>LEFT(Full!I14,(FIND(";",Full!I14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U12" s="112" t="str">
+        <f>LEFT(Full!H14,(FIND(";",Full!H14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V12" s="112" t="str">
+        <f>LEFT(Full!G14,(FIND(";",Full!G14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W12" s="104" t="str">
+        <f>LEFT(Full!F14,(FIND(";",Full!F14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X12" s="104" t="str">
+        <f>LEFT(Full!E14,(FIND(";",Full!E14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y12" s="112" t="str">
+        <f>LEFT(Full!D14,(FIND(";",Full!D14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Z12" s="129" t="str">
+        <f>LEFT(Full!C14,(FIND(";",Full!C14,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA12" s="142" t="str">
+        <f>LEFT(Full!B14,(FIND(";",Full!B14,1)-1))</f>
+        <v>SCAN_EN</v>
+      </c>
+      <c r="AD12" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE12" s="22">
+        <f>(2*AE8+AE8*(AE10-1))</f>
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="99">
+        <v>5</v>
+      </c>
+      <c r="B13" s="104" t="str">
+        <f>LEFT(Full!AA15,(FIND(";",Full!AA15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C13" s="104" t="str">
+        <f>LEFT(Full!Z15,(FIND(";",Full!Z15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D13" s="104" t="str">
+        <f>LEFT(Full!Y15,(FIND(";",Full!Y15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E13" s="112" t="str">
+        <f>LEFT(Full!X15,(FIND(";",Full!X15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F13" s="112" t="str">
+        <f>LEFT(Full!W15,(FIND(";",Full!W15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G13" s="104" t="str">
+        <f>LEFT(Full!V15,(FIND(";",Full!V15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H13" s="104" t="str">
+        <f>LEFT(Full!U15,(FIND(";",Full!U15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I13" s="112" t="str">
+        <f>LEFT(Full!T15,(FIND(";",Full!T15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J13" s="112" t="str">
+        <f>LEFT(Full!S15,(FIND(";",Full!S15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K13" s="104" t="str">
+        <f>LEFT(Full!R15,(FIND(";",Full!R15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L13" s="104" t="str">
+        <f>LEFT(Full!Q15,(FIND(";",Full!Q15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M13" s="177" t="str">
+        <f>LEFT(Full!P15,(FIND(";",Full!P15,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="N13" s="178" t="str">
+        <f>LEFT(Full!O15,(FIND(";",Full!O15,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="O13" s="104" t="str">
+        <f>LEFT(Full!N15,(FIND(";",Full!N15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P13" s="104" t="str">
+        <f>LEFT(Full!M15,(FIND(";",Full!M15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q13" s="112" t="str">
+        <f>LEFT(Full!L15,(FIND(";",Full!L15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R13" s="112" t="str">
+        <f>LEFT(Full!K15,(FIND(";",Full!K15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S13" s="104" t="str">
+        <f>LEFT(Full!J15,(FIND(";",Full!J15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T13" s="104" t="str">
+        <f>LEFT(Full!I15,(FIND(";",Full!I15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U13" s="112" t="str">
+        <f>LEFT(Full!H15,(FIND(";",Full!H15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V13" s="112" t="str">
+        <f>LEFT(Full!G15,(FIND(";",Full!G15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W13" s="104" t="str">
+        <f>LEFT(Full!F15,(FIND(";",Full!F15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X13" s="104" t="str">
+        <f>LEFT(Full!E15,(FIND(";",Full!E15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y13" s="112" t="str">
+        <f>LEFT(Full!D15,(FIND(";",Full!D15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Z13" s="129" t="str">
+        <f>LEFT(Full!C15,(FIND(";",Full!C15,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA13" s="142" t="str">
+        <f>LEFT(Full!B15,(FIND(";",Full!B15,1)-1))</f>
+        <v>SCAN_CLK</v>
+      </c>
+      <c r="AD13" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE13" s="22">
+        <f>(2*AE8+AE8*(AE9-1))</f>
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="99">
+        <v>6</v>
+      </c>
+      <c r="B14" s="104" t="str">
+        <f>LEFT(Full!AA16,(FIND(";",Full!AA16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C14" s="104" t="str">
+        <f>LEFT(Full!Z16,(FIND(";",Full!Z16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D14" s="104" t="str">
+        <f>LEFT(Full!Y16,(FIND(";",Full!Y16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E14" s="104" t="str">
+        <f>LEFT(Full!X16,(FIND(";",Full!X16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F14" s="104" t="str">
+        <f>LEFT(Full!W16,(FIND(";",Full!W16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G14" s="112" t="str">
+        <f>LEFT(Full!V16,(FIND(";",Full!V16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H14" s="112" t="str">
+        <f>LEFT(Full!U16,(FIND(";",Full!U16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I14" s="104" t="str">
+        <f>LEFT(Full!T16,(FIND(";",Full!T16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J14" s="104" t="str">
+        <f>LEFT(Full!S16,(FIND(";",Full!S16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K14" s="104" t="str">
+        <f>LEFT(Full!R16,(FIND(";",Full!R16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L14" s="104" t="str">
+        <f>LEFT(Full!Q16,(FIND(";",Full!Q16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M14" s="177" t="str">
+        <f>LEFT(Full!P16,(FIND(";",Full!P16,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="N14" s="177" t="str">
+        <f>LEFT(Full!O16,(FIND(";",Full!O16,1)-1))</f>
+        <v>VDD_BM0</v>
+      </c>
+      <c r="O14" s="136" t="str">
+        <f>LEFT(Full!N16,(FIND(";",Full!N16,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="P14" s="136" t="str">
+        <f>LEFT(Full!M16,(FIND(";",Full!M16,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Q14" s="136" t="str">
+        <f>LEFT(Full!L16,(FIND(";",Full!L16,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R14" s="136" t="str">
+        <f>LEFT(Full!K16,(FIND(";",Full!K16,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S14" s="112" t="str">
+        <f>LEFT(Full!J16,(FIND(";",Full!J16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T14" s="112" t="str">
+        <f>LEFT(Full!I16,(FIND(";",Full!I16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U14" s="104" t="str">
+        <f>LEFT(Full!H16,(FIND(";",Full!H16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V14" s="104" t="str">
+        <f>LEFT(Full!G16,(FIND(";",Full!G16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W14" s="112" t="str">
+        <f>LEFT(Full!F16,(FIND(";",Full!F16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X14" s="112" t="str">
+        <f>LEFT(Full!E16,(FIND(";",Full!E16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y14" s="104" t="str">
+        <f>LEFT(Full!D16,(FIND(";",Full!D16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Z14" s="117" t="str">
+        <f>LEFT(Full!C16,(FIND(";",Full!C16,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA14" s="142" t="str">
+        <f>LEFT(Full!B16,(FIND(";",Full!B16,1)-1))</f>
+        <v>SCAN_OUT</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="99">
+        <v>7</v>
+      </c>
+      <c r="B15" s="125" t="str">
+        <f>LEFT(Full!AA17,(FIND(";",Full!AA17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C15" s="140" t="str">
+        <f>LEFT(Full!Z17,(FIND(";",Full!Z17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D15" s="140" t="str">
+        <f>LEFT(Full!Y17,(FIND(";",Full!Y17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E15" s="127" t="str">
+        <f>LEFT(Full!X17,(FIND(";",Full!X17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F15" s="125" t="str">
+        <f>LEFT(Full!W17,(FIND(";",Full!W17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G15" s="128" t="str">
+        <f>LEFT(Full!V17,(FIND(";",Full!V17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H15" s="128" t="str">
+        <f>LEFT(Full!U17,(FIND(";",Full!U17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I15" s="124" t="str">
+        <f>LEFT(Full!T17,(FIND(";",Full!T17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J15" s="124" t="str">
+        <f>LEFT(Full!S17,(FIND(";",Full!S17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K15" s="124" t="str">
+        <f>LEFT(Full!R17,(FIND(";",Full!R17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L15" s="116" t="str">
+        <f>LEFT(Full!Q17,(FIND(";",Full!Q17,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="M15" s="116" t="str">
+        <f>LEFT(Full!P17,(FIND(";",Full!P17,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="N15" s="116" t="str">
+        <f>LEFT(Full!O17,(FIND(";",Full!O17,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="O15" s="139" t="str">
+        <f>LEFT(Full!N17,(FIND(";",Full!N17,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="P15" s="139" t="str">
+        <f>LEFT(Full!M17,(FIND(";",Full!M17,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Q15" s="139" t="str">
+        <f>LEFT(Full!L17,(FIND(";",Full!L17,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R15" s="139" t="str">
+        <f>LEFT(Full!K17,(FIND(";",Full!K17,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S15" s="112" t="str">
+        <f>LEFT(Full!J17,(FIND(";",Full!J17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T15" s="112" t="str">
+        <f>LEFT(Full!I17,(FIND(";",Full!I17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U15" s="104" t="str">
+        <f>LEFT(Full!H17,(FIND(";",Full!H17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V15" s="104" t="str">
+        <f>LEFT(Full!G17,(FIND(";",Full!G17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W15" s="112" t="str">
+        <f>LEFT(Full!F17,(FIND(";",Full!F17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X15" s="112" t="str">
+        <f>LEFT(Full!E17,(FIND(";",Full!E17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y15" s="104" t="str">
+        <f>LEFT(Full!D17,(FIND(";",Full!D17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Z15" s="104" t="str">
+        <f>LEFT(Full!C17,(FIND(";",Full!C17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA15" s="180" t="str">
+        <f>LEFT(Full!B17,(FIND(";",Full!B17,1)-1))</f>
+        <v>VSS</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="99">
+        <v>8</v>
+      </c>
+      <c r="B16" s="142" t="str">
+        <f>LEFT(Full!AA18,(FIND(";",Full!AA18,1)-1))</f>
+        <v>LINK_BM_TX_1_P</v>
+      </c>
+      <c r="C16" s="153" t="str">
+        <f>LEFT(Full!Z18,(FIND(";",Full!Z18,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="D16" s="154" t="str">
+        <f>LEFT(Full!Y18,(FIND(";",Full!Y18,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="E16" s="104" t="str">
+        <f>LEFT(Full!X18,(FIND(";",Full!X18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F16" s="104" t="str">
+        <f>LEFT(Full!W18,(FIND(";",Full!W18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G16" s="104" t="str">
+        <f>LEFT(Full!V18,(FIND(";",Full!V18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H16" s="104" t="str">
+        <f>LEFT(Full!U18,(FIND(";",Full!U18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I16" s="138" t="str">
+        <f>LEFT(Full!T18,(FIND(";",Full!T18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J16" s="138" t="str">
+        <f>LEFT(Full!S18,(FIND(";",Full!S18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K16" s="139" t="str">
+        <f>LEFT(Full!R18,(FIND(";",Full!R18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="L16" s="139" t="str">
+        <f>LEFT(Full!Q18,(FIND(";",Full!Q18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="M16" s="112" t="str">
+        <f>LEFT(Full!P18,(FIND(";",Full!P18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N16" s="112" t="str">
+        <f>LEFT(Full!O18,(FIND(";",Full!O18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O16" s="104" t="str">
+        <f>LEFT(Full!N18,(FIND(";",Full!N18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P16" s="104" t="str">
+        <f>LEFT(Full!M18,(FIND(";",Full!M18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q16" s="138" t="str">
+        <f>LEFT(Full!L18,(FIND(";",Full!L18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R16" s="138" t="str">
+        <f>LEFT(Full!K18,(FIND(";",Full!K18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S16" s="136" t="str">
+        <f>LEFT(Full!J18,(FIND(";",Full!J18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T16" s="139" t="str">
+        <f>LEFT(Full!I18,(FIND(";",Full!I18,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U16" s="112" t="str">
+        <f>LEFT(Full!H18,(FIND(";",Full!H18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V16" s="112" t="str">
+        <f>LEFT(Full!G18,(FIND(";",Full!G18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W16" s="104" t="str">
+        <f>LEFT(Full!F18,(FIND(";",Full!F18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X16" s="104" t="str">
+        <f>LEFT(Full!E18,(FIND(";",Full!E18,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y16" s="156" t="str">
+        <f>LEFT(Full!D18,(FIND(";",Full!D18,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="Z16" s="156" t="str">
+        <f>LEFT(Full!C18,(FIND(";",Full!C18,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="AA16" s="142" t="str">
+        <f>LEFT(Full!B18,(FIND(";",Full!B18,1)-1))</f>
+        <v>LINK_BM_RX_3_P</v>
+      </c>
+      <c r="AD16" s="134" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE16" s="134">
+        <f>COUNTIF($B$9:$AB$34, AD16)</f>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="99">
+        <v>9</v>
+      </c>
+      <c r="B17" s="142" t="str">
+        <f>LEFT(Full!AA19,(FIND(";",Full!AA19,1)-1))</f>
+        <v>LINK_BM_TX_1_N</v>
+      </c>
+      <c r="C17" s="153" t="str">
+        <f>LEFT(Full!Z19,(FIND(";",Full!Z19,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="D17" s="154" t="str">
+        <f>LEFT(Full!Y19,(FIND(";",Full!Y19,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="E17" s="104" t="str">
+        <f>LEFT(Full!X19,(FIND(";",Full!X19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F17" s="104" t="str">
+        <f>LEFT(Full!W19,(FIND(";",Full!W19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G17" s="104" t="str">
+        <f>LEFT(Full!V19,(FIND(";",Full!V19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H17" s="104" t="str">
+        <f>LEFT(Full!U19,(FIND(";",Full!U19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I17" s="138" t="str">
+        <f>LEFT(Full!T19,(FIND(";",Full!T19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J17" s="138" t="str">
+        <f>LEFT(Full!S19,(FIND(";",Full!S19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K17" s="139" t="str">
+        <f>LEFT(Full!R19,(FIND(";",Full!R19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="L17" s="139" t="str">
+        <f>LEFT(Full!Q19,(FIND(";",Full!Q19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="M17" s="112" t="str">
+        <f>LEFT(Full!P19,(FIND(";",Full!P19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N17" s="112" t="str">
+        <f>LEFT(Full!O19,(FIND(";",Full!O19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O17" s="104" t="str">
+        <f>LEFT(Full!N19,(FIND(";",Full!N19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P17" s="104" t="str">
+        <f>LEFT(Full!M19,(FIND(";",Full!M19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q17" s="138" t="str">
+        <f>LEFT(Full!L19,(FIND(";",Full!L19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R17" s="138" t="str">
+        <f>LEFT(Full!K19,(FIND(";",Full!K19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S17" s="139" t="str">
+        <f>LEFT(Full!J19,(FIND(";",Full!J19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T17" s="139" t="str">
+        <f>LEFT(Full!I19,(FIND(";",Full!I19,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U17" s="112" t="str">
+        <f>LEFT(Full!H19,(FIND(";",Full!H19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V17" s="112" t="str">
+        <f>LEFT(Full!G19,(FIND(";",Full!G19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W17" s="104" t="str">
+        <f>LEFT(Full!F19,(FIND(";",Full!F19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X17" s="104" t="str">
+        <f>LEFT(Full!E19,(FIND(";",Full!E19,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y17" s="156" t="str">
+        <f>LEFT(Full!D19,(FIND(";",Full!D19,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="Z17" s="156" t="str">
+        <f>LEFT(Full!C19,(FIND(";",Full!C19,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="AA17" s="142" t="str">
+        <f>LEFT(Full!B19,(FIND(";",Full!B19,1)-1))</f>
+        <v>LINK_BM_RX_3_N</v>
+      </c>
+      <c r="AD17" s="135" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE17" s="135">
+        <f>COUNTIF($B$9:$AB$34, AD17)</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="99">
+        <v>10</v>
+      </c>
+      <c r="B18" s="104" t="str">
+        <f>LEFT(Full!AA20,(FIND(";",Full!AA20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C18" s="116" t="str">
+        <f>LEFT(Full!Z20,(FIND(";",Full!Z20,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="D18" s="116" t="str">
+        <f>LEFT(Full!Y20,(FIND(";",Full!Y20,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="E18" s="116" t="str">
+        <f>LEFT(Full!X20,(FIND(";",Full!X20,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="F18" s="104" t="str">
+        <f>LEFT(Full!W20,(FIND(";",Full!W20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G18" s="112" t="str">
+        <f>LEFT(Full!V20,(FIND(";",Full!V20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H18" s="112" t="str">
+        <f>LEFT(Full!U20,(FIND(";",Full!U20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I18" s="104" t="str">
+        <f>LEFT(Full!T20,(FIND(";",Full!T20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J18" s="104" t="str">
+        <f>LEFT(Full!S20,(FIND(";",Full!S20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K18" s="103" t="str">
+        <f>LEFT(Full!R20,(FIND(";",Full!R20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L18" s="103" t="str">
+        <f>LEFT(Full!Q20,(FIND(";",Full!Q20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M18" s="102" t="str">
+        <f>LEFT(Full!P20,(FIND(";",Full!P20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N18" s="102" t="str">
+        <f>LEFT(Full!O20,(FIND(";",Full!O20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O18" s="160" t="str">
+        <f>LEFT(Full!N20,(FIND(";",Full!N20,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="P18" s="160" t="str">
+        <f>LEFT(Full!M20,(FIND(";",Full!M20,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="Q18" s="161" t="str">
+        <f>LEFT(Full!L20,(FIND(";",Full!L20,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="R18" s="161" t="str">
+        <f>LEFT(Full!K20,(FIND(";",Full!K20,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="S18" s="112" t="str">
+        <f>LEFT(Full!J20,(FIND(";",Full!J20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T18" s="112" t="str">
+        <f>LEFT(Full!I20,(FIND(";",Full!I20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U18" s="104" t="str">
+        <f>LEFT(Full!H20,(FIND(";",Full!H20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V18" s="104" t="str">
+        <f>LEFT(Full!G20,(FIND(";",Full!G20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W18" s="104" t="str">
+        <f>LEFT(Full!F20,(FIND(";",Full!F20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X18" s="57" t="str">
+        <f>LEFT(Full!E20,(FIND(";",Full!E20,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Y18" s="57" t="str">
+        <f>LEFT(Full!D20,(FIND(";",Full!D20,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Z18" s="57" t="str">
+        <f>LEFT(Full!C20,(FIND(";",Full!C20,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="AA18" s="104" t="str">
+        <f>LEFT(Full!B20,(FIND(";",Full!B20,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AD18" s="179" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE18" s="179">
+        <f>COUNTIF($B$9:$AB$34, AD18)</f>
+        <v>16</v>
+      </c>
+      <c r="AG18" s="173" t="s">
+        <v>130</v>
+      </c>
+      <c r="AH18" s="173">
+        <v>8</v>
+      </c>
+      <c r="AI18" s="167" t="s">
+        <v>131</v>
+      </c>
+      <c r="AJ18" s="167">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="99">
+        <v>11</v>
+      </c>
+      <c r="B19" s="142" t="str">
+        <f>LEFT(Full!AA21,(FIND(";",Full!AA21,1)-1))</f>
+        <v>LINK_BM_RX_1_P</v>
+      </c>
+      <c r="C19" s="153" t="str">
+        <f>LEFT(Full!Z21,(FIND(";",Full!Z21,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="D19" s="153" t="str">
+        <f>LEFT(Full!Y21,(FIND(";",Full!Y21,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="E19" s="125" t="str">
+        <f>LEFT(Full!X21,(FIND(";",Full!X21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F19" s="104" t="str">
+        <f>LEFT(Full!W21,(FIND(";",Full!W21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G19" s="112" t="str">
+        <f>LEFT(Full!V21,(FIND(";",Full!V21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H19" s="112" t="str">
+        <f>LEFT(Full!U21,(FIND(";",Full!U21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I19" s="104" t="str">
+        <f>LEFT(Full!T21,(FIND(";",Full!T21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J19" s="104" t="str">
+        <f>LEFT(Full!S21,(FIND(";",Full!S21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K19" s="103" t="str">
+        <f>LEFT(Full!R21,(FIND(";",Full!R21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L19" s="103" t="str">
+        <f>LEFT(Full!Q21,(FIND(";",Full!Q21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M19" s="104" t="str">
+        <f>LEFT(Full!P21,(FIND(";",Full!P21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N19" s="104" t="str">
+        <f>LEFT(Full!O21,(FIND(";",Full!O21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O19" s="160" t="str">
+        <f>LEFT(Full!N21,(FIND(";",Full!N21,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="P19" s="160" t="str">
+        <f>LEFT(Full!M21,(FIND(";",Full!M21,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="Q19" s="161" t="str">
+        <f>LEFT(Full!L21,(FIND(";",Full!L21,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="R19" s="161" t="str">
+        <f>LEFT(Full!K21,(FIND(";",Full!K21,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="S19" s="112" t="str">
+        <f>LEFT(Full!J21,(FIND(";",Full!J21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T19" s="112" t="str">
+        <f>LEFT(Full!I21,(FIND(";",Full!I21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U19" s="104" t="str">
+        <f>LEFT(Full!H21,(FIND(";",Full!H21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V19" s="104" t="str">
+        <f>LEFT(Full!G21,(FIND(";",Full!G21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W19" s="104" t="str">
+        <f>LEFT(Full!F21,(FIND(";",Full!F21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X19" s="104" t="str">
+        <f>LEFT(Full!E21,(FIND(";",Full!E21,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y19" s="156" t="str">
+        <f>LEFT(Full!D21,(FIND(";",Full!D21,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="Z19" s="156" t="str">
+        <f>LEFT(Full!C21,(FIND(";",Full!C21,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="AA19" s="142" t="str">
+        <f>LEFT(Full!B21,(FIND(";",Full!B21,1)-1))</f>
+        <v>LINK_BM_TX_3_P</v>
+      </c>
+      <c r="AD19" s="164" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE19" s="164">
+        <f>COUNTIF($B$9:$AB$34, AD19)</f>
+        <v>32</v>
+      </c>
+      <c r="AG19" s="176" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH19" s="176">
+        <v>8</v>
+      </c>
+      <c r="AI19" s="155" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ19" s="155">
+        <v>8</v>
+      </c>
+      <c r="AK19" s="159" t="s">
+        <v>129</v>
+      </c>
+      <c r="AL19" s="159">
+        <v>8</v>
+      </c>
+      <c r="AM19" s="157" t="s">
+        <v>128</v>
+      </c>
+      <c r="AN19" s="157">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="99">
+        <v>12</v>
+      </c>
+      <c r="B20" s="142" t="str">
+        <f>LEFT(Full!AA22,(FIND(";",Full!AA22,1)-1))</f>
+        <v>LINK_BM_RX_1_N</v>
+      </c>
+      <c r="C20" s="153" t="str">
+        <f>LEFT(Full!Z22,(FIND(";",Full!Z22,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="D20" s="153" t="str">
+        <f>LEFT(Full!Y22,(FIND(";",Full!Y22,1)-1))</f>
+        <v>VDD_BM1</v>
+      </c>
+      <c r="E20" s="124" t="str">
+        <f>LEFT(Full!X22,(FIND(";",Full!X22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F20" s="104" t="str">
+        <f>LEFT(Full!W22,(FIND(";",Full!W22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G20" s="136" t="str">
+        <f>LEFT(Full!V22,(FIND(";",Full!V22,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="H20" s="136" t="str">
+        <f>LEFT(Full!U22,(FIND(";",Full!U22,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="I20" s="137" t="str">
+        <f>LEFT(Full!T22,(FIND(";",Full!T22,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J20" s="138" t="str">
+        <f>LEFT(Full!S22,(FIND(";",Full!S22,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K20" s="162" t="str">
+        <f>LEFT(Full!R22,(FIND(";",Full!R22,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="L20" s="161" t="str">
+        <f>LEFT(Full!Q22,(FIND(";",Full!Q22,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="M20" s="163" t="str">
+        <f>LEFT(Full!P22,(FIND(";",Full!P22,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="N20" s="160" t="str">
+        <f>LEFT(Full!O22,(FIND(";",Full!O22,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="O20" s="104" t="str">
+        <f>LEFT(Full!N22,(FIND(";",Full!N22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P20" s="104" t="str">
+        <f>LEFT(Full!M22,(FIND(";",Full!M22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q20" s="112" t="str">
+        <f>LEFT(Full!L22,(FIND(";",Full!L22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R20" s="112" t="str">
+        <f>LEFT(Full!K22,(FIND(";",Full!K22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S20" s="104" t="str">
+        <f>LEFT(Full!J22,(FIND(";",Full!J22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T20" s="104" t="str">
+        <f>LEFT(Full!I22,(FIND(";",Full!I22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U20" s="112" t="str">
+        <f>LEFT(Full!H22,(FIND(";",Full!H22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V20" s="112" t="str">
+        <f>LEFT(Full!G22,(FIND(";",Full!G22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W20" s="104" t="str">
+        <f>LEFT(Full!F22,(FIND(";",Full!F22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X20" s="104" t="str">
+        <f>LEFT(Full!E22,(FIND(";",Full!E22,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y20" s="156" t="str">
+        <f>LEFT(Full!D22,(FIND(";",Full!D22,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="Z20" s="156" t="str">
+        <f>LEFT(Full!C22,(FIND(";",Full!C22,1)-1))</f>
+        <v>VDD_BM3</v>
+      </c>
+      <c r="AA20" s="142" t="str">
+        <f>LEFT(Full!B22,(FIND(";",Full!B22,1)-1))</f>
+        <v>LINK_BM_TX_3_N</v>
+      </c>
+      <c r="AD20" s="166" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE20" s="166">
+        <f>COUNTIF($B$9:$AB$34, AD20)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="99">
+        <v>13</v>
+      </c>
+      <c r="B21" s="104" t="str">
+        <f>LEFT(Full!AA23,(FIND(";",Full!AA23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C21" s="116" t="str">
+        <f>LEFT(Full!Z23,(FIND(";",Full!Z23,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="D21" s="116" t="str">
+        <f>LEFT(Full!Y23,(FIND(";",Full!Y23,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="E21" s="116" t="str">
+        <f>LEFT(Full!X23,(FIND(";",Full!X23,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="F21" s="104" t="str">
+        <f>LEFT(Full!W23,(FIND(";",Full!W23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G21" s="139" t="str">
+        <f>LEFT(Full!V23,(FIND(";",Full!V23,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="H21" s="139" t="str">
+        <f>LEFT(Full!U23,(FIND(";",Full!U23,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="I21" s="138" t="str">
+        <f>LEFT(Full!T23,(FIND(";",Full!T23,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J21" s="138" t="str">
+        <f>LEFT(Full!S23,(FIND(";",Full!S23,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K21" s="162" t="str">
+        <f>LEFT(Full!R23,(FIND(";",Full!R23,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="L21" s="161" t="str">
+        <f>LEFT(Full!Q23,(FIND(";",Full!Q23,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="M21" s="160" t="str">
+        <f>LEFT(Full!P23,(FIND(";",Full!P23,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="N21" s="160" t="str">
+        <f>LEFT(Full!O23,(FIND(";",Full!O23,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="O21" s="104" t="str">
+        <f>LEFT(Full!N23,(FIND(";",Full!N23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P21" s="104" t="str">
+        <f>LEFT(Full!M23,(FIND(";",Full!M23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q21" s="112" t="str">
+        <f>LEFT(Full!L23,(FIND(";",Full!L23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R21" s="112" t="str">
+        <f>LEFT(Full!K23,(FIND(";",Full!K23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S21" s="104" t="str">
+        <f>LEFT(Full!J23,(FIND(";",Full!J23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T21" s="104" t="str">
+        <f>LEFT(Full!I23,(FIND(";",Full!I23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U21" s="112" t="str">
+        <f>LEFT(Full!H23,(FIND(";",Full!H23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V21" s="112" t="str">
+        <f>LEFT(Full!G23,(FIND(";",Full!G23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W21" s="104" t="str">
+        <f>LEFT(Full!F23,(FIND(";",Full!F23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X21" s="116" t="str">
+        <f>LEFT(Full!E23,(FIND(";",Full!E23,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Y21" s="116" t="str">
+        <f>LEFT(Full!D23,(FIND(";",Full!D23,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Z21" s="116" t="str">
+        <f>LEFT(Full!C23,(FIND(";",Full!C23,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="AA21" s="104" t="str">
+        <f>LEFT(Full!B23,(FIND(";",Full!B23,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AD21" s="148" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE21" s="148">
+        <f>COUNTIF($B$9:$AB$34, AD21)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="99">
+        <v>14</v>
+      </c>
+      <c r="B22" s="142" t="str">
+        <f>LEFT(Full!AA24,(FIND(";",Full!AA24,1)-1))</f>
+        <v>LINK_CM_TX_0_P</v>
+      </c>
+      <c r="C22" s="174" t="str">
+        <f>LEFT(Full!Z24,(FIND(";",Full!Z24,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="D22" s="174" t="str">
+        <f>LEFT(Full!Y24,(FIND(";",Full!Y24,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="E22" s="125" t="str">
+        <f>LEFT(Full!X24,(FIND(";",Full!X24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F22" s="104" t="str">
+        <f>LEFT(Full!W24,(FIND(";",Full!W24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G22" s="112" t="str">
+        <f>LEFT(Full!V24,(FIND(";",Full!V24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H22" s="112" t="str">
+        <f>LEFT(Full!U24,(FIND(";",Full!U24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I22" s="104" t="str">
+        <f>LEFT(Full!T24,(FIND(";",Full!T24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J22" s="104" t="str">
+        <f>LEFT(Full!S24,(FIND(";",Full!S24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K22" s="160" t="str">
+        <f>LEFT(Full!R24,(FIND(";",Full!R24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="L22" s="160" t="str">
+        <f>LEFT(Full!Q24,(FIND(";",Full!Q24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="M22" s="161" t="str">
+        <f>LEFT(Full!P24,(FIND(";",Full!P24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="N22" s="161" t="str">
+        <f>LEFT(Full!O24,(FIND(";",Full!O24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="O22" s="163" t="str">
+        <f>LEFT(Full!N24,(FIND(";",Full!N24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="P22" s="160" t="str">
+        <f>LEFT(Full!M24,(FIND(";",Full!M24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="Q22" s="161" t="str">
+        <f>LEFT(Full!L24,(FIND(";",Full!L24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="R22" s="161" t="str">
+        <f>LEFT(Full!K24,(FIND(";",Full!K24,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="S22" s="141" t="str">
+        <f>LEFT(Full!J24,(FIND(";",Full!J24,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T22" s="141" t="str">
+        <f>LEFT(Full!I24,(FIND(";",Full!I24,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U22" s="139" t="str">
+        <f>LEFT(Full!H24,(FIND(";",Full!H24,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="V22" s="139" t="str">
+        <f>LEFT(Full!G24,(FIND(";",Full!G24,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="W22" s="104" t="str">
+        <f>LEFT(Full!F24,(FIND(";",Full!F24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X22" s="104" t="str">
+        <f>LEFT(Full!E24,(FIND(";",Full!E24,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y22" s="169" t="str">
+        <f>LEFT(Full!D24,(FIND(";",Full!D24,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="Z22" s="170" t="str">
+        <f>LEFT(Full!C24,(FIND(";",Full!C24,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="AA22" s="142" t="str">
+        <f>LEFT(Full!B24,(FIND(";",Full!B24,1)-1))</f>
+        <v>LINK_CM_RX_1_P</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="99">
+        <v>15</v>
+      </c>
+      <c r="B23" s="142" t="str">
+        <f>LEFT(Full!AA25,(FIND(";",Full!AA25,1)-1))</f>
+        <v>LINK_CM_TX_0_N</v>
+      </c>
+      <c r="C23" s="174" t="str">
+        <f>LEFT(Full!Z25,(FIND(";",Full!Z25,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="D23" s="174" t="str">
+        <f>LEFT(Full!Y25,(FIND(";",Full!Y25,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="E23" s="104" t="str">
+        <f>LEFT(Full!X25,(FIND(";",Full!X25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F23" s="104" t="str">
+        <f>LEFT(Full!W25,(FIND(";",Full!W25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G23" s="112" t="str">
+        <f>LEFT(Full!V25,(FIND(";",Full!V25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H23" s="112" t="str">
+        <f>LEFT(Full!U25,(FIND(";",Full!U25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I23" s="104" t="str">
+        <f>LEFT(Full!T25,(FIND(";",Full!T25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J23" s="104" t="str">
+        <f>LEFT(Full!S25,(FIND(";",Full!S25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K23" s="160" t="str">
+        <f>LEFT(Full!R25,(FIND(";",Full!R25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="L23" s="160" t="str">
+        <f>LEFT(Full!Q25,(FIND(";",Full!Q25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="M23" s="161" t="str">
+        <f>LEFT(Full!P25,(FIND(";",Full!P25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="N23" s="161" t="str">
+        <f>LEFT(Full!O25,(FIND(";",Full!O25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="O23" s="160" t="str">
+        <f>LEFT(Full!N25,(FIND(";",Full!N25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="P23" s="160" t="str">
+        <f>LEFT(Full!M25,(FIND(";",Full!M25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="Q23" s="161" t="str">
+        <f>LEFT(Full!L25,(FIND(";",Full!L25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="R23" s="161" t="str">
+        <f>LEFT(Full!K25,(FIND(";",Full!K25,1)-1))</f>
+        <v>VDDA</v>
+      </c>
+      <c r="S23" s="141" t="str">
+        <f>LEFT(Full!J25,(FIND(";",Full!J25,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T23" s="141" t="str">
+        <f>LEFT(Full!I25,(FIND(";",Full!I25,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U23" s="139" t="str">
+        <f>LEFT(Full!H25,(FIND(";",Full!H25,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="V23" s="139" t="str">
+        <f>LEFT(Full!G25,(FIND(";",Full!G25,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="W23" s="104" t="str">
+        <f>LEFT(Full!F25,(FIND(";",Full!F25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X23" s="104" t="str">
+        <f>LEFT(Full!E25,(FIND(";",Full!E25,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y23" s="171" t="str">
+        <f>LEFT(Full!D25,(FIND(";",Full!D25,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="Z23" s="172" t="str">
+        <f>LEFT(Full!C25,(FIND(";",Full!C25,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="AA23" s="142" t="str">
+        <f>LEFT(Full!B25,(FIND(";",Full!B25,1)-1))</f>
+        <v>LINK_CM_RX_1_N</v>
+      </c>
+      <c r="AD23" s="165" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE23" s="165">
+        <f>COUNTIF($B$9:$AB$34, AD23)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="99">
+        <v>16</v>
+      </c>
+      <c r="B24" s="104" t="str">
+        <f>LEFT(Full!AA26,(FIND(";",Full!AA26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C24" s="116" t="str">
+        <f>LEFT(Full!Z26,(FIND(";",Full!Z26,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="D24" s="116" t="str">
+        <f>LEFT(Full!Y26,(FIND(";",Full!Y26,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="E24" s="116" t="str">
+        <f>LEFT(Full!X26,(FIND(";",Full!X26,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="F24" s="104" t="str">
+        <f>LEFT(Full!W26,(FIND(";",Full!W26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G24" s="139" t="str">
+        <f>LEFT(Full!V26,(FIND(";",Full!V26,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="H24" s="139" t="str">
+        <f>LEFT(Full!U26,(FIND(";",Full!U26,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="I24" s="138" t="str">
+        <f>LEFT(Full!T26,(FIND(";",Full!T26,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J24" s="138" t="str">
+        <f>LEFT(Full!S26,(FIND(";",Full!S26,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K24" s="104" t="str">
+        <f>LEFT(Full!R26,(FIND(";",Full!R26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L24" s="104" t="str">
+        <f>LEFT(Full!Q26,(FIND(";",Full!Q26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M24" s="112" t="str">
+        <f>LEFT(Full!P26,(FIND(";",Full!P26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N24" s="112" t="str">
+        <f>LEFT(Full!O26,(FIND(";",Full!O26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O24" s="104" t="str">
+        <f>LEFT(Full!N26,(FIND(";",Full!N26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P24" s="104" t="str">
+        <f>LEFT(Full!M26,(FIND(";",Full!M26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q24" s="112" t="str">
+        <f>LEFT(Full!L26,(FIND(";",Full!L26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R24" s="112" t="str">
+        <f>LEFT(Full!K26,(FIND(";",Full!K26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S24" s="104" t="str">
+        <f>LEFT(Full!J26,(FIND(";",Full!J26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T24" s="104" t="str">
+        <f>LEFT(Full!I26,(FIND(";",Full!I26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U24" s="112" t="str">
+        <f>LEFT(Full!H26,(FIND(";",Full!H26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V24" s="112" t="str">
+        <f>LEFT(Full!G26,(FIND(";",Full!G26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W24" s="104" t="str">
+        <f>LEFT(Full!F26,(FIND(";",Full!F26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X24" s="116" t="str">
+        <f>LEFT(Full!E26,(FIND(";",Full!E26,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Y24" s="116" t="str">
+        <f>LEFT(Full!D26,(FIND(";",Full!D26,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Z24" s="116" t="str">
+        <f>LEFT(Full!C26,(FIND(";",Full!C26,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="AA24" s="104" t="str">
+        <f>LEFT(Full!B26,(FIND(";",Full!B26,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AD24" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE24" s="22">
+        <f>COUNTIF($B$9:$AB$34, AD24)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="99">
+        <v>17</v>
+      </c>
+      <c r="B25" s="142" t="str">
+        <f>LEFT(Full!AA27,(FIND(";",Full!AA27,1)-1))</f>
+        <v>LINK_CM_RX_0_P</v>
+      </c>
+      <c r="C25" s="174" t="str">
+        <f>LEFT(Full!Z27,(FIND(";",Full!Z27,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="D25" s="174" t="str">
+        <f>LEFT(Full!Y27,(FIND(";",Full!Y27,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="E25" s="104" t="str">
+        <f>LEFT(Full!X27,(FIND(";",Full!X27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F25" s="117" t="str">
+        <f>LEFT(Full!W27,(FIND(";",Full!W27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G25" s="139" t="str">
+        <f>LEFT(Full!V27,(FIND(";",Full!V27,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="H25" s="139" t="str">
+        <f>LEFT(Full!U27,(FIND(";",Full!U27,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="I25" s="138" t="str">
+        <f>LEFT(Full!T27,(FIND(";",Full!T27,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J25" s="138" t="str">
+        <f>LEFT(Full!S27,(FIND(";",Full!S27,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K25" s="104" t="str">
+        <f>LEFT(Full!R27,(FIND(";",Full!R27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L25" s="104" t="str">
+        <f>LEFT(Full!Q27,(FIND(";",Full!Q27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="M25" s="112" t="str">
+        <f>LEFT(Full!P27,(FIND(";",Full!P27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N25" s="112" t="str">
+        <f>LEFT(Full!O27,(FIND(";",Full!O27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O25" s="104" t="str">
+        <f>LEFT(Full!N27,(FIND(";",Full!N27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P25" s="104" t="str">
+        <f>LEFT(Full!M27,(FIND(";",Full!M27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q25" s="112" t="str">
+        <f>LEFT(Full!L27,(FIND(";",Full!L27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R25" s="112" t="str">
+        <f>LEFT(Full!K27,(FIND(";",Full!K27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S25" s="104" t="str">
+        <f>LEFT(Full!J27,(FIND(";",Full!J27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T25" s="104" t="str">
+        <f>LEFT(Full!I27,(FIND(";",Full!I27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U25" s="112" t="str">
+        <f>LEFT(Full!H27,(FIND(";",Full!H27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V25" s="112" t="str">
+        <f>LEFT(Full!G27,(FIND(";",Full!G27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W25" s="104" t="str">
+        <f>LEFT(Full!F27,(FIND(";",Full!F27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X25" s="104" t="str">
+        <f>LEFT(Full!E27,(FIND(";",Full!E27,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y25" s="168" t="str">
+        <f>LEFT(Full!D27,(FIND(";",Full!D27,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="Z25" s="168" t="str">
+        <f>LEFT(Full!C27,(FIND(";",Full!C27,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="AA25" s="142" t="str">
+        <f>LEFT(Full!B27,(FIND(";",Full!B27,1)-1))</f>
+        <v>LINK_CM_TX_1_P</v>
+      </c>
+      <c r="AD25" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE25" s="22">
+        <f>AE9*AE10-AE23-AE24</f>
+        <v>635</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="99">
+        <v>18</v>
+      </c>
+      <c r="B26" s="142" t="str">
+        <f>LEFT(Full!AA28,(FIND(";",Full!AA28,1)-1))</f>
+        <v>LINK_CM_RX_0_N</v>
+      </c>
+      <c r="C26" s="174" t="str">
+        <f>LEFT(Full!Z28,(FIND(";",Full!Z28,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="D26" s="174" t="str">
+        <f>LEFT(Full!Y28,(FIND(";",Full!Y28,1)-1))</f>
+        <v>VDD_LINK_CM0</v>
+      </c>
+      <c r="E26" s="104" t="str">
+        <f>LEFT(Full!X28,(FIND(";",Full!X28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F26" s="104" t="str">
+        <f>LEFT(Full!W28,(FIND(";",Full!W28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G26" s="112" t="str">
+        <f>LEFT(Full!V28,(FIND(";",Full!V28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H26" s="112" t="str">
+        <f>LEFT(Full!U28,(FIND(";",Full!U28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I26" s="104" t="str">
+        <f>LEFT(Full!T28,(FIND(";",Full!T28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J26" s="104" t="str">
+        <f>LEFT(Full!S28,(FIND(";",Full!S28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K26" s="137" t="str">
+        <f>LEFT(Full!R28,(FIND(";",Full!R28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="L26" s="137" t="str">
+        <f>LEFT(Full!Q28,(FIND(";",Full!Q28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="M26" s="136" t="str">
+        <f>LEFT(Full!P28,(FIND(";",Full!P28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="N26" s="136" t="str">
+        <f>LEFT(Full!O28,(FIND(";",Full!O28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="O26" s="137" t="str">
+        <f>LEFT(Full!N28,(FIND(";",Full!N28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="P26" s="137" t="str">
+        <f>LEFT(Full!M28,(FIND(";",Full!M28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Q26" s="136" t="str">
+        <f>LEFT(Full!L28,(FIND(";",Full!L28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R26" s="136" t="str">
+        <f>LEFT(Full!K28,(FIND(";",Full!K28,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S26" s="112" t="str">
+        <f>LEFT(Full!J28,(FIND(";",Full!J28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T26" s="112" t="str">
+        <f>LEFT(Full!I28,(FIND(";",Full!I28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U26" s="104" t="str">
+        <f>LEFT(Full!H28,(FIND(";",Full!H28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V26" s="104" t="str">
+        <f>LEFT(Full!G28,(FIND(";",Full!G28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W26" s="104" t="str">
+        <f>LEFT(Full!F28,(FIND(";",Full!F28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X26" s="104" t="str">
+        <f>LEFT(Full!E28,(FIND(";",Full!E28,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y26" s="168" t="str">
+        <f>LEFT(Full!D28,(FIND(";",Full!D28,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="Z26" s="168" t="str">
+        <f>LEFT(Full!C28,(FIND(";",Full!C28,1)-1))</f>
+        <v>VDD_LINK_CM1</v>
+      </c>
+      <c r="AA26" s="142" t="str">
+        <f>LEFT(Full!B28,(FIND(";",Full!B28,1)-1))</f>
+        <v>LINK_CM_TX_1_N</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="99">
+        <v>19</v>
+      </c>
+      <c r="B27" s="104" t="str">
+        <f>LEFT(Full!AA29,(FIND(";",Full!AA29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C27" s="116" t="str">
+        <f>LEFT(Full!Z29,(FIND(";",Full!Z29,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="D27" s="116" t="str">
+        <f>LEFT(Full!Y29,(FIND(";",Full!Y29,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="E27" s="119" t="str">
+        <f>LEFT(Full!X29,(FIND(";",Full!X29,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="F27" s="104" t="str">
+        <f>LEFT(Full!W29,(FIND(";",Full!W29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G27" s="112" t="str">
+        <f>LEFT(Full!V29,(FIND(";",Full!V29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H27" s="112" t="str">
+        <f>LEFT(Full!U29,(FIND(";",Full!U29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I27" s="104" t="str">
+        <f>LEFT(Full!T29,(FIND(";",Full!T29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J27" s="104" t="str">
+        <f>LEFT(Full!S29,(FIND(";",Full!S29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K27" s="138" t="str">
+        <f>LEFT(Full!R29,(FIND(";",Full!R29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="L27" s="138" t="str">
+        <f>LEFT(Full!Q29,(FIND(";",Full!Q29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="M27" s="139" t="str">
+        <f>LEFT(Full!P29,(FIND(";",Full!P29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="N27" s="139" t="str">
+        <f>LEFT(Full!O29,(FIND(";",Full!O29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="O27" s="138" t="str">
+        <f>LEFT(Full!N29,(FIND(";",Full!N29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="P27" s="138" t="str">
+        <f>LEFT(Full!M29,(FIND(";",Full!M29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Q27" s="139" t="str">
+        <f>LEFT(Full!L29,(FIND(";",Full!L29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R27" s="139" t="str">
+        <f>LEFT(Full!K29,(FIND(";",Full!K29,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S27" s="112" t="str">
+        <f>LEFT(Full!J29,(FIND(";",Full!J29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T27" s="112" t="str">
+        <f>LEFT(Full!I29,(FIND(";",Full!I29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U27" s="104" t="str">
+        <f>LEFT(Full!H29,(FIND(";",Full!H29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V27" s="104" t="str">
+        <f>LEFT(Full!G29,(FIND(";",Full!G29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W27" s="104" t="str">
+        <f>LEFT(Full!F29,(FIND(";",Full!F29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X27" s="122" t="str">
+        <f>LEFT(Full!E29,(FIND(";",Full!E29,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Y27" s="116" t="str">
+        <f>LEFT(Full!D29,(FIND(";",Full!D29,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="Z27" s="116" t="str">
+        <f>LEFT(Full!C29,(FIND(";",Full!C29,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="AA27" s="104" t="str">
+        <f>LEFT(Full!B29,(FIND(";",Full!B29,1)-1))</f>
+        <v>VSS</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="99">
+        <v>20</v>
+      </c>
+      <c r="B28" s="142" t="str">
+        <f>LEFT(Full!AA30,(FIND(";",Full!AA30,1)-1))</f>
+        <v>REF_SERDES_CM0_P</v>
+      </c>
+      <c r="C28" s="104" t="str">
+        <f>LEFT(Full!Z30,(FIND(";",Full!Z30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D28" s="104" t="str">
+        <f>LEFT(Full!Y30,(FIND(";",Full!Y30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E28" s="112" t="str">
+        <f>LEFT(Full!X30,(FIND(";",Full!X30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F28" s="112" t="str">
+        <f>LEFT(Full!W30,(FIND(";",Full!W30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G28" s="104" t="str">
+        <f>LEFT(Full!V30,(FIND(";",Full!V30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H28" s="104" t="str">
+        <f>LEFT(Full!U30,(FIND(";",Full!U30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I28" s="138" t="str">
+        <f>LEFT(Full!T30,(FIND(";",Full!T30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J28" s="138" t="str">
+        <f>LEFT(Full!S30,(FIND(";",Full!S30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K28" s="139" t="str">
+        <f>LEFT(Full!R30,(FIND(";",Full!R30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="L28" s="116" t="str">
+        <f>LEFT(Full!Q30,(FIND(";",Full!Q30,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="M28" s="116" t="str">
+        <f>LEFT(Full!P30,(FIND(";",Full!P30,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="N28" s="116" t="str">
+        <f>LEFT(Full!O30,(FIND(";",Full!O30,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="O28" s="104" t="str">
+        <f>LEFT(Full!N30,(FIND(";",Full!N30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P28" s="104" t="str">
+        <f>LEFT(Full!M30,(FIND(";",Full!M30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q28" s="138" t="str">
+        <f>LEFT(Full!L30,(FIND(";",Full!L30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R28" s="138" t="str">
+        <f>LEFT(Full!K30,(FIND(";",Full!K30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S28" s="139" t="str">
+        <f>LEFT(Full!J30,(FIND(";",Full!J30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T28" s="139" t="str">
+        <f>LEFT(Full!I30,(FIND(";",Full!I30,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U28" s="112" t="str">
+        <f>LEFT(Full!H30,(FIND(";",Full!H30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V28" s="112" t="str">
+        <f>LEFT(Full!G30,(FIND(";",Full!G30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W28" s="104" t="str">
+        <f>LEFT(Full!F30,(FIND(";",Full!F30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X28" s="104" t="str">
+        <f>LEFT(Full!E30,(FIND(";",Full!E30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y28" s="112" t="str">
+        <f>LEFT(Full!D30,(FIND(";",Full!D30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Z28" s="112" t="str">
+        <f>LEFT(Full!C30,(FIND(";",Full!C30,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA28" s="142" t="str">
+        <f>LEFT(Full!B30,(FIND(";",Full!B30,1)-1))</f>
+        <v>REF_SERDES_CM1_P</v>
+      </c>
+    </row>
+    <row r="29" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="99">
+        <v>21</v>
+      </c>
+      <c r="B29" s="142" t="str">
+        <f>LEFT(Full!AA31,(FIND(";",Full!AA31,1)-1))</f>
+        <v>REF_SERDES_CM0_N</v>
+      </c>
+      <c r="C29" s="104" t="str">
+        <f>LEFT(Full!Z31,(FIND(";",Full!Z31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D29" s="104" t="str">
+        <f>LEFT(Full!Y31,(FIND(";",Full!Y31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E29" s="112" t="str">
+        <f>LEFT(Full!X31,(FIND(";",Full!X31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F29" s="112" t="str">
+        <f>LEFT(Full!W31,(FIND(";",Full!W31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G29" s="104" t="str">
+        <f>LEFT(Full!V31,(FIND(";",Full!V31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H29" s="104" t="str">
+        <f>LEFT(Full!U31,(FIND(";",Full!U31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I29" s="138" t="str">
+        <f>LEFT(Full!T31,(FIND(";",Full!T31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="J29" s="138" t="str">
+        <f>LEFT(Full!S31,(FIND(";",Full!S31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="K29" s="139" t="str">
+        <f>LEFT(Full!R31,(FIND(";",Full!R31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="L29" s="158" t="str">
+        <f>LEFT(Full!Q31,(FIND(";",Full!Q31,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="M29" s="158" t="str">
+        <f>LEFT(Full!P31,(FIND(";",Full!P31,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="N29" s="104" t="str">
+        <f>LEFT(Full!O31,(FIND(";",Full!O31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O29" s="104" t="str">
+        <f>LEFT(Full!N31,(FIND(";",Full!N31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P29" s="104" t="str">
+        <f>LEFT(Full!M31,(FIND(";",Full!M31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q29" s="138" t="str">
+        <f>LEFT(Full!L31,(FIND(";",Full!L31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="R29" s="138" t="str">
+        <f>LEFT(Full!K31,(FIND(";",Full!K31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="S29" s="139" t="str">
+        <f>LEFT(Full!J31,(FIND(";",Full!J31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="T29" s="139" t="str">
+        <f>LEFT(Full!I31,(FIND(";",Full!I31,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="U29" s="112" t="str">
+        <f>LEFT(Full!H31,(FIND(";",Full!H31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V29" s="112" t="str">
+        <f>LEFT(Full!G31,(FIND(";",Full!G31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W29" s="104" t="str">
+        <f>LEFT(Full!F31,(FIND(";",Full!F31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X29" s="104" t="str">
+        <f>LEFT(Full!E31,(FIND(";",Full!E31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Y29" s="112" t="str">
+        <f>LEFT(Full!D31,(FIND(";",Full!D31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Z29" s="112" t="str">
+        <f>LEFT(Full!C31,(FIND(";",Full!C31,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA29" s="142" t="str">
+        <f>LEFT(Full!B31,(FIND(";",Full!B31,1)-1))</f>
+        <v>REF_SERDES_CM1_N</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="99">
+        <v>22</v>
+      </c>
+      <c r="B30" s="104" t="str">
+        <f>LEFT(Full!AA32,(FIND(";",Full!AA32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C30" s="112" t="str">
+        <f>LEFT(Full!Z32,(FIND(";",Full!Z32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D30" s="112" t="str">
+        <f>LEFT(Full!Y32,(FIND(";",Full!Y32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E30" s="104" t="str">
+        <f>LEFT(Full!X32,(FIND(";",Full!X32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F30" s="104" t="str">
+        <f>LEFT(Full!W32,(FIND(";",Full!W32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G30" s="112" t="str">
+        <f>LEFT(Full!V32,(FIND(";",Full!V32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H30" s="112" t="str">
+        <f>LEFT(Full!U32,(FIND(";",Full!U32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I30" s="113" t="str">
+        <f>LEFT(Full!T32,(FIND(";",Full!T32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J30" s="104" t="str">
+        <f>LEFT(Full!S32,(FIND(";",Full!S32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K30" s="104" t="str">
+        <f>LEFT(Full!R32,(FIND(";",Full!R32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L30" s="158" t="str">
+        <f>LEFT(Full!Q32,(FIND(";",Full!Q32,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="M30" s="158" t="str">
+        <f>LEFT(Full!P32,(FIND(";",Full!P32,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="N30" s="104" t="str">
+        <f>LEFT(Full!O32,(FIND(";",Full!O32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O30" s="104" t="str">
+        <f>LEFT(Full!N32,(FIND(";",Full!N32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P30" s="104" t="str">
+        <f>LEFT(Full!M32,(FIND(";",Full!M32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q30" s="113" t="str">
+        <f>LEFT(Full!L32,(FIND(";",Full!L32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R30" s="104" t="str">
+        <f>LEFT(Full!K32,(FIND(";",Full!K32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S30" s="112" t="str">
+        <f>LEFT(Full!J32,(FIND(";",Full!J32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T30" s="112" t="str">
+        <f>LEFT(Full!I32,(FIND(";",Full!I32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U30" s="104" t="str">
+        <f>LEFT(Full!H32,(FIND(";",Full!H32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V30" s="104" t="str">
+        <f>LEFT(Full!G32,(FIND(";",Full!G32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W30" s="138" t="str">
+        <f>LEFT(Full!F32,(FIND(";",Full!F32,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="X30" s="138" t="str">
+        <f>LEFT(Full!E32,(FIND(";",Full!E32,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Y30" s="139" t="str">
+        <f>LEFT(Full!D32,(FIND(";",Full!D32,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Z30" s="139" t="str">
+        <f>LEFT(Full!C32,(FIND(";",Full!C32,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="AA30" s="104" t="str">
+        <f>LEFT(Full!B32,(FIND(";",Full!B32,1)-1))</f>
+        <v>VSS</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="99">
+        <v>23</v>
+      </c>
+      <c r="B31" s="142" t="str">
+        <f>LEFT(Full!AA33,(FIND(";",Full!AA33,1)-1))</f>
+        <v>REF_DIG_N</v>
+      </c>
+      <c r="C31" s="112" t="str">
+        <f>LEFT(Full!Z33,(FIND(";",Full!Z33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D31" s="112" t="str">
+        <f>LEFT(Full!Y33,(FIND(";",Full!Y33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="E31" s="104" t="str">
+        <f>LEFT(Full!X33,(FIND(";",Full!X33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="F31" s="104" t="str">
+        <f>LEFT(Full!W33,(FIND(";",Full!W33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G31" s="112" t="str">
+        <f>LEFT(Full!V33,(FIND(";",Full!V33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H31" s="112" t="str">
+        <f>LEFT(Full!U33,(FIND(";",Full!U33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I31" s="113" t="str">
+        <f>LEFT(Full!T33,(FIND(";",Full!T33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J31" s="104" t="str">
+        <f>LEFT(Full!S33,(FIND(";",Full!S33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K31" s="104" t="str">
+        <f>LEFT(Full!R33,(FIND(";",Full!R33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L31" s="116" t="str">
+        <f>LEFT(Full!Q33,(FIND(";",Full!Q33,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="M31" s="116" t="str">
+        <f>LEFT(Full!P33,(FIND(";",Full!P33,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="N31" s="116" t="str">
+        <f>LEFT(Full!O33,(FIND(";",Full!O33,1)-1))</f>
+        <v>Inductor</v>
+      </c>
+      <c r="O31" s="104" t="str">
+        <f>LEFT(Full!N33,(FIND(";",Full!N33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P31" s="104" t="str">
+        <f>LEFT(Full!M33,(FIND(";",Full!M33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q31" s="113" t="str">
+        <f>LEFT(Full!L33,(FIND(";",Full!L33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R31" s="104" t="str">
+        <f>LEFT(Full!K33,(FIND(";",Full!K33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S31" s="112" t="str">
+        <f>LEFT(Full!J33,(FIND(";",Full!J33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T31" s="112" t="str">
+        <f>LEFT(Full!I33,(FIND(";",Full!I33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U31" s="104" t="str">
+        <f>LEFT(Full!H33,(FIND(";",Full!H33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V31" s="104" t="str">
+        <f>LEFT(Full!G33,(FIND(";",Full!G33,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W31" s="138" t="str">
+        <f>LEFT(Full!F33,(FIND(";",Full!F33,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="X31" s="138" t="str">
+        <f>LEFT(Full!E33,(FIND(";",Full!E33,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Y31" s="139" t="str">
+        <f>LEFT(Full!D33,(FIND(";",Full!D33,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="Z31" s="139" t="str">
+        <f>LEFT(Full!C33,(FIND(";",Full!C33,1)-1))</f>
+        <v>DVDD</v>
+      </c>
+      <c r="AA31" s="142" t="str">
+        <f>LEFT(Full!B33,(FIND(";",Full!B33,1)-1))</f>
+        <v>REF_LO_N</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="99">
+        <v>24</v>
+      </c>
+      <c r="B32" s="142" t="str">
+        <f>LEFT(Full!AA34,(FIND(";",Full!AA34,1)-1))</f>
+        <v>REF_DIG_P</v>
+      </c>
+      <c r="C32" s="147" t="str">
+        <f>LEFT(Full!Z34,(FIND(";",Full!Z34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="D32" s="147" t="str">
+        <f>LEFT(Full!Y34,(FIND(";",Full!Y34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="E32" s="146" t="str">
+        <f>LEFT(Full!X34,(FIND(";",Full!X34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="F32" s="146" t="str">
+        <f>LEFT(Full!W34,(FIND(";",Full!W34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="G32" s="104" t="str">
+        <f>LEFT(Full!V34,(FIND(";",Full!V34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H32" s="104" t="str">
+        <f>LEFT(Full!U34,(FIND(";",Full!U34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I32" s="112" t="str">
+        <f>LEFT(Full!T34,(FIND(";",Full!T34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J32" s="112" t="str">
+        <f>LEFT(Full!S34,(FIND(";",Full!S34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K32" s="104" t="str">
+        <f>LEFT(Full!R34,(FIND(";",Full!R34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L32" s="158" t="str">
+        <f>LEFT(Full!Q34,(FIND(";",Full!Q34,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="M32" s="158" t="str">
+        <f>LEFT(Full!P34,(FIND(";",Full!P34,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="N32" s="104" t="str">
+        <f>LEFT(Full!O34,(FIND(";",Full!O34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O32" s="104" t="str">
+        <f>LEFT(Full!N34,(FIND(";",Full!N34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P32" s="104" t="str">
+        <f>LEFT(Full!M34,(FIND(";",Full!M34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q32" s="114" t="str">
+        <f>LEFT(Full!L34,(FIND(";",Full!L34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R32" s="112" t="str">
+        <f>LEFT(Full!K34,(FIND(";",Full!K34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S32" s="104" t="str">
+        <f>LEFT(Full!J34,(FIND(";",Full!J34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T32" s="104" t="str">
+        <f>LEFT(Full!I34,(FIND(";",Full!I34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U32" s="112" t="str">
+        <f>LEFT(Full!H34,(FIND(";",Full!H34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V32" s="112" t="str">
+        <f>LEFT(Full!G34,(FIND(";",Full!G34,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W32" s="150" t="str">
+        <f>LEFT(Full!F34,(FIND(";",Full!F34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="X32" s="147" t="str">
+        <f>LEFT(Full!E34,(FIND(";",Full!E34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Y32" s="146" t="str">
+        <f>LEFT(Full!D34,(FIND(";",Full!D34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Z32" s="146" t="str">
+        <f>LEFT(Full!C34,(FIND(";",Full!C34,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="AA32" s="142" t="str">
+        <f>LEFT(Full!B34,(FIND(";",Full!B34,1)-1))</f>
+        <v>REF_LO_P</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="99">
+        <v>25</v>
+      </c>
+      <c r="B33" s="104" t="str">
+        <f>LEFT(Full!AA35,(FIND(";",Full!AA35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="C33" s="149" t="str">
+        <f>LEFT(Full!Z35,(FIND(";",Full!Z35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="D33" s="149" t="str">
+        <f>LEFT(Full!Y35,(FIND(";",Full!Y35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="E33" s="146" t="str">
+        <f>LEFT(Full!X35,(FIND(";",Full!X35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="F33" s="146" t="str">
+        <f>LEFT(Full!W35,(FIND(";",Full!W35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="G33" s="104" t="str">
+        <f>LEFT(Full!V35,(FIND(";",Full!V35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="H33" s="104" t="str">
+        <f>LEFT(Full!U35,(FIND(";",Full!U35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="I33" s="112" t="str">
+        <f>LEFT(Full!T35,(FIND(";",Full!T35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J33" s="112" t="str">
+        <f>LEFT(Full!S35,(FIND(";",Full!S35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K33" s="104" t="str">
+        <f>LEFT(Full!R35,(FIND(";",Full!R35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="L33" s="158" t="str">
+        <f>LEFT(Full!Q35,(FIND(";",Full!Q35,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="M33" s="158" t="str">
+        <f>LEFT(Full!P35,(FIND(";",Full!P35,1)-1))</f>
+        <v>VDD_BM2</v>
+      </c>
+      <c r="N33" s="104" t="str">
+        <f>LEFT(Full!O35,(FIND(";",Full!O35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="O33" s="104" t="str">
+        <f>LEFT(Full!N35,(FIND(";",Full!N35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="P33" s="104" t="str">
+        <f>LEFT(Full!M35,(FIND(";",Full!M35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q33" s="114" t="str">
+        <f>LEFT(Full!L35,(FIND(";",Full!L35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="R33" s="112" t="str">
+        <f>LEFT(Full!K35,(FIND(";",Full!K35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S33" s="104" t="str">
+        <f>LEFT(Full!J35,(FIND(";",Full!J35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T33" s="104" t="str">
+        <f>LEFT(Full!I35,(FIND(";",Full!I35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="U33" s="112" t="str">
+        <f>LEFT(Full!H35,(FIND(";",Full!H35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="V33" s="112" t="str">
+        <f>LEFT(Full!G35,(FIND(";",Full!G35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W33" s="151" t="str">
+        <f>LEFT(Full!F35,(FIND(";",Full!F35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="X33" s="149" t="str">
+        <f>LEFT(Full!E35,(FIND(";",Full!E35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Y33" s="152" t="str">
+        <f>LEFT(Full!D35,(FIND(";",Full!D35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="Z33" s="152" t="str">
+        <f>LEFT(Full!C35,(FIND(";",Full!C35,1)-1))</f>
+        <v>VDD_IO</v>
+      </c>
+      <c r="AA33" s="104" t="str">
+        <f>LEFT(Full!B35,(FIND(";",Full!B35,1)-1))</f>
+        <v>VSS</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="99">
+        <v>26</v>
+      </c>
+      <c r="B34" s="142" t="str">
+        <f>LEFT(Full!AA36,(FIND(";",Full!AA36,1)-1))</f>
+        <v>NC</v>
+      </c>
+      <c r="C34" s="104" t="str">
+        <f>LEFT(Full!Z36,(FIND(";",Full!Z36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="D34" s="142" t="str">
+        <f>LEFT(Full!Y36,(FIND(";",Full!Y36,1)-1))</f>
+        <v>ANT_2_N</v>
+      </c>
+      <c r="E34" s="142" t="str">
+        <f>LEFT(Full!X36,(FIND(";",Full!X36,1)-1))</f>
+        <v>ANT_2_P</v>
+      </c>
+      <c r="F34" s="104" t="str">
+        <f>LEFT(Full!W36,(FIND(";",Full!W36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="G34" s="142" t="str">
+        <f>LEFT(Full!V36,(FIND(";",Full!V36,1)-1))</f>
+        <v>CLK_DIG_OVERRIDE_N</v>
+      </c>
+      <c r="H34" s="142" t="str">
+        <f>LEFT(Full!U36,(FIND(";",Full!U36,1)-1))</f>
+        <v>CLK_DIG_OVERRIDE_P</v>
+      </c>
+      <c r="I34" s="104" t="str">
+        <f>LEFT(Full!T36,(FIND(";",Full!T36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="J34" s="104" t="str">
+        <f>LEFT(Full!S36,(FIND(";",Full!S36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="K34" s="142" t="str">
+        <f>LEFT(Full!R36,(FIND(";",Full!R36,1)-1))</f>
+        <v>LINK_BM_TX_2_N</v>
+      </c>
+      <c r="L34" s="142" t="str">
+        <f>LEFT(Full!Q36,(FIND(";",Full!Q36,1)-1))</f>
+        <v>LINK_BM_TX_2_P</v>
+      </c>
+      <c r="M34" s="104" t="str">
+        <f>LEFT(Full!P36,(FIND(";",Full!P36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="N34" s="142" t="str">
+        <f>LEFT(Full!O36,(FIND(";",Full!O36,1)-1))</f>
+        <v>LINK_BM_RX_2_N</v>
+      </c>
+      <c r="O34" s="142" t="str">
+        <f>LEFT(Full!N36,(FIND(";",Full!N36,1)-1))</f>
+        <v>LINK_BM_RX_2_P</v>
+      </c>
+      <c r="P34" s="104" t="str">
+        <f>LEFT(Full!M36,(FIND(";",Full!M36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="Q34" s="142" t="str">
+        <f>LEFT(Full!L36,(FIND(";",Full!L36,1)-1))</f>
+        <v>SERDES_SUPPLY_PROBE_2</v>
+      </c>
+      <c r="R34" s="104" t="str">
+        <f>LEFT(Full!K36,(FIND(";",Full!K36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="S34" s="104" t="str">
+        <f>LEFT(Full!J36,(FIND(";",Full!J36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="T34" s="142" t="str">
+        <f>LEFT(Full!I36,(FIND(";",Full!I36,1)-1))</f>
+        <v>ANA_MUX_N</v>
+      </c>
+      <c r="U34" s="142" t="str">
+        <f>LEFT(Full!H36,(FIND(";",Full!H36,1)-1))</f>
+        <v>ANA_MUX_P</v>
+      </c>
+      <c r="V34" s="104" t="str">
+        <f>LEFT(Full!G36,(FIND(";",Full!G36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="W34" s="104" t="str">
+        <f>LEFT(Full!F36,(FIND(";",Full!F36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="X34" s="142" t="str">
+        <f>LEFT(Full!E36,(FIND(";",Full!E36,1)-1))</f>
+        <v>ANT_3_N</v>
+      </c>
+      <c r="Y34" s="142" t="str">
+        <f>LEFT(Full!D36,(FIND(";",Full!D36,1)-1))</f>
+        <v>ANT_3_P</v>
+      </c>
+      <c r="Z34" s="104" t="str">
+        <f>LEFT(Full!C36,(FIND(";",Full!C36,1)-1))</f>
+        <v>VSS</v>
+      </c>
+      <c r="AA34" s="142" t="str">
+        <f>LEFT(Full!B36,(FIND(";",Full!B36,1)-1))</f>
+        <v>NC</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added 7 TestPoint_SMD to help break out signals from the FADER chip.
</commit_message>
<xml_diff>
--- a/Files_for_TestPlan_TestReports/FADER2_bumps.xlsx
+++ b/Files_for_TestPlan_TestReports/FADER2_bumps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caolen\Nokia\Fader2.5\fader25_pcb\Files_for_TestPlan_TestReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1F85C6-A12D-4DF2-9F92-D13A3E6A36F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2358BA-C667-46C2-A91F-BE0DF1B89107}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="240" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="240" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="1" r:id="rId1"/>
@@ -1875,7 +1875,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1924,12 +1924,6 @@
       <color rgb="FF000000"/>
       <name val="Comic Sans MS"/>
       <family val="4"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2954,7 +2948,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2969,10 +2963,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
@@ -2989,7 +2983,7 @@
     <xf numFmtId="0" fontId="1" fillId="29" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3054,7 +3048,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="49" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3942,8 +3936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AM49"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17953,11 +17947,11 @@
   <dimension ref="A2:AN34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
       <selection pane="topRight" activeCell="B8" sqref="B8"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="AX20" sqref="AX20"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18969,7 +18963,7 @@
         <v>81</v>
       </c>
       <c r="AE16" s="134">
-        <f>COUNTIF($B$9:$AB$34, AD16)</f>
+        <f t="shared" ref="AE16:AE21" si="0">COUNTIF($B$9:$AB$34, AD16)</f>
         <v>376</v>
       </c>
     </row>
@@ -19085,7 +19079,7 @@
         <v>82</v>
       </c>
       <c r="AE17" s="135">
-        <f>COUNTIF($B$9:$AB$34, AD17)</f>
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
     </row>
@@ -19201,7 +19195,7 @@
         <v>83</v>
       </c>
       <c r="AE18" s="179">
-        <f>COUNTIF($B$9:$AB$34, AD18)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="AG18" s="173" t="s">
@@ -19329,7 +19323,7 @@
         <v>84</v>
       </c>
       <c r="AE19" s="164">
-        <f>COUNTIF($B$9:$AB$34, AD19)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="AG19" s="176" t="s">
@@ -19469,7 +19463,7 @@
         <v>85</v>
       </c>
       <c r="AE20" s="166">
-        <f>COUNTIF($B$9:$AB$34, AD20)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
@@ -19585,7 +19579,7 @@
         <v>86</v>
       </c>
       <c r="AE21" s="148">
-        <f>COUNTIF($B$9:$AB$34, AD21)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>

</xml_diff>